<commit_message>
Le s. pump 2
</commit_message>
<xml_diff>
--- a/Calibracion.xlsx
+++ b/Calibracion.xlsx
@@ -653,7 +653,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="108">
   <si>
     <t>uL/h</t>
   </si>
@@ -952,18 +952,126 @@
   <si>
     <t>Caudal máximo</t>
   </si>
+  <si>
+    <t>C=</t>
+  </si>
+  <si>
+    <t>Q/f</t>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>e</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">n </t>
+    </r>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>e</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">n </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(uL)</t>
+    </r>
+  </si>
+  <si>
+    <t>A (uL)</t>
+  </si>
+  <si>
+    <t>C (1/mm)</t>
+  </si>
+  <si>
+    <t>uL</t>
+  </si>
+  <si>
+    <t>1/mm</t>
+  </si>
+  <si>
+    <t>um</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.000000"/>
     <numFmt numFmtId="167" formatCode="0.0%"/>
+    <numFmt numFmtId="175" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -994,6 +1102,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1595,7 +1717,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1779,10 +1901,22 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1799,11 +1933,59 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1823,66 +2005,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1892,12 +2020,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2126,11 +2259,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="92474176"/>
-        <c:axId val="92474752"/>
+        <c:axId val="75155136"/>
+        <c:axId val="75156864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="92474176"/>
+        <c:axId val="75155136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2140,12 +2273,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92474752"/>
+        <c:crossAx val="75156864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="92474752"/>
+        <c:axId val="75156864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2156,7 +2289,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92474176"/>
+        <c:crossAx val="75155136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2184,13 +2317,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>57151</xdr:colOff>
+          <xdr:colOff>57150</xdr:colOff>
           <xdr:row>35</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>6</xdr:col>
-          <xdr:colOff>462539</xdr:colOff>
+          <xdr:colOff>466725</xdr:colOff>
           <xdr:row>53</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -2231,9 +2364,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>20</xdr:col>
-          <xdr:colOff>228600</xdr:colOff>
-          <xdr:row>52</xdr:row>
-          <xdr:rowOff>186854</xdr:rowOff>
+          <xdr:colOff>352425</xdr:colOff>
+          <xdr:row>53</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2963,47 +3096,47 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="75" t="s">
+      <c r="A8" s="77" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="76"/>
+      <c r="B8" s="78"/>
       <c r="C8" s="53">
         <v>16</v>
       </c>
-      <c r="D8" s="83" t="s">
+      <c r="D8" s="79" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="76"/>
+      <c r="E8" s="78"/>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" t="s">
         <v>44</v>
       </c>
-      <c r="H8" s="84" t="s">
+      <c r="H8" s="80" t="s">
         <v>45</v>
       </c>
-      <c r="I8" s="84"/>
+      <c r="I8" s="80"/>
       <c r="J8">
         <v>25</v>
       </c>
-      <c r="K8" s="84" t="s">
+      <c r="K8" s="80" t="s">
         <v>46</v>
       </c>
-      <c r="L8" s="84"/>
+      <c r="L8" s="80"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="75" t="s">
+      <c r="A9" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="76"/>
+      <c r="B9" s="78"/>
       <c r="C9" s="54">
         <v>200</v>
       </c>
-      <c r="D9" s="77" t="s">
+      <c r="D9" s="81" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="78"/>
+      <c r="E9" s="82"/>
       <c r="F9">
         <f>F8*B8</f>
         <v>0</v>
@@ -3011,31 +3144,31 @@
       <c r="G9" t="s">
         <v>48</v>
       </c>
-      <c r="H9" s="84" t="s">
+      <c r="H9" s="80" t="s">
         <v>49</v>
       </c>
-      <c r="I9" s="84"/>
+      <c r="I9" s="80"/>
       <c r="J9" s="55">
         <f>C10*J8</f>
         <v>1272.3724999999999</v>
       </c>
-      <c r="K9" s="84" t="s">
+      <c r="K9" s="80" t="s">
         <v>50</v>
       </c>
-      <c r="L9" s="84"/>
+      <c r="L9" s="80"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="75" t="s">
+      <c r="A10" s="77" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="76"/>
+      <c r="B10" s="78"/>
       <c r="C10" s="54">
         <v>50.8949</v>
       </c>
-      <c r="D10" s="77" t="s">
+      <c r="D10" s="81" t="s">
         <v>52</v>
       </c>
-      <c r="E10" s="78"/>
+      <c r="E10" s="82"/>
       <c r="J10" s="55">
         <f>J9*C9*C8/60</f>
         <v>67859.866666666669</v>
@@ -3046,31 +3179,31 @@
       <c r="L10" s="56"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="75" t="s">
+      <c r="A11" s="77" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="76"/>
+      <c r="B11" s="78"/>
       <c r="C11" s="54">
         <v>8</v>
       </c>
-      <c r="D11" s="79" t="s">
+      <c r="D11" s="83" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="80"/>
+      <c r="E11" s="84"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="81" t="s">
+      <c r="A12" s="85" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="82"/>
+      <c r="B12" s="86"/>
       <c r="C12" s="57">
         <f>C8*C9*C10/C11</f>
         <v>20357.96</v>
       </c>
-      <c r="D12" s="77" t="s">
+      <c r="D12" s="81" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="78"/>
+      <c r="E12" s="82"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -3101,6 +3234,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="H8:I8"/>
@@ -3109,12 +3248,6 @@
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="K9:L9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="D12:E12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="67" orientation="landscape" r:id="rId1"/>
@@ -3165,39 +3298,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="111" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="85" t="s">
+      <c r="B1" s="105" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="86"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="85" t="s">
+      <c r="C1" s="106"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="105" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="86"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="85" t="s">
+      <c r="F1" s="106"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="105" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="86"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="85" t="s">
+      <c r="I1" s="106"/>
+      <c r="J1" s="107"/>
+      <c r="K1" s="105" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="86"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="85" t="s">
+      <c r="L1" s="106"/>
+      <c r="M1" s="107"/>
+      <c r="N1" s="105" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="86"/>
-      <c r="P1" s="87"/>
-      <c r="Q1" s="85" t="s">
+      <c r="O1" s="106"/>
+      <c r="P1" s="107"/>
+      <c r="Q1" s="105" t="s">
         <v>3</v>
       </c>
-      <c r="R1" s="86"/>
-      <c r="S1" s="87"/>
+      <c r="R1" s="106"/>
+      <c r="S1" s="107"/>
       <c r="T1" t="s">
         <v>8</v>
       </c>
@@ -3209,7 +3342,7 @@
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="98"/>
+      <c r="A2" s="112"/>
       <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
@@ -3346,216 +3479,216 @@
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="88" t="s">
+      <c r="A4" s="108" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="91"/>
-      <c r="C4" s="92"/>
-      <c r="D4" s="93"/>
-      <c r="E4" s="94"/>
-      <c r="F4" s="95"/>
-      <c r="G4" s="96"/>
-      <c r="H4" s="91"/>
-      <c r="I4" s="92"/>
-      <c r="J4" s="93"/>
-      <c r="K4" s="91"/>
-      <c r="L4" s="92"/>
-      <c r="M4" s="93"/>
-      <c r="N4" s="91"/>
-      <c r="O4" s="92"/>
-      <c r="P4" s="93"/>
-      <c r="Q4" s="94"/>
-      <c r="R4" s="95"/>
-      <c r="S4" s="96"/>
+      <c r="B4" s="96"/>
+      <c r="C4" s="97"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="99"/>
+      <c r="F4" s="100"/>
+      <c r="G4" s="101"/>
+      <c r="H4" s="96"/>
+      <c r="I4" s="97"/>
+      <c r="J4" s="98"/>
+      <c r="K4" s="96"/>
+      <c r="L4" s="97"/>
+      <c r="M4" s="98"/>
+      <c r="N4" s="96"/>
+      <c r="O4" s="97"/>
+      <c r="P4" s="98"/>
+      <c r="Q4" s="99"/>
+      <c r="R4" s="100"/>
+      <c r="S4" s="101"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="89"/>
-      <c r="B5" s="91"/>
-      <c r="C5" s="92"/>
-      <c r="D5" s="93"/>
-      <c r="E5" s="94"/>
-      <c r="F5" s="95"/>
-      <c r="G5" s="96"/>
-      <c r="H5" s="91"/>
-      <c r="I5" s="92"/>
-      <c r="J5" s="93"/>
-      <c r="K5" s="94"/>
-      <c r="L5" s="95"/>
-      <c r="M5" s="96"/>
-      <c r="N5" s="91"/>
-      <c r="O5" s="92"/>
-      <c r="P5" s="93"/>
-      <c r="Q5" s="91"/>
-      <c r="R5" s="92"/>
-      <c r="S5" s="93"/>
+      <c r="A5" s="109"/>
+      <c r="B5" s="96"/>
+      <c r="C5" s="97"/>
+      <c r="D5" s="98"/>
+      <c r="E5" s="99"/>
+      <c r="F5" s="100"/>
+      <c r="G5" s="101"/>
+      <c r="H5" s="96"/>
+      <c r="I5" s="97"/>
+      <c r="J5" s="98"/>
+      <c r="K5" s="99"/>
+      <c r="L5" s="100"/>
+      <c r="M5" s="101"/>
+      <c r="N5" s="96"/>
+      <c r="O5" s="97"/>
+      <c r="P5" s="98"/>
+      <c r="Q5" s="96"/>
+      <c r="R5" s="97"/>
+      <c r="S5" s="98"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="89"/>
-      <c r="B6" s="91"/>
-      <c r="C6" s="92"/>
-      <c r="D6" s="93"/>
-      <c r="E6" s="94"/>
-      <c r="F6" s="95"/>
-      <c r="G6" s="96"/>
-      <c r="H6" s="91"/>
-      <c r="I6" s="92"/>
-      <c r="J6" s="93"/>
-      <c r="K6" s="94"/>
-      <c r="L6" s="95"/>
-      <c r="M6" s="96"/>
-      <c r="N6" s="91"/>
-      <c r="O6" s="92"/>
-      <c r="P6" s="93"/>
-      <c r="Q6" s="94"/>
-      <c r="R6" s="95"/>
-      <c r="S6" s="96"/>
+      <c r="A6" s="109"/>
+      <c r="B6" s="96"/>
+      <c r="C6" s="97"/>
+      <c r="D6" s="98"/>
+      <c r="E6" s="99"/>
+      <c r="F6" s="100"/>
+      <c r="G6" s="101"/>
+      <c r="H6" s="96"/>
+      <c r="I6" s="97"/>
+      <c r="J6" s="98"/>
+      <c r="K6" s="99"/>
+      <c r="L6" s="100"/>
+      <c r="M6" s="101"/>
+      <c r="N6" s="96"/>
+      <c r="O6" s="97"/>
+      <c r="P6" s="98"/>
+      <c r="Q6" s="99"/>
+      <c r="R6" s="100"/>
+      <c r="S6" s="101"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="89"/>
-      <c r="B7" s="91"/>
-      <c r="C7" s="92"/>
-      <c r="D7" s="93"/>
-      <c r="E7" s="94"/>
-      <c r="F7" s="95"/>
-      <c r="G7" s="96"/>
-      <c r="H7" s="91"/>
-      <c r="I7" s="92"/>
-      <c r="J7" s="93"/>
-      <c r="K7" s="94"/>
-      <c r="L7" s="95"/>
-      <c r="M7" s="96"/>
-      <c r="N7" s="91"/>
-      <c r="O7" s="92"/>
-      <c r="P7" s="93"/>
-      <c r="Q7" s="91"/>
-      <c r="R7" s="92"/>
-      <c r="S7" s="93"/>
+      <c r="A7" s="109"/>
+      <c r="B7" s="96"/>
+      <c r="C7" s="97"/>
+      <c r="D7" s="98"/>
+      <c r="E7" s="99"/>
+      <c r="F7" s="100"/>
+      <c r="G7" s="101"/>
+      <c r="H7" s="96"/>
+      <c r="I7" s="97"/>
+      <c r="J7" s="98"/>
+      <c r="K7" s="99"/>
+      <c r="L7" s="100"/>
+      <c r="M7" s="101"/>
+      <c r="N7" s="96"/>
+      <c r="O7" s="97"/>
+      <c r="P7" s="98"/>
+      <c r="Q7" s="96"/>
+      <c r="R7" s="97"/>
+      <c r="S7" s="98"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="89"/>
-      <c r="B8" s="91"/>
-      <c r="C8" s="92"/>
-      <c r="D8" s="93"/>
-      <c r="E8" s="94"/>
-      <c r="F8" s="95"/>
-      <c r="G8" s="96"/>
-      <c r="H8" s="91"/>
-      <c r="I8" s="92"/>
-      <c r="J8" s="93"/>
-      <c r="K8" s="94"/>
-      <c r="L8" s="95"/>
-      <c r="M8" s="96"/>
-      <c r="N8" s="91"/>
-      <c r="O8" s="92"/>
-      <c r="P8" s="93"/>
-      <c r="Q8" s="94"/>
-      <c r="R8" s="95"/>
-      <c r="S8" s="96"/>
+      <c r="A8" s="109"/>
+      <c r="B8" s="96"/>
+      <c r="C8" s="97"/>
+      <c r="D8" s="98"/>
+      <c r="E8" s="99"/>
+      <c r="F8" s="100"/>
+      <c r="G8" s="101"/>
+      <c r="H8" s="96"/>
+      <c r="I8" s="97"/>
+      <c r="J8" s="98"/>
+      <c r="K8" s="99"/>
+      <c r="L8" s="100"/>
+      <c r="M8" s="101"/>
+      <c r="N8" s="96"/>
+      <c r="O8" s="97"/>
+      <c r="P8" s="98"/>
+      <c r="Q8" s="99"/>
+      <c r="R8" s="100"/>
+      <c r="S8" s="101"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="90"/>
-      <c r="B9" s="91"/>
-      <c r="C9" s="92"/>
-      <c r="D9" s="93"/>
-      <c r="E9" s="99"/>
-      <c r="F9" s="100"/>
-      <c r="G9" s="101"/>
-      <c r="H9" s="91"/>
-      <c r="I9" s="92"/>
-      <c r="J9" s="93"/>
-      <c r="K9" s="99"/>
-      <c r="L9" s="100"/>
-      <c r="M9" s="101"/>
-      <c r="N9" s="91"/>
-      <c r="O9" s="92"/>
-      <c r="P9" s="93"/>
-      <c r="Q9" s="94"/>
-      <c r="R9" s="95"/>
-      <c r="S9" s="96"/>
+      <c r="A9" s="110"/>
+      <c r="B9" s="96"/>
+      <c r="C9" s="97"/>
+      <c r="D9" s="98"/>
+      <c r="E9" s="102"/>
+      <c r="F9" s="103"/>
+      <c r="G9" s="104"/>
+      <c r="H9" s="96"/>
+      <c r="I9" s="97"/>
+      <c r="J9" s="98"/>
+      <c r="K9" s="102"/>
+      <c r="L9" s="103"/>
+      <c r="M9" s="104"/>
+      <c r="N9" s="96"/>
+      <c r="O9" s="97"/>
+      <c r="P9" s="98"/>
+      <c r="Q9" s="99"/>
+      <c r="R9" s="100"/>
+      <c r="S9" s="101"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="105"/>
-      <c r="C10" s="106"/>
-      <c r="D10" s="107"/>
-      <c r="E10" s="105"/>
-      <c r="F10" s="106"/>
-      <c r="G10" s="107"/>
-      <c r="H10" s="105"/>
-      <c r="I10" s="106"/>
-      <c r="J10" s="107"/>
-      <c r="K10" s="105"/>
-      <c r="L10" s="106"/>
-      <c r="M10" s="107"/>
-      <c r="N10" s="105"/>
-      <c r="O10" s="106"/>
-      <c r="P10" s="107"/>
-      <c r="Q10" s="105"/>
-      <c r="R10" s="106"/>
-      <c r="S10" s="107"/>
+      <c r="B10" s="93"/>
+      <c r="C10" s="94"/>
+      <c r="D10" s="95"/>
+      <c r="E10" s="93"/>
+      <c r="F10" s="94"/>
+      <c r="G10" s="95"/>
+      <c r="H10" s="93"/>
+      <c r="I10" s="94"/>
+      <c r="J10" s="95"/>
+      <c r="K10" s="93"/>
+      <c r="L10" s="94"/>
+      <c r="M10" s="95"/>
+      <c r="N10" s="93"/>
+      <c r="O10" s="94"/>
+      <c r="P10" s="95"/>
+      <c r="Q10" s="93"/>
+      <c r="R10" s="94"/>
+      <c r="S10" s="95"/>
     </row>
     <row r="11" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="102"/>
-      <c r="C11" s="103"/>
-      <c r="D11" s="104"/>
-      <c r="E11" s="102"/>
-      <c r="F11" s="103"/>
-      <c r="G11" s="104"/>
-      <c r="H11" s="102"/>
-      <c r="I11" s="103"/>
-      <c r="J11" s="104"/>
-      <c r="K11" s="102"/>
-      <c r="L11" s="103"/>
-      <c r="M11" s="104"/>
-      <c r="N11" s="102"/>
-      <c r="O11" s="103"/>
-      <c r="P11" s="104"/>
-      <c r="Q11" s="102"/>
-      <c r="R11" s="103"/>
-      <c r="S11" s="104"/>
+      <c r="B11" s="87"/>
+      <c r="C11" s="88"/>
+      <c r="D11" s="89"/>
+      <c r="E11" s="87"/>
+      <c r="F11" s="88"/>
+      <c r="G11" s="89"/>
+      <c r="H11" s="87"/>
+      <c r="I11" s="88"/>
+      <c r="J11" s="89"/>
+      <c r="K11" s="87"/>
+      <c r="L11" s="88"/>
+      <c r="M11" s="89"/>
+      <c r="N11" s="87"/>
+      <c r="O11" s="88"/>
+      <c r="P11" s="89"/>
+      <c r="Q11" s="87"/>
+      <c r="R11" s="88"/>
+      <c r="S11" s="89"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="97" t="s">
+      <c r="A13" s="111" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="85" t="s">
+      <c r="B13" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="86"/>
-      <c r="D13" s="87"/>
-      <c r="E13" s="85" t="s">
+      <c r="C13" s="106"/>
+      <c r="D13" s="107"/>
+      <c r="E13" s="105" t="s">
         <v>3</v>
       </c>
-      <c r="F13" s="86"/>
-      <c r="G13" s="87"/>
-      <c r="H13" s="85" t="s">
+      <c r="F13" s="106"/>
+      <c r="G13" s="107"/>
+      <c r="H13" s="105" t="s">
         <v>3</v>
       </c>
-      <c r="I13" s="86"/>
-      <c r="J13" s="87"/>
-      <c r="K13" s="85" t="s">
+      <c r="I13" s="106"/>
+      <c r="J13" s="107"/>
+      <c r="K13" s="105" t="s">
         <v>3</v>
       </c>
-      <c r="L13" s="86"/>
-      <c r="M13" s="87"/>
-      <c r="N13" s="85" t="s">
+      <c r="L13" s="106"/>
+      <c r="M13" s="107"/>
+      <c r="N13" s="105" t="s">
         <v>3</v>
       </c>
-      <c r="O13" s="86"/>
-      <c r="P13" s="87"/>
-      <c r="Q13" s="85" t="s">
+      <c r="O13" s="106"/>
+      <c r="P13" s="107"/>
+      <c r="Q13" s="105" t="s">
         <v>6</v>
       </c>
-      <c r="R13" s="86"/>
-      <c r="S13" s="87"/>
+      <c r="R13" s="106"/>
+      <c r="S13" s="107"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="98"/>
+      <c r="A14" s="112"/>
       <c r="B14" s="11" t="s">
         <v>0</v>
       </c>
@@ -3683,213 +3816,237 @@
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="88" t="s">
+      <c r="A16" s="108" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="91"/>
-      <c r="C16" s="92"/>
-      <c r="D16" s="93"/>
-      <c r="E16" s="94"/>
-      <c r="F16" s="95"/>
-      <c r="G16" s="96"/>
-      <c r="H16" s="91"/>
-      <c r="I16" s="92"/>
-      <c r="J16" s="93"/>
-      <c r="K16" s="94"/>
-      <c r="L16" s="95"/>
-      <c r="M16" s="96"/>
-      <c r="N16" s="91"/>
-      <c r="O16" s="92"/>
-      <c r="P16" s="93"/>
-      <c r="Q16" s="94"/>
-      <c r="R16" s="95"/>
-      <c r="S16" s="96"/>
+      <c r="B16" s="96"/>
+      <c r="C16" s="97"/>
+      <c r="D16" s="98"/>
+      <c r="E16" s="99"/>
+      <c r="F16" s="100"/>
+      <c r="G16" s="101"/>
+      <c r="H16" s="96"/>
+      <c r="I16" s="97"/>
+      <c r="J16" s="98"/>
+      <c r="K16" s="99"/>
+      <c r="L16" s="100"/>
+      <c r="M16" s="101"/>
+      <c r="N16" s="96"/>
+      <c r="O16" s="97"/>
+      <c r="P16" s="98"/>
+      <c r="Q16" s="99"/>
+      <c r="R16" s="100"/>
+      <c r="S16" s="101"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="89"/>
-      <c r="B17" s="91"/>
-      <c r="C17" s="92"/>
-      <c r="D17" s="93"/>
-      <c r="E17" s="94"/>
-      <c r="F17" s="95"/>
-      <c r="G17" s="96"/>
-      <c r="H17" s="91"/>
-      <c r="I17" s="92"/>
-      <c r="J17" s="93"/>
-      <c r="K17" s="94"/>
-      <c r="L17" s="95"/>
-      <c r="M17" s="96"/>
-      <c r="N17" s="91"/>
-      <c r="O17" s="92"/>
-      <c r="P17" s="93"/>
-      <c r="Q17" s="91"/>
-      <c r="R17" s="92"/>
-      <c r="S17" s="93"/>
+      <c r="A17" s="109"/>
+      <c r="B17" s="96"/>
+      <c r="C17" s="97"/>
+      <c r="D17" s="98"/>
+      <c r="E17" s="99"/>
+      <c r="F17" s="100"/>
+      <c r="G17" s="101"/>
+      <c r="H17" s="96"/>
+      <c r="I17" s="97"/>
+      <c r="J17" s="98"/>
+      <c r="K17" s="99"/>
+      <c r="L17" s="100"/>
+      <c r="M17" s="101"/>
+      <c r="N17" s="96"/>
+      <c r="O17" s="97"/>
+      <c r="P17" s="98"/>
+      <c r="Q17" s="96"/>
+      <c r="R17" s="97"/>
+      <c r="S17" s="98"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="89"/>
-      <c r="B18" s="91"/>
-      <c r="C18" s="92"/>
-      <c r="D18" s="93"/>
-      <c r="E18" s="94"/>
-      <c r="F18" s="95"/>
-      <c r="G18" s="96"/>
-      <c r="H18" s="91"/>
-      <c r="I18" s="92"/>
-      <c r="J18" s="93"/>
-      <c r="K18" s="94"/>
-      <c r="L18" s="95"/>
-      <c r="M18" s="96"/>
-      <c r="N18" s="91"/>
-      <c r="O18" s="92"/>
-      <c r="P18" s="93"/>
-      <c r="Q18" s="94"/>
-      <c r="R18" s="95"/>
-      <c r="S18" s="96"/>
+      <c r="A18" s="109"/>
+      <c r="B18" s="96"/>
+      <c r="C18" s="97"/>
+      <c r="D18" s="98"/>
+      <c r="E18" s="99"/>
+      <c r="F18" s="100"/>
+      <c r="G18" s="101"/>
+      <c r="H18" s="96"/>
+      <c r="I18" s="97"/>
+      <c r="J18" s="98"/>
+      <c r="K18" s="99"/>
+      <c r="L18" s="100"/>
+      <c r="M18" s="101"/>
+      <c r="N18" s="96"/>
+      <c r="O18" s="97"/>
+      <c r="P18" s="98"/>
+      <c r="Q18" s="99"/>
+      <c r="R18" s="100"/>
+      <c r="S18" s="101"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="89"/>
-      <c r="B19" s="91"/>
-      <c r="C19" s="92"/>
-      <c r="D19" s="93"/>
-      <c r="E19" s="94"/>
-      <c r="F19" s="95"/>
-      <c r="G19" s="96"/>
-      <c r="H19" s="91"/>
-      <c r="I19" s="92"/>
-      <c r="J19" s="93"/>
-      <c r="K19" s="94"/>
-      <c r="L19" s="95"/>
-      <c r="M19" s="96"/>
-      <c r="N19" s="91"/>
-      <c r="O19" s="92"/>
-      <c r="P19" s="93"/>
-      <c r="Q19" s="91"/>
-      <c r="R19" s="92"/>
-      <c r="S19" s="93"/>
+      <c r="A19" s="109"/>
+      <c r="B19" s="96"/>
+      <c r="C19" s="97"/>
+      <c r="D19" s="98"/>
+      <c r="E19" s="99"/>
+      <c r="F19" s="100"/>
+      <c r="G19" s="101"/>
+      <c r="H19" s="96"/>
+      <c r="I19" s="97"/>
+      <c r="J19" s="98"/>
+      <c r="K19" s="99"/>
+      <c r="L19" s="100"/>
+      <c r="M19" s="101"/>
+      <c r="N19" s="96"/>
+      <c r="O19" s="97"/>
+      <c r="P19" s="98"/>
+      <c r="Q19" s="96"/>
+      <c r="R19" s="97"/>
+      <c r="S19" s="98"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="89"/>
-      <c r="B20" s="91"/>
-      <c r="C20" s="92"/>
-      <c r="D20" s="93"/>
-      <c r="E20" s="94"/>
-      <c r="F20" s="95"/>
-      <c r="G20" s="96"/>
-      <c r="H20" s="91"/>
-      <c r="I20" s="92"/>
-      <c r="J20" s="93"/>
-      <c r="K20" s="94"/>
-      <c r="L20" s="95"/>
-      <c r="M20" s="96"/>
-      <c r="N20" s="91"/>
-      <c r="O20" s="92"/>
-      <c r="P20" s="93"/>
-      <c r="Q20" s="94"/>
-      <c r="R20" s="95"/>
-      <c r="S20" s="96"/>
+      <c r="A20" s="109"/>
+      <c r="B20" s="96"/>
+      <c r="C20" s="97"/>
+      <c r="D20" s="98"/>
+      <c r="E20" s="99"/>
+      <c r="F20" s="100"/>
+      <c r="G20" s="101"/>
+      <c r="H20" s="96"/>
+      <c r="I20" s="97"/>
+      <c r="J20" s="98"/>
+      <c r="K20" s="99"/>
+      <c r="L20" s="100"/>
+      <c r="M20" s="101"/>
+      <c r="N20" s="96"/>
+      <c r="O20" s="97"/>
+      <c r="P20" s="98"/>
+      <c r="Q20" s="99"/>
+      <c r="R20" s="100"/>
+      <c r="S20" s="101"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="90"/>
-      <c r="B21" s="91"/>
-      <c r="C21" s="92"/>
-      <c r="D21" s="93"/>
-      <c r="E21" s="99"/>
-      <c r="F21" s="100"/>
-      <c r="G21" s="101"/>
-      <c r="H21" s="91"/>
-      <c r="I21" s="92"/>
-      <c r="J21" s="93"/>
-      <c r="K21" s="99"/>
-      <c r="L21" s="100"/>
-      <c r="M21" s="101"/>
-      <c r="N21" s="91"/>
-      <c r="O21" s="92"/>
-      <c r="P21" s="93"/>
-      <c r="Q21" s="94"/>
-      <c r="R21" s="95"/>
-      <c r="S21" s="96"/>
+      <c r="A21" s="110"/>
+      <c r="B21" s="96"/>
+      <c r="C21" s="97"/>
+      <c r="D21" s="98"/>
+      <c r="E21" s="102"/>
+      <c r="F21" s="103"/>
+      <c r="G21" s="104"/>
+      <c r="H21" s="96"/>
+      <c r="I21" s="97"/>
+      <c r="J21" s="98"/>
+      <c r="K21" s="102"/>
+      <c r="L21" s="103"/>
+      <c r="M21" s="104"/>
+      <c r="N21" s="96"/>
+      <c r="O21" s="97"/>
+      <c r="P21" s="98"/>
+      <c r="Q21" s="99"/>
+      <c r="R21" s="100"/>
+      <c r="S21" s="101"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="105"/>
-      <c r="C22" s="106"/>
-      <c r="D22" s="107"/>
-      <c r="E22" s="105"/>
-      <c r="F22" s="106"/>
-      <c r="G22" s="107"/>
-      <c r="H22" s="105"/>
-      <c r="I22" s="106"/>
-      <c r="J22" s="107"/>
-      <c r="K22" s="105"/>
-      <c r="L22" s="106"/>
-      <c r="M22" s="107"/>
-      <c r="N22" s="105"/>
-      <c r="O22" s="106"/>
-      <c r="P22" s="107"/>
-      <c r="Q22" s="105"/>
-      <c r="R22" s="106"/>
-      <c r="S22" s="107"/>
+      <c r="B22" s="93"/>
+      <c r="C22" s="94"/>
+      <c r="D22" s="95"/>
+      <c r="E22" s="93"/>
+      <c r="F22" s="94"/>
+      <c r="G22" s="95"/>
+      <c r="H22" s="93"/>
+      <c r="I22" s="94"/>
+      <c r="J22" s="95"/>
+      <c r="K22" s="93"/>
+      <c r="L22" s="94"/>
+      <c r="M22" s="95"/>
+      <c r="N22" s="93"/>
+      <c r="O22" s="94"/>
+      <c r="P22" s="95"/>
+      <c r="Q22" s="93"/>
+      <c r="R22" s="94"/>
+      <c r="S22" s="95"/>
     </row>
     <row r="23" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="102"/>
-      <c r="C23" s="103"/>
-      <c r="D23" s="104"/>
-      <c r="E23" s="102"/>
-      <c r="F23" s="103"/>
-      <c r="G23" s="104"/>
-      <c r="H23" s="102"/>
-      <c r="I23" s="103"/>
-      <c r="J23" s="104"/>
-      <c r="K23" s="108"/>
-      <c r="L23" s="109"/>
-      <c r="M23" s="110"/>
-      <c r="N23" s="102"/>
-      <c r="O23" s="103"/>
-      <c r="P23" s="104"/>
-      <c r="Q23" s="108"/>
-      <c r="R23" s="109"/>
-      <c r="S23" s="110"/>
+      <c r="B23" s="87"/>
+      <c r="C23" s="88"/>
+      <c r="D23" s="89"/>
+      <c r="E23" s="87"/>
+      <c r="F23" s="88"/>
+      <c r="G23" s="89"/>
+      <c r="H23" s="87"/>
+      <c r="I23" s="88"/>
+      <c r="J23" s="89"/>
+      <c r="K23" s="90"/>
+      <c r="L23" s="91"/>
+      <c r="M23" s="92"/>
+      <c r="N23" s="87"/>
+      <c r="O23" s="88"/>
+      <c r="P23" s="89"/>
+      <c r="Q23" s="90"/>
+      <c r="R23" s="91"/>
+      <c r="S23" s="92"/>
     </row>
   </sheetData>
   <mergeCells count="112">
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="N23:P23"/>
-    <mergeCell ref="Q23:S23"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="H22:J22"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="N22:P22"/>
-    <mergeCell ref="Q22:S22"/>
-    <mergeCell ref="N17:P17"/>
-    <mergeCell ref="Q17:S17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="N18:P18"/>
-    <mergeCell ref="Q18:S18"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="N21:P21"/>
-    <mergeCell ref="Q21:S21"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="N20:P20"/>
-    <mergeCell ref="Q20:S20"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="Q5:S5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="Q6:S6"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="N8:P8"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="N11:P11"/>
+    <mergeCell ref="Q11:S11"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="Q10:S10"/>
     <mergeCell ref="Q13:S13"/>
     <mergeCell ref="A16:A21"/>
     <mergeCell ref="B16:D16"/>
@@ -3914,62 +4071,38 @@
     <mergeCell ref="Q19:S19"/>
     <mergeCell ref="H17:J17"/>
     <mergeCell ref="K17:M17"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="N11:P11"/>
-    <mergeCell ref="Q11:S11"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="N10:P10"/>
-    <mergeCell ref="Q10:S10"/>
-    <mergeCell ref="N5:P5"/>
-    <mergeCell ref="Q5:S5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="Q6:S6"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="N9:P9"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="N8:P8"/>
-    <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="Q4:S4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="N17:P17"/>
+    <mergeCell ref="Q17:S17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="N18:P18"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="N21:P21"/>
+    <mergeCell ref="Q21:S21"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="Q20:S20"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="N23:P23"/>
+    <mergeCell ref="Q23:S23"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="N22:P22"/>
+    <mergeCell ref="Q22:S22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3979,10 +4112,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T44"/>
+  <dimension ref="A1:V44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4001,40 +4134,40 @@
     <col min="12" max="12" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="13" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6" customWidth="1"/>
-    <col min="19" max="19" width="6" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.42578125" customWidth="1"/>
+    <col min="16" max="16" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="97" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="111" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="111" t="s">
+      <c r="B1" s="113" t="s">
         <v>92</v>
       </c>
-      <c r="C1" s="112"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="111" t="s">
+      <c r="C1" s="114"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="113" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="112"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="111" t="s">
+      <c r="F1" s="114"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="113" t="s">
         <v>93</v>
       </c>
-      <c r="I1" s="112"/>
-      <c r="J1" s="113"/>
-      <c r="K1" s="111" t="s">
+      <c r="I1" s="114"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="113" t="s">
         <v>93</v>
       </c>
-      <c r="L1" s="112"/>
-      <c r="M1" s="113"/>
-      <c r="N1" s="115" t="s">
+      <c r="L1" s="114"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="76" t="s">
         <v>8</v>
       </c>
       <c r="O1" s="67">
@@ -4043,10 +4176,27 @@
       <c r="P1" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="67"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="98"/>
+      <c r="Q1" s="63" t="s">
+        <v>59</v>
+      </c>
+      <c r="R1" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="S1" s="65" t="s">
+        <v>99</v>
+      </c>
+      <c r="T1" s="65" t="s">
+        <v>63</v>
+      </c>
+      <c r="U1" s="65" t="s">
+        <v>62</v>
+      </c>
+      <c r="V1" s="65" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" s="112"/>
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
@@ -4092,8 +4242,21 @@
       <c r="P2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="S2" s="65" t="s">
+        <v>99</v>
+      </c>
+      <c r="T2" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="U2">
+        <f>P34</f>
+        <v>0.18410000000000001</v>
+      </c>
+      <c r="V2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -4141,32 +4304,45 @@
         <f>L3*1000</f>
         <v>250</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="88" t="s">
+      <c r="S3" s="65" t="s">
+        <v>99</v>
+      </c>
+      <c r="T3" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="U3" s="117">
+        <f>U2/60</f>
+        <v>3.0683333333333335E-3</v>
+      </c>
+      <c r="V3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="108" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="91">
+      <c r="B4" s="96">
         <f>36.2/7.05</f>
         <v>5.1347517730496461</v>
       </c>
-      <c r="C4" s="92"/>
-      <c r="D4" s="93"/>
-      <c r="E4" s="91">
+      <c r="C4" s="97"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="96">
         <f>39/1.16</f>
         <v>33.620689655172413</v>
       </c>
-      <c r="F4" s="92"/>
-      <c r="G4" s="93"/>
-      <c r="H4" s="91">
+      <c r="F4" s="97"/>
+      <c r="G4" s="98"/>
+      <c r="H4" s="96">
         <f>195/1.09</f>
         <v>178.89908256880733</v>
       </c>
-      <c r="I4" s="92"/>
-      <c r="J4" s="93"/>
-      <c r="K4" s="94"/>
-      <c r="L4" s="95"/>
-      <c r="M4" s="96"/>
+      <c r="I4" s="97"/>
+      <c r="J4" s="98"/>
+      <c r="K4" s="99"/>
+      <c r="L4" s="100"/>
+      <c r="M4" s="101"/>
       <c r="N4" s="63" t="s">
         <v>91</v>
       </c>
@@ -4181,29 +4357,33 @@
       </c>
       <c r="R4" s="72"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="89"/>
-      <c r="B5" s="91">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="109"/>
+      <c r="B5" s="96">
         <f>37.9/7.11</f>
         <v>5.3305203938115326</v>
       </c>
-      <c r="C5" s="92"/>
-      <c r="D5" s="93"/>
-      <c r="E5" s="91">
+      <c r="C5" s="97"/>
+      <c r="D5" s="98"/>
+      <c r="E5" s="96">
         <f>38.6/1.17</f>
         <v>32.991452991452995</v>
       </c>
-      <c r="F5" s="92"/>
-      <c r="G5" s="93"/>
-      <c r="H5" s="91">
+      <c r="F5" s="97"/>
+      <c r="G5" s="98"/>
+      <c r="H5" s="96">
         <f>194/1.11</f>
         <v>174.77477477477476</v>
       </c>
-      <c r="I5" s="92"/>
-      <c r="J5" s="93"/>
-      <c r="K5" s="91"/>
-      <c r="L5" s="92"/>
-      <c r="M5" s="93"/>
+      <c r="I5" s="97"/>
+      <c r="J5" s="98"/>
+      <c r="K5" s="96"/>
+      <c r="L5" s="97"/>
+      <c r="M5" s="98"/>
+      <c r="N5">
+        <f>'Flow Rate'!C16</f>
+        <v>21610</v>
+      </c>
       <c r="P5" s="65" t="s">
         <v>89</v>
       </c>
@@ -4211,194 +4391,262 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="89"/>
-      <c r="B6" s="91">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="109"/>
+      <c r="B6" s="96">
         <f>37/7.03</f>
         <v>5.2631578947368416</v>
       </c>
-      <c r="C6" s="92"/>
-      <c r="D6" s="93"/>
-      <c r="E6" s="91">
+      <c r="C6" s="97"/>
+      <c r="D6" s="98"/>
+      <c r="E6" s="96">
         <f>38.2/1.16</f>
         <v>32.931034482758626</v>
       </c>
-      <c r="F6" s="92"/>
-      <c r="G6" s="93"/>
-      <c r="H6" s="91">
+      <c r="F6" s="97"/>
+      <c r="G6" s="98"/>
+      <c r="H6" s="96">
         <f>194.3/1.1</f>
         <v>176.63636363636363</v>
       </c>
-      <c r="I6" s="92"/>
-      <c r="J6" s="93"/>
-      <c r="K6" s="94"/>
-      <c r="L6" s="95"/>
-      <c r="M6" s="96"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="89"/>
-      <c r="B7" s="91">
+      <c r="I6" s="97"/>
+      <c r="J6" s="98"/>
+      <c r="K6" s="99"/>
+      <c r="L6" s="100"/>
+      <c r="M6" s="101"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="109"/>
+      <c r="B7" s="96">
         <f>36/6.48</f>
         <v>5.5555555555555554</v>
       </c>
-      <c r="C7" s="92"/>
-      <c r="D7" s="93"/>
-      <c r="E7" s="91">
+      <c r="C7" s="97"/>
+      <c r="D7" s="98"/>
+      <c r="E7" s="96">
         <f>38/1.15</f>
         <v>33.04347826086957</v>
       </c>
-      <c r="F7" s="92"/>
-      <c r="G7" s="93"/>
-      <c r="H7" s="91">
+      <c r="F7" s="97"/>
+      <c r="G7" s="98"/>
+      <c r="H7" s="96">
         <f>192.4/1.08</f>
         <v>178.14814814814815</v>
       </c>
-      <c r="I7" s="92"/>
-      <c r="J7" s="93"/>
-      <c r="K7" s="91"/>
-      <c r="L7" s="92"/>
-      <c r="M7" s="93"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="89"/>
-      <c r="B8" s="91">
+      <c r="I7" s="97"/>
+      <c r="J7" s="98"/>
+      <c r="K7" s="96"/>
+      <c r="L7" s="97"/>
+      <c r="M7" s="98"/>
+      <c r="O7" s="63" t="s">
+        <v>95</v>
+      </c>
+      <c r="P7" s="103" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q7" s="103"/>
+      <c r="R7" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="S7" s="103" t="s">
+        <v>98</v>
+      </c>
+      <c r="T7" s="103"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="109"/>
+      <c r="B8" s="96">
         <f>32.8/6.39</f>
         <v>5.1330203442879494</v>
       </c>
-      <c r="C8" s="92"/>
-      <c r="D8" s="93"/>
-      <c r="E8" s="91">
+      <c r="C8" s="97"/>
+      <c r="D8" s="98"/>
+      <c r="E8" s="96">
         <f>38.1/1.14</f>
         <v>33.421052631578952</v>
       </c>
-      <c r="F8" s="92"/>
-      <c r="G8" s="93"/>
-      <c r="H8" s="91">
+      <c r="F8" s="97"/>
+      <c r="G8" s="98"/>
+      <c r="H8" s="96">
         <f>191.8/1.09</f>
         <v>175.96330275229357</v>
       </c>
-      <c r="I8" s="92"/>
-      <c r="J8" s="93"/>
-      <c r="K8" s="94"/>
-      <c r="L8" s="95"/>
-      <c r="M8" s="96"/>
-      <c r="S8" s="61"/>
-      <c r="T8" s="61"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="90"/>
-      <c r="B9" s="91">
+      <c r="I8" s="97"/>
+      <c r="J8" s="98"/>
+      <c r="K8" s="99"/>
+      <c r="L8" s="100"/>
+      <c r="M8" s="101"/>
+      <c r="P8" s="65" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q8" s="65" t="s">
+        <v>97</v>
+      </c>
+      <c r="S8" s="116" t="s">
+        <v>99</v>
+      </c>
+      <c r="T8" s="116" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="110"/>
+      <c r="B9" s="96">
         <f>35.5/7.25</f>
         <v>4.8965517241379306</v>
       </c>
-      <c r="C9" s="92"/>
-      <c r="D9" s="93"/>
-      <c r="E9" s="91">
+      <c r="C9" s="97"/>
+      <c r="D9" s="98"/>
+      <c r="E9" s="96">
         <f>37.8/1.12</f>
         <v>33.749999999999993</v>
       </c>
-      <c r="F9" s="92"/>
-      <c r="G9" s="93"/>
-      <c r="H9" s="91">
+      <c r="F9" s="97"/>
+      <c r="G9" s="98"/>
+      <c r="H9" s="96">
         <f>191.7/1.1</f>
         <v>174.27272727272725</v>
       </c>
-      <c r="I9" s="92"/>
-      <c r="J9" s="93"/>
-      <c r="K9" s="94"/>
-      <c r="L9" s="95"/>
-      <c r="M9" s="96"/>
-      <c r="S9" s="61"/>
-      <c r="T9" s="61"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I9" s="97"/>
+      <c r="J9" s="98"/>
+      <c r="K9" s="99"/>
+      <c r="L9" s="100"/>
+      <c r="M9" s="101"/>
+      <c r="O9" s="63" t="s">
+        <v>101</v>
+      </c>
+      <c r="P9" s="103" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q9" s="103"/>
+      <c r="R9" t="s">
+        <v>60</v>
+      </c>
+      <c r="S9" s="120"/>
+      <c r="T9" s="118">
+        <v>3000</v>
+      </c>
+      <c r="U9" s="119" t="s">
+        <v>105</v>
+      </c>
+      <c r="V9" s="120"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="105" t="s">
+      <c r="B10" s="93" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="106"/>
-      <c r="D10" s="107"/>
-      <c r="E10" s="105" t="s">
+      <c r="C10" s="94"/>
+      <c r="D10" s="95"/>
+      <c r="E10" s="93" t="s">
         <v>67</v>
       </c>
-      <c r="F10" s="106"/>
-      <c r="G10" s="107"/>
-      <c r="H10" s="105" t="s">
+      <c r="F10" s="94"/>
+      <c r="G10" s="95"/>
+      <c r="H10" s="93" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="106"/>
-      <c r="J10" s="107"/>
-      <c r="K10" s="105" t="s">
+      <c r="I10" s="94"/>
+      <c r="J10" s="95"/>
+      <c r="K10" s="93" t="s">
         <v>76</v>
       </c>
-      <c r="L10" s="106"/>
-      <c r="M10" s="107"/>
-      <c r="S10" s="61"/>
-      <c r="T10" s="61"/>
-    </row>
-    <row r="11" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="L10" s="94"/>
+      <c r="M10" s="95"/>
+      <c r="P10" s="65" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q10" s="65" t="s">
+        <v>104</v>
+      </c>
+      <c r="S10" s="117">
+        <f>U3</f>
+        <v>3.0683333333333335E-3</v>
+      </c>
+      <c r="T10" s="61" t="s">
+        <v>105</v>
+      </c>
+      <c r="U10">
+        <f>N5</f>
+        <v>21610</v>
+      </c>
+      <c r="V10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="30" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="102">
+      <c r="B11" s="87">
         <f>(336.12*1000)/($O$1*$O$2)</f>
         <v>5.6020000000000003</v>
       </c>
-      <c r="C11" s="103"/>
-      <c r="D11" s="104"/>
-      <c r="E11" s="102">
+      <c r="C11" s="88"/>
+      <c r="D11" s="89"/>
+      <c r="E11" s="87">
         <f>(1995.71*1000)/($O$1*$O$2)</f>
         <v>33.261833333333335</v>
       </c>
-      <c r="F11" s="103"/>
-      <c r="G11" s="104"/>
-      <c r="H11" s="102">
+      <c r="F11" s="88"/>
+      <c r="G11" s="89"/>
+      <c r="H11" s="87">
         <f>(9999.6*1000)/($O$1*$O$2)</f>
         <v>166.66</v>
       </c>
-      <c r="I11" s="103"/>
-      <c r="J11" s="104"/>
-      <c r="K11" s="102"/>
-      <c r="L11" s="103"/>
-      <c r="M11" s="104"/>
+      <c r="I11" s="88"/>
+      <c r="J11" s="89"/>
+      <c r="K11" s="87"/>
+      <c r="L11" s="88"/>
+      <c r="M11" s="89"/>
+      <c r="O11" s="63" t="s">
+        <v>101</v>
+      </c>
+      <c r="P11" s="55">
+        <f>T9/(S10*U10)*1000</f>
+        <v>45244.307951863069</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>107</v>
+      </c>
       <c r="S11" s="61"/>
       <c r="T11" s="61"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="S12" s="61"/>
       <c r="T12" s="61"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="97" t="s">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" s="111" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="111" t="s">
+      <c r="B13" s="113" t="s">
         <v>93</v>
       </c>
-      <c r="C13" s="112"/>
-      <c r="D13" s="113"/>
-      <c r="E13" s="111" t="s">
+      <c r="C13" s="114"/>
+      <c r="D13" s="115"/>
+      <c r="E13" s="113" t="s">
         <v>93</v>
       </c>
-      <c r="F13" s="112"/>
-      <c r="G13" s="113"/>
-      <c r="H13" s="111" t="s">
+      <c r="F13" s="114"/>
+      <c r="G13" s="115"/>
+      <c r="H13" s="113" t="s">
         <v>93</v>
       </c>
-      <c r="I13" s="112"/>
-      <c r="J13" s="113"/>
-      <c r="K13" s="85" t="s">
+      <c r="I13" s="114"/>
+      <c r="J13" s="115"/>
+      <c r="K13" s="105" t="s">
         <v>94</v>
       </c>
-      <c r="L13" s="86"/>
-      <c r="M13" s="87"/>
+      <c r="L13" s="106"/>
+      <c r="M13" s="107"/>
       <c r="S13" s="61"/>
       <c r="T13" s="61"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="98"/>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" s="112"/>
       <c r="B14" s="7" t="s">
         <v>0</v>
       </c>
@@ -4436,7 +4684,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
@@ -4485,202 +4733,202 @@
         <v>4645.7333333333336</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="88" t="s">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" s="108" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="91">
+      <c r="B16" s="96">
         <f>407.7/1.1</f>
         <v>370.63636363636357</v>
       </c>
-      <c r="C16" s="92"/>
-      <c r="D16" s="93"/>
-      <c r="E16" s="91">
+      <c r="C16" s="97"/>
+      <c r="D16" s="98"/>
+      <c r="E16" s="96">
         <f>1804.7/1.03</f>
         <v>1752.1359223300972</v>
       </c>
-      <c r="F16" s="92"/>
-      <c r="G16" s="93"/>
-      <c r="H16" s="91">
+      <c r="F16" s="97"/>
+      <c r="G16" s="98"/>
+      <c r="H16" s="96">
         <f>1796.1/(31/60)</f>
         <v>3476.3225806451605</v>
       </c>
-      <c r="I16" s="92"/>
-      <c r="J16" s="93"/>
-      <c r="K16" s="94"/>
-      <c r="L16" s="95"/>
-      <c r="M16" s="96"/>
+      <c r="I16" s="97"/>
+      <c r="J16" s="98"/>
+      <c r="K16" s="99"/>
+      <c r="L16" s="100"/>
+      <c r="M16" s="101"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="89"/>
-      <c r="B17" s="91">
+      <c r="A17" s="109"/>
+      <c r="B17" s="96">
         <f>401.3/1.09</f>
         <v>368.16513761467888</v>
       </c>
-      <c r="C17" s="92"/>
-      <c r="D17" s="93"/>
-      <c r="E17" s="91">
+      <c r="C17" s="97"/>
+      <c r="D17" s="98"/>
+      <c r="E17" s="96">
         <f>1744/1.01</f>
         <v>1726.7326732673266</v>
       </c>
-      <c r="F17" s="92"/>
-      <c r="G17" s="93"/>
-      <c r="H17" s="91">
+      <c r="F17" s="97"/>
+      <c r="G17" s="98"/>
+      <c r="H17" s="96">
         <f>1690.7/(29/60)</f>
         <v>3498</v>
       </c>
-      <c r="I17" s="92"/>
-      <c r="J17" s="93"/>
-      <c r="K17" s="91"/>
-      <c r="L17" s="92"/>
-      <c r="M17" s="93"/>
+      <c r="I17" s="97"/>
+      <c r="J17" s="98"/>
+      <c r="K17" s="96"/>
+      <c r="L17" s="97"/>
+      <c r="M17" s="98"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="89"/>
-      <c r="B18" s="91">
+      <c r="A18" s="109"/>
+      <c r="B18" s="96">
         <f>413.2/1.12</f>
         <v>368.92857142857139</v>
       </c>
-      <c r="C18" s="92"/>
-      <c r="D18" s="93"/>
-      <c r="E18" s="91">
+      <c r="C18" s="97"/>
+      <c r="D18" s="98"/>
+      <c r="E18" s="96">
         <f>1786/1.02</f>
         <v>1750.9803921568628</v>
       </c>
-      <c r="F18" s="92"/>
-      <c r="G18" s="93"/>
-      <c r="H18" s="91">
+      <c r="F18" s="97"/>
+      <c r="G18" s="98"/>
+      <c r="H18" s="96">
         <f>1838/(31/60)</f>
         <v>3557.4193548387093</v>
       </c>
-      <c r="I18" s="92"/>
-      <c r="J18" s="93"/>
-      <c r="K18" s="94"/>
-      <c r="L18" s="95"/>
-      <c r="M18" s="96"/>
+      <c r="I18" s="97"/>
+      <c r="J18" s="98"/>
+      <c r="K18" s="99"/>
+      <c r="L18" s="100"/>
+      <c r="M18" s="101"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="89"/>
-      <c r="B19" s="91">
+      <c r="A19" s="109"/>
+      <c r="B19" s="96">
         <f>406.3/1.11</f>
         <v>366.03603603603602</v>
       </c>
-      <c r="C19" s="92"/>
-      <c r="D19" s="93"/>
-      <c r="E19" s="91">
+      <c r="C19" s="97"/>
+      <c r="D19" s="98"/>
+      <c r="E19" s="96">
         <f>1801.7/1.02</f>
         <v>1766.372549019608</v>
       </c>
-      <c r="F19" s="92"/>
-      <c r="G19" s="93"/>
-      <c r="H19" s="91">
+      <c r="F19" s="97"/>
+      <c r="G19" s="98"/>
+      <c r="H19" s="96">
         <f>1751/(30/60)</f>
         <v>3502</v>
       </c>
-      <c r="I19" s="92"/>
-      <c r="J19" s="93"/>
-      <c r="K19" s="91"/>
-      <c r="L19" s="92"/>
-      <c r="M19" s="93"/>
+      <c r="I19" s="97"/>
+      <c r="J19" s="98"/>
+      <c r="K19" s="96"/>
+      <c r="L19" s="97"/>
+      <c r="M19" s="98"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="89"/>
-      <c r="B20" s="91">
+      <c r="A20" s="109"/>
+      <c r="B20" s="96">
         <f>419.5/1.14</f>
         <v>367.98245614035091</v>
       </c>
-      <c r="C20" s="92"/>
-      <c r="D20" s="93"/>
-      <c r="E20" s="91">
+      <c r="C20" s="97"/>
+      <c r="D20" s="98"/>
+      <c r="E20" s="96">
         <f>1738.2/1</f>
         <v>1738.2</v>
       </c>
-      <c r="F20" s="92"/>
-      <c r="G20" s="93"/>
-      <c r="H20" s="91">
+      <c r="F20" s="97"/>
+      <c r="G20" s="98"/>
+      <c r="H20" s="96">
         <f>1933.9/(33/60)</f>
         <v>3516.181818181818</v>
       </c>
-      <c r="I20" s="92"/>
-      <c r="J20" s="93"/>
-      <c r="K20" s="94"/>
-      <c r="L20" s="95"/>
-      <c r="M20" s="96"/>
+      <c r="I20" s="97"/>
+      <c r="J20" s="98"/>
+      <c r="K20" s="99"/>
+      <c r="L20" s="100"/>
+      <c r="M20" s="101"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="90"/>
-      <c r="B21" s="91">
+      <c r="A21" s="110"/>
+      <c r="B21" s="96">
         <f>405.1/1.13</f>
         <v>358.49557522123899</v>
       </c>
-      <c r="C21" s="92"/>
-      <c r="D21" s="93"/>
-      <c r="E21" s="91">
+      <c r="C21" s="97"/>
+      <c r="D21" s="98"/>
+      <c r="E21" s="96">
         <f>1734.7/1</f>
         <v>1734.7</v>
       </c>
-      <c r="F21" s="92"/>
-      <c r="G21" s="93"/>
-      <c r="H21" s="91">
+      <c r="F21" s="97"/>
+      <c r="G21" s="98"/>
+      <c r="H21" s="96">
         <f>1697.8/(29/60)</f>
         <v>3512.6896551724135</v>
       </c>
-      <c r="I21" s="92"/>
-      <c r="J21" s="93"/>
-      <c r="K21" s="94"/>
-      <c r="L21" s="95"/>
-      <c r="M21" s="96"/>
+      <c r="I21" s="97"/>
+      <c r="J21" s="98"/>
+      <c r="K21" s="99"/>
+      <c r="L21" s="100"/>
+      <c r="M21" s="101"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="105" t="s">
+      <c r="B22" s="93" t="s">
         <v>73</v>
       </c>
-      <c r="C22" s="106"/>
-      <c r="D22" s="107"/>
-      <c r="E22" s="105" t="s">
+      <c r="C22" s="94"/>
+      <c r="D22" s="95"/>
+      <c r="E22" s="93" t="s">
         <v>74</v>
       </c>
-      <c r="F22" s="106"/>
-      <c r="G22" s="107"/>
-      <c r="H22" s="105" t="s">
+      <c r="F22" s="94"/>
+      <c r="G22" s="95"/>
+      <c r="H22" s="93" t="s">
         <v>75</v>
       </c>
-      <c r="I22" s="106"/>
-      <c r="J22" s="107"/>
-      <c r="K22" s="105" t="s">
+      <c r="I22" s="94"/>
+      <c r="J22" s="95"/>
+      <c r="K22" s="93" t="s">
         <v>66</v>
       </c>
-      <c r="L22" s="106"/>
-      <c r="M22" s="107"/>
+      <c r="L22" s="94"/>
+      <c r="M22" s="95"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="102">
+      <c r="B23" s="87">
         <f>(19999.15*1000)/($O$1*$O$2)</f>
         <v>333.31916666666666</v>
       </c>
-      <c r="C23" s="103"/>
-      <c r="D23" s="104"/>
-      <c r="E23" s="102">
+      <c r="C23" s="88"/>
+      <c r="D23" s="89"/>
+      <c r="E23" s="87">
         <f>(99995.75*1000)/($O$1*$O$2)</f>
         <v>1666.5958333333333</v>
       </c>
-      <c r="F23" s="103"/>
-      <c r="G23" s="104"/>
-      <c r="H23" s="102">
+      <c r="F23" s="88"/>
+      <c r="G23" s="89"/>
+      <c r="H23" s="87">
         <f>1*(199991.48*1000)/($O$1*$O$2)</f>
         <v>3333.1913333333332</v>
       </c>
-      <c r="I23" s="103"/>
-      <c r="J23" s="104"/>
-      <c r="K23" s="108"/>
-      <c r="L23" s="109"/>
-      <c r="M23" s="110"/>
+      <c r="I23" s="88"/>
+      <c r="J23" s="89"/>
+      <c r="K23" s="90"/>
+      <c r="L23" s="91"/>
+      <c r="M23" s="92"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="22"/>
@@ -4704,10 +4952,10 @@
       <c r="B25" s="68" t="s">
         <v>77</v>
       </c>
-      <c r="D25" s="114" t="s">
+      <c r="D25" s="75" t="s">
         <v>59</v>
       </c>
-      <c r="E25" s="114" t="s">
+      <c r="E25" s="75" t="s">
         <v>78</v>
       </c>
       <c r="N25" s="68" t="s">
@@ -4739,7 +4987,7 @@
         <v>32</v>
       </c>
       <c r="J26" s="61">
-        <f>I26*$D$34+$G$34</f>
+        <f t="shared" ref="J26:J31" si="1">I26*$D$34+$G$34</f>
         <v>6.2972099999999998</v>
       </c>
       <c r="N26">
@@ -4765,14 +5013,14 @@
         <v>33.658498786127176</v>
       </c>
       <c r="E27" s="70">
-        <f t="shared" ref="E27:E33" si="1">(B27-D27)/B27</f>
+        <f t="shared" ref="E27:E33" si="2">(B27-D27)/B27</f>
         <v>-9.754963583815196E-3</v>
       </c>
       <c r="I27">
         <v>190</v>
       </c>
       <c r="J27" s="61">
-        <f>I27*$D$34+$G$34</f>
+        <f t="shared" si="1"/>
         <v>35.667830000000002</v>
       </c>
       <c r="N27">
@@ -4787,7 +5035,7 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="55">
-        <f t="shared" ref="A28:A32" si="2">(A27*B28)/B27</f>
+        <f t="shared" ref="A28:A32" si="3">(A27*B28)/B27</f>
         <v>895.95375722543361</v>
       </c>
       <c r="B28" s="61">
@@ -4798,14 +5046,14 @@
         <v>166.89757393063584</v>
       </c>
       <c r="E28" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.3854435838151177E-3</v>
       </c>
       <c r="I28">
         <v>952</v>
       </c>
       <c r="J28" s="61">
-        <f>I28*$D$34+$G$34</f>
+        <f t="shared" si="1"/>
         <v>177.31600999999998</v>
       </c>
       <c r="N28">
@@ -4820,7 +5068,7 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1343.9306358381505</v>
       </c>
       <c r="B29" s="61">
@@ -4831,14 +5079,14 @@
         <v>250.17199589595378</v>
       </c>
       <c r="E29" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-6.8798358381513933E-4</v>
       </c>
       <c r="I29">
         <v>1904</v>
       </c>
       <c r="J29" s="61">
-        <f>I29*$D$34+$G$34</f>
+        <f t="shared" si="1"/>
         <v>354.28328999999997</v>
       </c>
       <c r="N29">
@@ -4853,7 +5101,7 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1791.9075144508672</v>
       </c>
       <c r="B30" s="61">
@@ -4864,14 +5112,14 @@
         <v>333.4464178612717</v>
       </c>
       <c r="E30" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-3.3925358381515028E-4</v>
       </c>
       <c r="I30">
         <v>9520</v>
       </c>
       <c r="J30" s="61">
-        <f>I30*$D$34+$G$34</f>
+        <f t="shared" si="1"/>
         <v>1770.02153</v>
       </c>
       <c r="N30">
@@ -4886,7 +5134,7 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8959.5375722543376</v>
       </c>
       <c r="B31" s="61">
@@ -4897,14 +5145,14 @@
         <v>1665.8371693063586</v>
       </c>
       <c r="E31" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.9769841618485771E-4</v>
       </c>
       <c r="I31">
         <v>19040</v>
       </c>
       <c r="J31" s="61">
-        <f>I31*$D$34+$G$34</f>
+        <f t="shared" si="1"/>
         <v>3539.6943300000003</v>
       </c>
       <c r="N31">
@@ -4919,7 +5167,7 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>17919.075144508675</v>
       </c>
       <c r="B32" s="61">
@@ -4930,7 +5178,7 @@
         <v>3331.3256086127176</v>
       </c>
       <c r="E32" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.0231741618476916E-4</v>
       </c>
     </row>
@@ -4946,8 +5194,26 @@
         <v>4647.5987299999997</v>
       </c>
       <c r="E33" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-4.0152900152099321E-4</v>
+      </c>
+      <c r="I33" s="65" t="s">
+        <v>59</v>
+      </c>
+      <c r="J33" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="K33" s="65" t="s">
+        <v>99</v>
+      </c>
+      <c r="L33" s="65" t="s">
+        <v>63</v>
+      </c>
+      <c r="M33" s="65" t="s">
+        <v>62</v>
+      </c>
+      <c r="N33" s="65" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5104,29 +5370,48 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="76">
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="H22:J22"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="K20:M20"/>
+  <mergeCells count="79">
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="K10:M10"/>
     <mergeCell ref="K13:M13"/>
     <mergeCell ref="A16:A21"/>
     <mergeCell ref="B16:D16"/>
@@ -5143,44 +5428,28 @@
     <mergeCell ref="H19:J19"/>
     <mergeCell ref="K19:M19"/>
     <mergeCell ref="E17:G17"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="K22:M22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5225,9 +5494,9 @@
               </from>
               <to>
                 <xdr:col>20</xdr:col>
-                <xdr:colOff>228600</xdr:colOff>
-                <xdr:row>52</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:colOff>352425</xdr:colOff>
+                <xdr:row>53</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>

</xml_diff>

<commit_message>
Compilado y carga de datos a la bomba 1
20381 pulsos/mm
syringeLenght 45252
syringeVolume 3000
</commit_message>
<xml_diff>
--- a/Calibracion.xlsx
+++ b/Calibracion.xlsx
@@ -383,6 +383,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="P11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>NANOMEDICINA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+45251,7 dio calculo manual y se cargo en el software</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B16" authorId="0">
       <text>
         <r>
@@ -1069,7 +1093,7 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.000000"/>
     <numFmt numFmtId="167" formatCode="0.0%"/>
-    <numFmt numFmtId="175" formatCode="0.00000"/>
+    <numFmt numFmtId="168" formatCode="0.00000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -1907,16 +1931,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1933,6 +1962,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1943,6 +2029,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1951,66 +2046,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2020,21 +2055,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
@@ -2057,7 +2081,7 @@
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="0.000"/>
+      <numFmt numFmtId="169" formatCode="0.000"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -2259,11 +2283,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="75155136"/>
-        <c:axId val="75156864"/>
+        <c:axId val="151045824"/>
+        <c:axId val="151047552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="75155136"/>
+        <c:axId val="151045824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2273,12 +2297,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75156864"/>
+        <c:crossAx val="151047552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="75156864"/>
+        <c:axId val="151047552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2289,7 +2313,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75155136"/>
+        <c:crossAx val="151045824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2468,7 +2492,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2760,10 +2784,10 @@
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" customWidth="1"/>
@@ -2781,7 +2805,7 @@
     <col min="14" max="14" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>19</v>
       </c>
@@ -3096,47 +3120,47 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="77" t="s">
+      <c r="A8" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="78"/>
+      <c r="B8" s="83"/>
       <c r="C8" s="53">
         <v>16</v>
       </c>
-      <c r="D8" s="79" t="s">
+      <c r="D8" s="90" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="78"/>
+      <c r="E8" s="83"/>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" t="s">
         <v>44</v>
       </c>
-      <c r="H8" s="80" t="s">
+      <c r="H8" s="91" t="s">
         <v>45</v>
       </c>
-      <c r="I8" s="80"/>
+      <c r="I8" s="91"/>
       <c r="J8">
         <v>25</v>
       </c>
-      <c r="K8" s="80" t="s">
+      <c r="K8" s="91" t="s">
         <v>46</v>
       </c>
-      <c r="L8" s="80"/>
+      <c r="L8" s="91"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="77" t="s">
+      <c r="A9" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="78"/>
+      <c r="B9" s="83"/>
       <c r="C9" s="54">
         <v>200</v>
       </c>
-      <c r="D9" s="81" t="s">
+      <c r="D9" s="84" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="82"/>
+      <c r="E9" s="85"/>
       <c r="F9">
         <f>F8*B8</f>
         <v>0</v>
@@ -3144,31 +3168,31 @@
       <c r="G9" t="s">
         <v>48</v>
       </c>
-      <c r="H9" s="80" t="s">
+      <c r="H9" s="91" t="s">
         <v>49</v>
       </c>
-      <c r="I9" s="80"/>
+      <c r="I9" s="91"/>
       <c r="J9" s="55">
         <f>C10*J8</f>
         <v>1272.3724999999999</v>
       </c>
-      <c r="K9" s="80" t="s">
+      <c r="K9" s="91" t="s">
         <v>50</v>
       </c>
-      <c r="L9" s="80"/>
+      <c r="L9" s="91"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="77" t="s">
+      <c r="A10" s="82" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="78"/>
+      <c r="B10" s="83"/>
       <c r="C10" s="54">
         <v>50.8949</v>
       </c>
-      <c r="D10" s="81" t="s">
+      <c r="D10" s="84" t="s">
         <v>52</v>
       </c>
-      <c r="E10" s="82"/>
+      <c r="E10" s="85"/>
       <c r="J10" s="55">
         <f>J9*C9*C8/60</f>
         <v>67859.866666666669</v>
@@ -3179,31 +3203,31 @@
       <c r="L10" s="56"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="77" t="s">
+      <c r="A11" s="82" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="78"/>
+      <c r="B11" s="83"/>
       <c r="C11" s="54">
         <v>8</v>
       </c>
-      <c r="D11" s="83" t="s">
+      <c r="D11" s="86" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="84"/>
+      <c r="E11" s="87"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="85" t="s">
+      <c r="A12" s="88" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="86"/>
+      <c r="B12" s="89"/>
       <c r="C12" s="57">
         <f>C8*C9*C10/C11</f>
         <v>20357.96</v>
       </c>
-      <c r="D12" s="81" t="s">
+      <c r="D12" s="84" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="82"/>
+      <c r="E12" s="85"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -3234,12 +3258,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="H8:I8"/>
@@ -3248,6 +3266,12 @@
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="K9:L9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="D12:E12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="67" orientation="landscape" r:id="rId1"/>
@@ -3266,7 +3290,7 @@
       <selection activeCell="B10" sqref="B10:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
@@ -3298,39 +3322,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="111" t="s">
+      <c r="A1" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="105" t="s">
+      <c r="B1" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="106"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="105" t="s">
+      <c r="C1" s="93"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="106"/>
-      <c r="G1" s="107"/>
-      <c r="H1" s="105" t="s">
+      <c r="F1" s="93"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="106"/>
-      <c r="J1" s="107"/>
-      <c r="K1" s="105" t="s">
+      <c r="I1" s="93"/>
+      <c r="J1" s="94"/>
+      <c r="K1" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="106"/>
-      <c r="M1" s="107"/>
-      <c r="N1" s="105" t="s">
+      <c r="L1" s="93"/>
+      <c r="M1" s="94"/>
+      <c r="N1" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="106"/>
-      <c r="P1" s="107"/>
-      <c r="Q1" s="105" t="s">
+      <c r="O1" s="93"/>
+      <c r="P1" s="94"/>
+      <c r="Q1" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="R1" s="106"/>
-      <c r="S1" s="107"/>
+      <c r="R1" s="93"/>
+      <c r="S1" s="94"/>
       <c r="T1" t="s">
         <v>8</v>
       </c>
@@ -3342,7 +3366,7 @@
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="112"/>
+      <c r="A2" s="105"/>
       <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
@@ -3479,216 +3503,216 @@
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="108" t="s">
+      <c r="A4" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="96"/>
-      <c r="C4" s="97"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="99"/>
-      <c r="F4" s="100"/>
-      <c r="G4" s="101"/>
-      <c r="H4" s="96"/>
-      <c r="I4" s="97"/>
-      <c r="J4" s="98"/>
-      <c r="K4" s="96"/>
-      <c r="L4" s="97"/>
-      <c r="M4" s="98"/>
-      <c r="N4" s="96"/>
-      <c r="O4" s="97"/>
-      <c r="P4" s="98"/>
-      <c r="Q4" s="99"/>
-      <c r="R4" s="100"/>
-      <c r="S4" s="101"/>
+      <c r="B4" s="98"/>
+      <c r="C4" s="99"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="101"/>
+      <c r="F4" s="102"/>
+      <c r="G4" s="103"/>
+      <c r="H4" s="98"/>
+      <c r="I4" s="99"/>
+      <c r="J4" s="100"/>
+      <c r="K4" s="98"/>
+      <c r="L4" s="99"/>
+      <c r="M4" s="100"/>
+      <c r="N4" s="98"/>
+      <c r="O4" s="99"/>
+      <c r="P4" s="100"/>
+      <c r="Q4" s="101"/>
+      <c r="R4" s="102"/>
+      <c r="S4" s="103"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="109"/>
-      <c r="B5" s="96"/>
-      <c r="C5" s="97"/>
-      <c r="D5" s="98"/>
-      <c r="E5" s="99"/>
-      <c r="F5" s="100"/>
-      <c r="G5" s="101"/>
-      <c r="H5" s="96"/>
-      <c r="I5" s="97"/>
-      <c r="J5" s="98"/>
-      <c r="K5" s="99"/>
-      <c r="L5" s="100"/>
-      <c r="M5" s="101"/>
-      <c r="N5" s="96"/>
-      <c r="O5" s="97"/>
-      <c r="P5" s="98"/>
-      <c r="Q5" s="96"/>
-      <c r="R5" s="97"/>
-      <c r="S5" s="98"/>
+      <c r="A5" s="96"/>
+      <c r="B5" s="98"/>
+      <c r="C5" s="99"/>
+      <c r="D5" s="100"/>
+      <c r="E5" s="101"/>
+      <c r="F5" s="102"/>
+      <c r="G5" s="103"/>
+      <c r="H5" s="98"/>
+      <c r="I5" s="99"/>
+      <c r="J5" s="100"/>
+      <c r="K5" s="101"/>
+      <c r="L5" s="102"/>
+      <c r="M5" s="103"/>
+      <c r="N5" s="98"/>
+      <c r="O5" s="99"/>
+      <c r="P5" s="100"/>
+      <c r="Q5" s="98"/>
+      <c r="R5" s="99"/>
+      <c r="S5" s="100"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="109"/>
-      <c r="B6" s="96"/>
-      <c r="C6" s="97"/>
-      <c r="D6" s="98"/>
-      <c r="E6" s="99"/>
-      <c r="F6" s="100"/>
-      <c r="G6" s="101"/>
-      <c r="H6" s="96"/>
-      <c r="I6" s="97"/>
-      <c r="J6" s="98"/>
-      <c r="K6" s="99"/>
-      <c r="L6" s="100"/>
-      <c r="M6" s="101"/>
-      <c r="N6" s="96"/>
-      <c r="O6" s="97"/>
-      <c r="P6" s="98"/>
-      <c r="Q6" s="99"/>
-      <c r="R6" s="100"/>
-      <c r="S6" s="101"/>
+      <c r="A6" s="96"/>
+      <c r="B6" s="98"/>
+      <c r="C6" s="99"/>
+      <c r="D6" s="100"/>
+      <c r="E6" s="101"/>
+      <c r="F6" s="102"/>
+      <c r="G6" s="103"/>
+      <c r="H6" s="98"/>
+      <c r="I6" s="99"/>
+      <c r="J6" s="100"/>
+      <c r="K6" s="101"/>
+      <c r="L6" s="102"/>
+      <c r="M6" s="103"/>
+      <c r="N6" s="98"/>
+      <c r="O6" s="99"/>
+      <c r="P6" s="100"/>
+      <c r="Q6" s="101"/>
+      <c r="R6" s="102"/>
+      <c r="S6" s="103"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="109"/>
-      <c r="B7" s="96"/>
-      <c r="C7" s="97"/>
-      <c r="D7" s="98"/>
-      <c r="E7" s="99"/>
-      <c r="F7" s="100"/>
-      <c r="G7" s="101"/>
-      <c r="H7" s="96"/>
-      <c r="I7" s="97"/>
-      <c r="J7" s="98"/>
-      <c r="K7" s="99"/>
-      <c r="L7" s="100"/>
-      <c r="M7" s="101"/>
-      <c r="N7" s="96"/>
-      <c r="O7" s="97"/>
-      <c r="P7" s="98"/>
-      <c r="Q7" s="96"/>
-      <c r="R7" s="97"/>
-      <c r="S7" s="98"/>
+      <c r="A7" s="96"/>
+      <c r="B7" s="98"/>
+      <c r="C7" s="99"/>
+      <c r="D7" s="100"/>
+      <c r="E7" s="101"/>
+      <c r="F7" s="102"/>
+      <c r="G7" s="103"/>
+      <c r="H7" s="98"/>
+      <c r="I7" s="99"/>
+      <c r="J7" s="100"/>
+      <c r="K7" s="101"/>
+      <c r="L7" s="102"/>
+      <c r="M7" s="103"/>
+      <c r="N7" s="98"/>
+      <c r="O7" s="99"/>
+      <c r="P7" s="100"/>
+      <c r="Q7" s="98"/>
+      <c r="R7" s="99"/>
+      <c r="S7" s="100"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="109"/>
-      <c r="B8" s="96"/>
-      <c r="C8" s="97"/>
-      <c r="D8" s="98"/>
-      <c r="E8" s="99"/>
-      <c r="F8" s="100"/>
-      <c r="G8" s="101"/>
-      <c r="H8" s="96"/>
-      <c r="I8" s="97"/>
-      <c r="J8" s="98"/>
-      <c r="K8" s="99"/>
-      <c r="L8" s="100"/>
-      <c r="M8" s="101"/>
-      <c r="N8" s="96"/>
-      <c r="O8" s="97"/>
-      <c r="P8" s="98"/>
-      <c r="Q8" s="99"/>
-      <c r="R8" s="100"/>
-      <c r="S8" s="101"/>
+      <c r="A8" s="96"/>
+      <c r="B8" s="98"/>
+      <c r="C8" s="99"/>
+      <c r="D8" s="100"/>
+      <c r="E8" s="101"/>
+      <c r="F8" s="102"/>
+      <c r="G8" s="103"/>
+      <c r="H8" s="98"/>
+      <c r="I8" s="99"/>
+      <c r="J8" s="100"/>
+      <c r="K8" s="101"/>
+      <c r="L8" s="102"/>
+      <c r="M8" s="103"/>
+      <c r="N8" s="98"/>
+      <c r="O8" s="99"/>
+      <c r="P8" s="100"/>
+      <c r="Q8" s="101"/>
+      <c r="R8" s="102"/>
+      <c r="S8" s="103"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="110"/>
-      <c r="B9" s="96"/>
-      <c r="C9" s="97"/>
-      <c r="D9" s="98"/>
-      <c r="E9" s="102"/>
-      <c r="F9" s="103"/>
-      <c r="G9" s="104"/>
-      <c r="H9" s="96"/>
-      <c r="I9" s="97"/>
-      <c r="J9" s="98"/>
-      <c r="K9" s="102"/>
-      <c r="L9" s="103"/>
-      <c r="M9" s="104"/>
-      <c r="N9" s="96"/>
-      <c r="O9" s="97"/>
-      <c r="P9" s="98"/>
-      <c r="Q9" s="99"/>
-      <c r="R9" s="100"/>
-      <c r="S9" s="101"/>
+      <c r="A9" s="97"/>
+      <c r="B9" s="98"/>
+      <c r="C9" s="99"/>
+      <c r="D9" s="100"/>
+      <c r="E9" s="106"/>
+      <c r="F9" s="107"/>
+      <c r="G9" s="108"/>
+      <c r="H9" s="98"/>
+      <c r="I9" s="99"/>
+      <c r="J9" s="100"/>
+      <c r="K9" s="106"/>
+      <c r="L9" s="107"/>
+      <c r="M9" s="108"/>
+      <c r="N9" s="98"/>
+      <c r="O9" s="99"/>
+      <c r="P9" s="100"/>
+      <c r="Q9" s="101"/>
+      <c r="R9" s="102"/>
+      <c r="S9" s="103"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="93"/>
-      <c r="C10" s="94"/>
-      <c r="D10" s="95"/>
-      <c r="E10" s="93"/>
-      <c r="F10" s="94"/>
-      <c r="G10" s="95"/>
-      <c r="H10" s="93"/>
-      <c r="I10" s="94"/>
-      <c r="J10" s="95"/>
-      <c r="K10" s="93"/>
-      <c r="L10" s="94"/>
-      <c r="M10" s="95"/>
-      <c r="N10" s="93"/>
-      <c r="O10" s="94"/>
-      <c r="P10" s="95"/>
-      <c r="Q10" s="93"/>
-      <c r="R10" s="94"/>
-      <c r="S10" s="95"/>
+      <c r="B10" s="112"/>
+      <c r="C10" s="113"/>
+      <c r="D10" s="114"/>
+      <c r="E10" s="112"/>
+      <c r="F10" s="113"/>
+      <c r="G10" s="114"/>
+      <c r="H10" s="112"/>
+      <c r="I10" s="113"/>
+      <c r="J10" s="114"/>
+      <c r="K10" s="112"/>
+      <c r="L10" s="113"/>
+      <c r="M10" s="114"/>
+      <c r="N10" s="112"/>
+      <c r="O10" s="113"/>
+      <c r="P10" s="114"/>
+      <c r="Q10" s="112"/>
+      <c r="R10" s="113"/>
+      <c r="S10" s="114"/>
     </row>
     <row r="11" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="87"/>
-      <c r="C11" s="88"/>
-      <c r="D11" s="89"/>
-      <c r="E11" s="87"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="89"/>
-      <c r="H11" s="87"/>
-      <c r="I11" s="88"/>
-      <c r="J11" s="89"/>
-      <c r="K11" s="87"/>
-      <c r="L11" s="88"/>
-      <c r="M11" s="89"/>
-      <c r="N11" s="87"/>
-      <c r="O11" s="88"/>
-      <c r="P11" s="89"/>
-      <c r="Q11" s="87"/>
-      <c r="R11" s="88"/>
-      <c r="S11" s="89"/>
+      <c r="B11" s="109"/>
+      <c r="C11" s="110"/>
+      <c r="D11" s="111"/>
+      <c r="E11" s="109"/>
+      <c r="F11" s="110"/>
+      <c r="G11" s="111"/>
+      <c r="H11" s="109"/>
+      <c r="I11" s="110"/>
+      <c r="J11" s="111"/>
+      <c r="K11" s="109"/>
+      <c r="L11" s="110"/>
+      <c r="M11" s="111"/>
+      <c r="N11" s="109"/>
+      <c r="O11" s="110"/>
+      <c r="P11" s="111"/>
+      <c r="Q11" s="109"/>
+      <c r="R11" s="110"/>
+      <c r="S11" s="111"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="111" t="s">
+      <c r="A13" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="105" t="s">
+      <c r="B13" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="106"/>
-      <c r="D13" s="107"/>
-      <c r="E13" s="105" t="s">
+      <c r="C13" s="93"/>
+      <c r="D13" s="94"/>
+      <c r="E13" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="F13" s="106"/>
-      <c r="G13" s="107"/>
-      <c r="H13" s="105" t="s">
+      <c r="F13" s="93"/>
+      <c r="G13" s="94"/>
+      <c r="H13" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="I13" s="106"/>
-      <c r="J13" s="107"/>
-      <c r="K13" s="105" t="s">
+      <c r="I13" s="93"/>
+      <c r="J13" s="94"/>
+      <c r="K13" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="L13" s="106"/>
-      <c r="M13" s="107"/>
-      <c r="N13" s="105" t="s">
+      <c r="L13" s="93"/>
+      <c r="M13" s="94"/>
+      <c r="N13" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="O13" s="106"/>
-      <c r="P13" s="107"/>
-      <c r="Q13" s="105" t="s">
+      <c r="O13" s="93"/>
+      <c r="P13" s="94"/>
+      <c r="Q13" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="R13" s="106"/>
-      <c r="S13" s="107"/>
+      <c r="R13" s="93"/>
+      <c r="S13" s="94"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="112"/>
+      <c r="A14" s="105"/>
       <c r="B14" s="11" t="s">
         <v>0</v>
       </c>
@@ -3816,181 +3840,269 @@
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="108" t="s">
+      <c r="A16" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="96"/>
-      <c r="C16" s="97"/>
-      <c r="D16" s="98"/>
-      <c r="E16" s="99"/>
-      <c r="F16" s="100"/>
-      <c r="G16" s="101"/>
-      <c r="H16" s="96"/>
-      <c r="I16" s="97"/>
-      <c r="J16" s="98"/>
-      <c r="K16" s="99"/>
-      <c r="L16" s="100"/>
-      <c r="M16" s="101"/>
-      <c r="N16" s="96"/>
-      <c r="O16" s="97"/>
-      <c r="P16" s="98"/>
-      <c r="Q16" s="99"/>
-      <c r="R16" s="100"/>
-      <c r="S16" s="101"/>
+      <c r="B16" s="98"/>
+      <c r="C16" s="99"/>
+      <c r="D16" s="100"/>
+      <c r="E16" s="101"/>
+      <c r="F16" s="102"/>
+      <c r="G16" s="103"/>
+      <c r="H16" s="98"/>
+      <c r="I16" s="99"/>
+      <c r="J16" s="100"/>
+      <c r="K16" s="101"/>
+      <c r="L16" s="102"/>
+      <c r="M16" s="103"/>
+      <c r="N16" s="98"/>
+      <c r="O16" s="99"/>
+      <c r="P16" s="100"/>
+      <c r="Q16" s="101"/>
+      <c r="R16" s="102"/>
+      <c r="S16" s="103"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="109"/>
-      <c r="B17" s="96"/>
-      <c r="C17" s="97"/>
-      <c r="D17" s="98"/>
-      <c r="E17" s="99"/>
-      <c r="F17" s="100"/>
-      <c r="G17" s="101"/>
-      <c r="H17" s="96"/>
-      <c r="I17" s="97"/>
-      <c r="J17" s="98"/>
-      <c r="K17" s="99"/>
-      <c r="L17" s="100"/>
-      <c r="M17" s="101"/>
-      <c r="N17" s="96"/>
-      <c r="O17" s="97"/>
-      <c r="P17" s="98"/>
-      <c r="Q17" s="96"/>
-      <c r="R17" s="97"/>
-      <c r="S17" s="98"/>
+      <c r="A17" s="96"/>
+      <c r="B17" s="98"/>
+      <c r="C17" s="99"/>
+      <c r="D17" s="100"/>
+      <c r="E17" s="101"/>
+      <c r="F17" s="102"/>
+      <c r="G17" s="103"/>
+      <c r="H17" s="98"/>
+      <c r="I17" s="99"/>
+      <c r="J17" s="100"/>
+      <c r="K17" s="101"/>
+      <c r="L17" s="102"/>
+      <c r="M17" s="103"/>
+      <c r="N17" s="98"/>
+      <c r="O17" s="99"/>
+      <c r="P17" s="100"/>
+      <c r="Q17" s="98"/>
+      <c r="R17" s="99"/>
+      <c r="S17" s="100"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="109"/>
-      <c r="B18" s="96"/>
-      <c r="C18" s="97"/>
-      <c r="D18" s="98"/>
-      <c r="E18" s="99"/>
-      <c r="F18" s="100"/>
-      <c r="G18" s="101"/>
-      <c r="H18" s="96"/>
-      <c r="I18" s="97"/>
-      <c r="J18" s="98"/>
-      <c r="K18" s="99"/>
-      <c r="L18" s="100"/>
-      <c r="M18" s="101"/>
-      <c r="N18" s="96"/>
-      <c r="O18" s="97"/>
-      <c r="P18" s="98"/>
-      <c r="Q18" s="99"/>
-      <c r="R18" s="100"/>
-      <c r="S18" s="101"/>
+      <c r="A18" s="96"/>
+      <c r="B18" s="98"/>
+      <c r="C18" s="99"/>
+      <c r="D18" s="100"/>
+      <c r="E18" s="101"/>
+      <c r="F18" s="102"/>
+      <c r="G18" s="103"/>
+      <c r="H18" s="98"/>
+      <c r="I18" s="99"/>
+      <c r="J18" s="100"/>
+      <c r="K18" s="101"/>
+      <c r="L18" s="102"/>
+      <c r="M18" s="103"/>
+      <c r="N18" s="98"/>
+      <c r="O18" s="99"/>
+      <c r="P18" s="100"/>
+      <c r="Q18" s="101"/>
+      <c r="R18" s="102"/>
+      <c r="S18" s="103"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="109"/>
-      <c r="B19" s="96"/>
-      <c r="C19" s="97"/>
-      <c r="D19" s="98"/>
-      <c r="E19" s="99"/>
-      <c r="F19" s="100"/>
-      <c r="G19" s="101"/>
-      <c r="H19" s="96"/>
-      <c r="I19" s="97"/>
-      <c r="J19" s="98"/>
-      <c r="K19" s="99"/>
-      <c r="L19" s="100"/>
-      <c r="M19" s="101"/>
-      <c r="N19" s="96"/>
-      <c r="O19" s="97"/>
-      <c r="P19" s="98"/>
-      <c r="Q19" s="96"/>
-      <c r="R19" s="97"/>
-      <c r="S19" s="98"/>
+      <c r="A19" s="96"/>
+      <c r="B19" s="98"/>
+      <c r="C19" s="99"/>
+      <c r="D19" s="100"/>
+      <c r="E19" s="101"/>
+      <c r="F19" s="102"/>
+      <c r="G19" s="103"/>
+      <c r="H19" s="98"/>
+      <c r="I19" s="99"/>
+      <c r="J19" s="100"/>
+      <c r="K19" s="101"/>
+      <c r="L19" s="102"/>
+      <c r="M19" s="103"/>
+      <c r="N19" s="98"/>
+      <c r="O19" s="99"/>
+      <c r="P19" s="100"/>
+      <c r="Q19" s="98"/>
+      <c r="R19" s="99"/>
+      <c r="S19" s="100"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="109"/>
-      <c r="B20" s="96"/>
-      <c r="C20" s="97"/>
-      <c r="D20" s="98"/>
-      <c r="E20" s="99"/>
-      <c r="F20" s="100"/>
-      <c r="G20" s="101"/>
-      <c r="H20" s="96"/>
-      <c r="I20" s="97"/>
-      <c r="J20" s="98"/>
-      <c r="K20" s="99"/>
-      <c r="L20" s="100"/>
-      <c r="M20" s="101"/>
-      <c r="N20" s="96"/>
-      <c r="O20" s="97"/>
-      <c r="P20" s="98"/>
-      <c r="Q20" s="99"/>
-      <c r="R20" s="100"/>
-      <c r="S20" s="101"/>
+      <c r="A20" s="96"/>
+      <c r="B20" s="98"/>
+      <c r="C20" s="99"/>
+      <c r="D20" s="100"/>
+      <c r="E20" s="101"/>
+      <c r="F20" s="102"/>
+      <c r="G20" s="103"/>
+      <c r="H20" s="98"/>
+      <c r="I20" s="99"/>
+      <c r="J20" s="100"/>
+      <c r="K20" s="101"/>
+      <c r="L20" s="102"/>
+      <c r="M20" s="103"/>
+      <c r="N20" s="98"/>
+      <c r="O20" s="99"/>
+      <c r="P20" s="100"/>
+      <c r="Q20" s="101"/>
+      <c r="R20" s="102"/>
+      <c r="S20" s="103"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="110"/>
-      <c r="B21" s="96"/>
-      <c r="C21" s="97"/>
-      <c r="D21" s="98"/>
-      <c r="E21" s="102"/>
-      <c r="F21" s="103"/>
-      <c r="G21" s="104"/>
-      <c r="H21" s="96"/>
-      <c r="I21" s="97"/>
-      <c r="J21" s="98"/>
-      <c r="K21" s="102"/>
-      <c r="L21" s="103"/>
-      <c r="M21" s="104"/>
-      <c r="N21" s="96"/>
-      <c r="O21" s="97"/>
-      <c r="P21" s="98"/>
-      <c r="Q21" s="99"/>
-      <c r="R21" s="100"/>
-      <c r="S21" s="101"/>
+      <c r="A21" s="97"/>
+      <c r="B21" s="98"/>
+      <c r="C21" s="99"/>
+      <c r="D21" s="100"/>
+      <c r="E21" s="106"/>
+      <c r="F21" s="107"/>
+      <c r="G21" s="108"/>
+      <c r="H21" s="98"/>
+      <c r="I21" s="99"/>
+      <c r="J21" s="100"/>
+      <c r="K21" s="106"/>
+      <c r="L21" s="107"/>
+      <c r="M21" s="108"/>
+      <c r="N21" s="98"/>
+      <c r="O21" s="99"/>
+      <c r="P21" s="100"/>
+      <c r="Q21" s="101"/>
+      <c r="R21" s="102"/>
+      <c r="S21" s="103"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="93"/>
-      <c r="C22" s="94"/>
-      <c r="D22" s="95"/>
-      <c r="E22" s="93"/>
-      <c r="F22" s="94"/>
-      <c r="G22" s="95"/>
-      <c r="H22" s="93"/>
-      <c r="I22" s="94"/>
-      <c r="J22" s="95"/>
-      <c r="K22" s="93"/>
-      <c r="L22" s="94"/>
-      <c r="M22" s="95"/>
-      <c r="N22" s="93"/>
-      <c r="O22" s="94"/>
-      <c r="P22" s="95"/>
-      <c r="Q22" s="93"/>
-      <c r="R22" s="94"/>
-      <c r="S22" s="95"/>
+      <c r="B22" s="112"/>
+      <c r="C22" s="113"/>
+      <c r="D22" s="114"/>
+      <c r="E22" s="112"/>
+      <c r="F22" s="113"/>
+      <c r="G22" s="114"/>
+      <c r="H22" s="112"/>
+      <c r="I22" s="113"/>
+      <c r="J22" s="114"/>
+      <c r="K22" s="112"/>
+      <c r="L22" s="113"/>
+      <c r="M22" s="114"/>
+      <c r="N22" s="112"/>
+      <c r="O22" s="113"/>
+      <c r="P22" s="114"/>
+      <c r="Q22" s="112"/>
+      <c r="R22" s="113"/>
+      <c r="S22" s="114"/>
     </row>
     <row r="23" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="87"/>
-      <c r="C23" s="88"/>
-      <c r="D23" s="89"/>
-      <c r="E23" s="87"/>
-      <c r="F23" s="88"/>
-      <c r="G23" s="89"/>
-      <c r="H23" s="87"/>
-      <c r="I23" s="88"/>
-      <c r="J23" s="89"/>
-      <c r="K23" s="90"/>
-      <c r="L23" s="91"/>
-      <c r="M23" s="92"/>
-      <c r="N23" s="87"/>
-      <c r="O23" s="88"/>
-      <c r="P23" s="89"/>
-      <c r="Q23" s="90"/>
-      <c r="R23" s="91"/>
-      <c r="S23" s="92"/>
+      <c r="B23" s="109"/>
+      <c r="C23" s="110"/>
+      <c r="D23" s="111"/>
+      <c r="E23" s="109"/>
+      <c r="F23" s="110"/>
+      <c r="G23" s="111"/>
+      <c r="H23" s="109"/>
+      <c r="I23" s="110"/>
+      <c r="J23" s="111"/>
+      <c r="K23" s="115"/>
+      <c r="L23" s="116"/>
+      <c r="M23" s="117"/>
+      <c r="N23" s="109"/>
+      <c r="O23" s="110"/>
+      <c r="P23" s="111"/>
+      <c r="Q23" s="115"/>
+      <c r="R23" s="116"/>
+      <c r="S23" s="117"/>
     </row>
   </sheetData>
   <mergeCells count="112">
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="N23:P23"/>
+    <mergeCell ref="Q23:S23"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="N22:P22"/>
+    <mergeCell ref="Q22:S22"/>
+    <mergeCell ref="N17:P17"/>
+    <mergeCell ref="Q17:S17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="N18:P18"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="N21:P21"/>
+    <mergeCell ref="Q21:S21"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="Q20:S20"/>
+    <mergeCell ref="Q13:S13"/>
+    <mergeCell ref="A16:A21"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="N16:P16"/>
+    <mergeCell ref="Q16:S16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="N13:P13"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="N19:P19"/>
+    <mergeCell ref="Q19:S19"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="N11:P11"/>
+    <mergeCell ref="Q11:S11"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="Q10:S10"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="Q5:S5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="Q6:S6"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="N8:P8"/>
+    <mergeCell ref="Q8:S8"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="A4:A9"/>
     <mergeCell ref="B4:D4"/>
@@ -4015,94 +4127,6 @@
     <mergeCell ref="Q7:S7"/>
     <mergeCell ref="H5:J5"/>
     <mergeCell ref="K5:M5"/>
-    <mergeCell ref="N5:P5"/>
-    <mergeCell ref="Q5:S5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="Q6:S6"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="N9:P9"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="N8:P8"/>
-    <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="N11:P11"/>
-    <mergeCell ref="Q11:S11"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="N10:P10"/>
-    <mergeCell ref="Q10:S10"/>
-    <mergeCell ref="Q13:S13"/>
-    <mergeCell ref="A16:A21"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="N16:P16"/>
-    <mergeCell ref="Q16:S16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="N13:P13"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="N19:P19"/>
-    <mergeCell ref="Q19:S19"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="N17:P17"/>
-    <mergeCell ref="Q17:S17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="N18:P18"/>
-    <mergeCell ref="Q18:S18"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="N21:P21"/>
-    <mergeCell ref="Q21:S21"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="N20:P20"/>
-    <mergeCell ref="Q20:S20"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="N23:P23"/>
-    <mergeCell ref="Q23:S23"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="H22:J22"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="N22:P22"/>
-    <mergeCell ref="Q22:S22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4115,10 +4139,10 @@
   <dimension ref="A1:V44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
@@ -4144,29 +4168,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="111" t="s">
+      <c r="A1" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="113" t="s">
+      <c r="B1" s="118" t="s">
         <v>92</v>
       </c>
-      <c r="C1" s="114"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="113" t="s">
+      <c r="C1" s="119"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="118" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="114"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="113" t="s">
+      <c r="F1" s="119"/>
+      <c r="G1" s="120"/>
+      <c r="H1" s="118" t="s">
         <v>93</v>
       </c>
-      <c r="I1" s="114"/>
-      <c r="J1" s="115"/>
-      <c r="K1" s="113" t="s">
+      <c r="I1" s="119"/>
+      <c r="J1" s="120"/>
+      <c r="K1" s="118" t="s">
         <v>93</v>
       </c>
-      <c r="L1" s="114"/>
-      <c r="M1" s="115"/>
+      <c r="L1" s="119"/>
+      <c r="M1" s="120"/>
       <c r="N1" s="76" t="s">
         <v>8</v>
       </c>
@@ -4196,7 +4220,7 @@
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="112"/>
+      <c r="A2" s="105"/>
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
@@ -4310,7 +4334,7 @@
       <c r="T3" s="65" t="s">
         <v>60</v>
       </c>
-      <c r="U3" s="117">
+      <c r="U3" s="78">
         <f>U2/60</f>
         <v>3.0683333333333335E-3</v>
       </c>
@@ -4319,30 +4343,30 @@
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="108" t="s">
+      <c r="A4" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="96">
+      <c r="B4" s="98">
         <f>36.2/7.05</f>
         <v>5.1347517730496461</v>
       </c>
-      <c r="C4" s="97"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="96">
+      <c r="C4" s="99"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="98">
         <f>39/1.16</f>
         <v>33.620689655172413</v>
       </c>
-      <c r="F4" s="97"/>
-      <c r="G4" s="98"/>
-      <c r="H4" s="96">
+      <c r="F4" s="99"/>
+      <c r="G4" s="100"/>
+      <c r="H4" s="98">
         <f>195/1.09</f>
         <v>178.89908256880733</v>
       </c>
-      <c r="I4" s="97"/>
-      <c r="J4" s="98"/>
-      <c r="K4" s="99"/>
-      <c r="L4" s="100"/>
-      <c r="M4" s="101"/>
+      <c r="I4" s="99"/>
+      <c r="J4" s="100"/>
+      <c r="K4" s="101"/>
+      <c r="L4" s="102"/>
+      <c r="M4" s="103"/>
       <c r="N4" s="63" t="s">
         <v>91</v>
       </c>
@@ -4358,28 +4382,28 @@
       <c r="R4" s="72"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="109"/>
-      <c r="B5" s="96">
+      <c r="A5" s="96"/>
+      <c r="B5" s="98">
         <f>37.9/7.11</f>
         <v>5.3305203938115326</v>
       </c>
-      <c r="C5" s="97"/>
-      <c r="D5" s="98"/>
-      <c r="E5" s="96">
+      <c r="C5" s="99"/>
+      <c r="D5" s="100"/>
+      <c r="E5" s="98">
         <f>38.6/1.17</f>
         <v>32.991452991452995</v>
       </c>
-      <c r="F5" s="97"/>
-      <c r="G5" s="98"/>
-      <c r="H5" s="96">
+      <c r="F5" s="99"/>
+      <c r="G5" s="100"/>
+      <c r="H5" s="98">
         <f>194/1.11</f>
         <v>174.77477477477476</v>
       </c>
-      <c r="I5" s="97"/>
-      <c r="J5" s="98"/>
-      <c r="K5" s="96"/>
-      <c r="L5" s="97"/>
-      <c r="M5" s="98"/>
+      <c r="I5" s="99"/>
+      <c r="J5" s="100"/>
+      <c r="K5" s="98"/>
+      <c r="L5" s="99"/>
+      <c r="M5" s="100"/>
       <c r="N5">
         <f>'Flow Rate'!C16</f>
         <v>21610</v>
@@ -4392,176 +4416,176 @@
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="109"/>
-      <c r="B6" s="96">
+      <c r="A6" s="96"/>
+      <c r="B6" s="98">
         <f>37/7.03</f>
         <v>5.2631578947368416</v>
       </c>
-      <c r="C6" s="97"/>
-      <c r="D6" s="98"/>
-      <c r="E6" s="96">
+      <c r="C6" s="99"/>
+      <c r="D6" s="100"/>
+      <c r="E6" s="98">
         <f>38.2/1.16</f>
         <v>32.931034482758626</v>
       </c>
-      <c r="F6" s="97"/>
-      <c r="G6" s="98"/>
-      <c r="H6" s="96">
+      <c r="F6" s="99"/>
+      <c r="G6" s="100"/>
+      <c r="H6" s="98">
         <f>194.3/1.1</f>
         <v>176.63636363636363</v>
       </c>
-      <c r="I6" s="97"/>
-      <c r="J6" s="98"/>
-      <c r="K6" s="99"/>
-      <c r="L6" s="100"/>
-      <c r="M6" s="101"/>
+      <c r="I6" s="99"/>
+      <c r="J6" s="100"/>
+      <c r="K6" s="101"/>
+      <c r="L6" s="102"/>
+      <c r="M6" s="103"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="109"/>
-      <c r="B7" s="96">
+      <c r="A7" s="96"/>
+      <c r="B7" s="98">
         <f>36/6.48</f>
         <v>5.5555555555555554</v>
       </c>
-      <c r="C7" s="97"/>
-      <c r="D7" s="98"/>
-      <c r="E7" s="96">
+      <c r="C7" s="99"/>
+      <c r="D7" s="100"/>
+      <c r="E7" s="98">
         <f>38/1.15</f>
         <v>33.04347826086957</v>
       </c>
-      <c r="F7" s="97"/>
-      <c r="G7" s="98"/>
-      <c r="H7" s="96">
+      <c r="F7" s="99"/>
+      <c r="G7" s="100"/>
+      <c r="H7" s="98">
         <f>192.4/1.08</f>
         <v>178.14814814814815</v>
       </c>
-      <c r="I7" s="97"/>
-      <c r="J7" s="98"/>
-      <c r="K7" s="96"/>
-      <c r="L7" s="97"/>
-      <c r="M7" s="98"/>
+      <c r="I7" s="99"/>
+      <c r="J7" s="100"/>
+      <c r="K7" s="98"/>
+      <c r="L7" s="99"/>
+      <c r="M7" s="100"/>
       <c r="O7" s="63" t="s">
         <v>95</v>
       </c>
-      <c r="P7" s="103" t="s">
+      <c r="P7" s="107" t="s">
         <v>98</v>
       </c>
-      <c r="Q7" s="103"/>
+      <c r="Q7" s="107"/>
       <c r="R7" s="65" t="s">
         <v>60</v>
       </c>
-      <c r="S7" s="103" t="s">
+      <c r="S7" s="107" t="s">
         <v>98</v>
       </c>
-      <c r="T7" s="103"/>
+      <c r="T7" s="107"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="109"/>
-      <c r="B8" s="96">
+      <c r="A8" s="96"/>
+      <c r="B8" s="98">
         <f>32.8/6.39</f>
         <v>5.1330203442879494</v>
       </c>
-      <c r="C8" s="97"/>
-      <c r="D8" s="98"/>
-      <c r="E8" s="96">
+      <c r="C8" s="99"/>
+      <c r="D8" s="100"/>
+      <c r="E8" s="98">
         <f>38.1/1.14</f>
         <v>33.421052631578952</v>
       </c>
-      <c r="F8" s="97"/>
-      <c r="G8" s="98"/>
-      <c r="H8" s="96">
+      <c r="F8" s="99"/>
+      <c r="G8" s="100"/>
+      <c r="H8" s="98">
         <f>191.8/1.09</f>
         <v>175.96330275229357</v>
       </c>
-      <c r="I8" s="97"/>
-      <c r="J8" s="98"/>
-      <c r="K8" s="99"/>
-      <c r="L8" s="100"/>
-      <c r="M8" s="101"/>
+      <c r="I8" s="99"/>
+      <c r="J8" s="100"/>
+      <c r="K8" s="101"/>
+      <c r="L8" s="102"/>
+      <c r="M8" s="103"/>
       <c r="P8" s="65" t="s">
         <v>96</v>
       </c>
       <c r="Q8" s="65" t="s">
         <v>97</v>
       </c>
-      <c r="S8" s="116" t="s">
+      <c r="S8" s="77" t="s">
         <v>99</v>
       </c>
-      <c r="T8" s="116" t="s">
+      <c r="T8" s="77" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="110"/>
-      <c r="B9" s="96">
+      <c r="A9" s="97"/>
+      <c r="B9" s="98">
         <f>35.5/7.25</f>
         <v>4.8965517241379306</v>
       </c>
-      <c r="C9" s="97"/>
-      <c r="D9" s="98"/>
-      <c r="E9" s="96">
+      <c r="C9" s="99"/>
+      <c r="D9" s="100"/>
+      <c r="E9" s="98">
         <f>37.8/1.12</f>
         <v>33.749999999999993</v>
       </c>
-      <c r="F9" s="97"/>
-      <c r="G9" s="98"/>
-      <c r="H9" s="96">
+      <c r="F9" s="99"/>
+      <c r="G9" s="100"/>
+      <c r="H9" s="98">
         <f>191.7/1.1</f>
         <v>174.27272727272725</v>
       </c>
-      <c r="I9" s="97"/>
-      <c r="J9" s="98"/>
-      <c r="K9" s="99"/>
-      <c r="L9" s="100"/>
-      <c r="M9" s="101"/>
+      <c r="I9" s="99"/>
+      <c r="J9" s="100"/>
+      <c r="K9" s="101"/>
+      <c r="L9" s="102"/>
+      <c r="M9" s="103"/>
       <c r="O9" s="63" t="s">
         <v>101</v>
       </c>
-      <c r="P9" s="103" t="s">
+      <c r="P9" s="107" t="s">
         <v>102</v>
       </c>
-      <c r="Q9" s="103"/>
+      <c r="Q9" s="107"/>
       <c r="R9" t="s">
         <v>60</v>
       </c>
-      <c r="S9" s="120"/>
-      <c r="T9" s="118">
+      <c r="S9" s="81"/>
+      <c r="T9" s="79">
         <v>3000</v>
       </c>
-      <c r="U9" s="119" t="s">
+      <c r="U9" s="80" t="s">
         <v>105</v>
       </c>
-      <c r="V9" s="120"/>
+      <c r="V9" s="81"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="93" t="s">
+      <c r="B10" s="112" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="94"/>
-      <c r="D10" s="95"/>
-      <c r="E10" s="93" t="s">
+      <c r="C10" s="113"/>
+      <c r="D10" s="114"/>
+      <c r="E10" s="112" t="s">
         <v>67</v>
       </c>
-      <c r="F10" s="94"/>
-      <c r="G10" s="95"/>
-      <c r="H10" s="93" t="s">
+      <c r="F10" s="113"/>
+      <c r="G10" s="114"/>
+      <c r="H10" s="112" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="94"/>
-      <c r="J10" s="95"/>
-      <c r="K10" s="93" t="s">
+      <c r="I10" s="113"/>
+      <c r="J10" s="114"/>
+      <c r="K10" s="112" t="s">
         <v>76</v>
       </c>
-      <c r="L10" s="94"/>
-      <c r="M10" s="95"/>
+      <c r="L10" s="113"/>
+      <c r="M10" s="114"/>
       <c r="P10" s="65" t="s">
         <v>103</v>
       </c>
       <c r="Q10" s="65" t="s">
         <v>104</v>
       </c>
-      <c r="S10" s="117">
+      <c r="S10" s="78">
         <f>U3</f>
         <v>3.0683333333333335E-3</v>
       </c>
@@ -4580,27 +4604,27 @@
       <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="87">
+      <c r="B11" s="109">
         <f>(336.12*1000)/($O$1*$O$2)</f>
         <v>5.6020000000000003</v>
       </c>
-      <c r="C11" s="88"/>
-      <c r="D11" s="89"/>
-      <c r="E11" s="87">
+      <c r="C11" s="110"/>
+      <c r="D11" s="111"/>
+      <c r="E11" s="109">
         <f>(1995.71*1000)/($O$1*$O$2)</f>
         <v>33.261833333333335</v>
       </c>
-      <c r="F11" s="88"/>
-      <c r="G11" s="89"/>
-      <c r="H11" s="87">
+      <c r="F11" s="110"/>
+      <c r="G11" s="111"/>
+      <c r="H11" s="109">
         <f>(9999.6*1000)/($O$1*$O$2)</f>
         <v>166.66</v>
       </c>
-      <c r="I11" s="88"/>
-      <c r="J11" s="89"/>
-      <c r="K11" s="87"/>
-      <c r="L11" s="88"/>
-      <c r="M11" s="89"/>
+      <c r="I11" s="110"/>
+      <c r="J11" s="111"/>
+      <c r="K11" s="109"/>
+      <c r="L11" s="110"/>
+      <c r="M11" s="111"/>
       <c r="O11" s="63" t="s">
         <v>101</v>
       </c>
@@ -4619,34 +4643,34 @@
       <c r="T12" s="61"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="111" t="s">
+      <c r="A13" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="113" t="s">
+      <c r="B13" s="118" t="s">
         <v>93</v>
       </c>
-      <c r="C13" s="114"/>
-      <c r="D13" s="115"/>
-      <c r="E13" s="113" t="s">
+      <c r="C13" s="119"/>
+      <c r="D13" s="120"/>
+      <c r="E13" s="118" t="s">
         <v>93</v>
       </c>
-      <c r="F13" s="114"/>
-      <c r="G13" s="115"/>
-      <c r="H13" s="113" t="s">
+      <c r="F13" s="119"/>
+      <c r="G13" s="120"/>
+      <c r="H13" s="118" t="s">
         <v>93</v>
       </c>
-      <c r="I13" s="114"/>
-      <c r="J13" s="115"/>
-      <c r="K13" s="105" t="s">
+      <c r="I13" s="119"/>
+      <c r="J13" s="120"/>
+      <c r="K13" s="92" t="s">
         <v>94</v>
       </c>
-      <c r="L13" s="106"/>
-      <c r="M13" s="107"/>
+      <c r="L13" s="93"/>
+      <c r="M13" s="94"/>
       <c r="S13" s="61"/>
       <c r="T13" s="61"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="112"/>
+      <c r="A14" s="105"/>
       <c r="B14" s="7" t="s">
         <v>0</v>
       </c>
@@ -4734,201 +4758,201 @@
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="108" t="s">
+      <c r="A16" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="96">
+      <c r="B16" s="98">
         <f>407.7/1.1</f>
         <v>370.63636363636357</v>
       </c>
-      <c r="C16" s="97"/>
-      <c r="D16" s="98"/>
-      <c r="E16" s="96">
+      <c r="C16" s="99"/>
+      <c r="D16" s="100"/>
+      <c r="E16" s="98">
         <f>1804.7/1.03</f>
         <v>1752.1359223300972</v>
       </c>
-      <c r="F16" s="97"/>
-      <c r="G16" s="98"/>
-      <c r="H16" s="96">
+      <c r="F16" s="99"/>
+      <c r="G16" s="100"/>
+      <c r="H16" s="98">
         <f>1796.1/(31/60)</f>
         <v>3476.3225806451605</v>
       </c>
-      <c r="I16" s="97"/>
-      <c r="J16" s="98"/>
-      <c r="K16" s="99"/>
-      <c r="L16" s="100"/>
-      <c r="M16" s="101"/>
+      <c r="I16" s="99"/>
+      <c r="J16" s="100"/>
+      <c r="K16" s="101"/>
+      <c r="L16" s="102"/>
+      <c r="M16" s="103"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="109"/>
-      <c r="B17" s="96">
+      <c r="A17" s="96"/>
+      <c r="B17" s="98">
         <f>401.3/1.09</f>
         <v>368.16513761467888</v>
       </c>
-      <c r="C17" s="97"/>
-      <c r="D17" s="98"/>
-      <c r="E17" s="96">
+      <c r="C17" s="99"/>
+      <c r="D17" s="100"/>
+      <c r="E17" s="98">
         <f>1744/1.01</f>
         <v>1726.7326732673266</v>
       </c>
-      <c r="F17" s="97"/>
-      <c r="G17" s="98"/>
-      <c r="H17" s="96">
+      <c r="F17" s="99"/>
+      <c r="G17" s="100"/>
+      <c r="H17" s="98">
         <f>1690.7/(29/60)</f>
         <v>3498</v>
       </c>
-      <c r="I17" s="97"/>
-      <c r="J17" s="98"/>
-      <c r="K17" s="96"/>
-      <c r="L17" s="97"/>
-      <c r="M17" s="98"/>
+      <c r="I17" s="99"/>
+      <c r="J17" s="100"/>
+      <c r="K17" s="98"/>
+      <c r="L17" s="99"/>
+      <c r="M17" s="100"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="109"/>
-      <c r="B18" s="96">
+      <c r="A18" s="96"/>
+      <c r="B18" s="98">
         <f>413.2/1.12</f>
         <v>368.92857142857139</v>
       </c>
-      <c r="C18" s="97"/>
-      <c r="D18" s="98"/>
-      <c r="E18" s="96">
+      <c r="C18" s="99"/>
+      <c r="D18" s="100"/>
+      <c r="E18" s="98">
         <f>1786/1.02</f>
         <v>1750.9803921568628</v>
       </c>
-      <c r="F18" s="97"/>
-      <c r="G18" s="98"/>
-      <c r="H18" s="96">
+      <c r="F18" s="99"/>
+      <c r="G18" s="100"/>
+      <c r="H18" s="98">
         <f>1838/(31/60)</f>
         <v>3557.4193548387093</v>
       </c>
-      <c r="I18" s="97"/>
-      <c r="J18" s="98"/>
-      <c r="K18" s="99"/>
-      <c r="L18" s="100"/>
-      <c r="M18" s="101"/>
+      <c r="I18" s="99"/>
+      <c r="J18" s="100"/>
+      <c r="K18" s="101"/>
+      <c r="L18" s="102"/>
+      <c r="M18" s="103"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="109"/>
-      <c r="B19" s="96">
+      <c r="A19" s="96"/>
+      <c r="B19" s="98">
         <f>406.3/1.11</f>
         <v>366.03603603603602</v>
       </c>
-      <c r="C19" s="97"/>
-      <c r="D19" s="98"/>
-      <c r="E19" s="96">
+      <c r="C19" s="99"/>
+      <c r="D19" s="100"/>
+      <c r="E19" s="98">
         <f>1801.7/1.02</f>
         <v>1766.372549019608</v>
       </c>
-      <c r="F19" s="97"/>
-      <c r="G19" s="98"/>
-      <c r="H19" s="96">
+      <c r="F19" s="99"/>
+      <c r="G19" s="100"/>
+      <c r="H19" s="98">
         <f>1751/(30/60)</f>
         <v>3502</v>
       </c>
-      <c r="I19" s="97"/>
-      <c r="J19" s="98"/>
-      <c r="K19" s="96"/>
-      <c r="L19" s="97"/>
-      <c r="M19" s="98"/>
+      <c r="I19" s="99"/>
+      <c r="J19" s="100"/>
+      <c r="K19" s="98"/>
+      <c r="L19" s="99"/>
+      <c r="M19" s="100"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="109"/>
-      <c r="B20" s="96">
+      <c r="A20" s="96"/>
+      <c r="B20" s="98">
         <f>419.5/1.14</f>
         <v>367.98245614035091</v>
       </c>
-      <c r="C20" s="97"/>
-      <c r="D20" s="98"/>
-      <c r="E20" s="96">
+      <c r="C20" s="99"/>
+      <c r="D20" s="100"/>
+      <c r="E20" s="98">
         <f>1738.2/1</f>
         <v>1738.2</v>
       </c>
-      <c r="F20" s="97"/>
-      <c r="G20" s="98"/>
-      <c r="H20" s="96">
+      <c r="F20" s="99"/>
+      <c r="G20" s="100"/>
+      <c r="H20" s="98">
         <f>1933.9/(33/60)</f>
         <v>3516.181818181818</v>
       </c>
-      <c r="I20" s="97"/>
-      <c r="J20" s="98"/>
-      <c r="K20" s="99"/>
-      <c r="L20" s="100"/>
-      <c r="M20" s="101"/>
+      <c r="I20" s="99"/>
+      <c r="J20" s="100"/>
+      <c r="K20" s="101"/>
+      <c r="L20" s="102"/>
+      <c r="M20" s="103"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="110"/>
-      <c r="B21" s="96">
+      <c r="A21" s="97"/>
+      <c r="B21" s="98">
         <f>405.1/1.13</f>
         <v>358.49557522123899</v>
       </c>
-      <c r="C21" s="97"/>
-      <c r="D21" s="98"/>
-      <c r="E21" s="96">
+      <c r="C21" s="99"/>
+      <c r="D21" s="100"/>
+      <c r="E21" s="98">
         <f>1734.7/1</f>
         <v>1734.7</v>
       </c>
-      <c r="F21" s="97"/>
-      <c r="G21" s="98"/>
-      <c r="H21" s="96">
+      <c r="F21" s="99"/>
+      <c r="G21" s="100"/>
+      <c r="H21" s="98">
         <f>1697.8/(29/60)</f>
         <v>3512.6896551724135</v>
       </c>
-      <c r="I21" s="97"/>
-      <c r="J21" s="98"/>
-      <c r="K21" s="99"/>
-      <c r="L21" s="100"/>
-      <c r="M21" s="101"/>
+      <c r="I21" s="99"/>
+      <c r="J21" s="100"/>
+      <c r="K21" s="101"/>
+      <c r="L21" s="102"/>
+      <c r="M21" s="103"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="93" t="s">
+      <c r="B22" s="112" t="s">
         <v>73</v>
       </c>
-      <c r="C22" s="94"/>
-      <c r="D22" s="95"/>
-      <c r="E22" s="93" t="s">
+      <c r="C22" s="113"/>
+      <c r="D22" s="114"/>
+      <c r="E22" s="112" t="s">
         <v>74</v>
       </c>
-      <c r="F22" s="94"/>
-      <c r="G22" s="95"/>
-      <c r="H22" s="93" t="s">
+      <c r="F22" s="113"/>
+      <c r="G22" s="114"/>
+      <c r="H22" s="112" t="s">
         <v>75</v>
       </c>
-      <c r="I22" s="94"/>
-      <c r="J22" s="95"/>
-      <c r="K22" s="93" t="s">
+      <c r="I22" s="113"/>
+      <c r="J22" s="114"/>
+      <c r="K22" s="112" t="s">
         <v>66</v>
       </c>
-      <c r="L22" s="94"/>
-      <c r="M22" s="95"/>
+      <c r="L22" s="113"/>
+      <c r="M22" s="114"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="87">
+      <c r="B23" s="109">
         <f>(19999.15*1000)/($O$1*$O$2)</f>
         <v>333.31916666666666</v>
       </c>
-      <c r="C23" s="88"/>
-      <c r="D23" s="89"/>
-      <c r="E23" s="87">
+      <c r="C23" s="110"/>
+      <c r="D23" s="111"/>
+      <c r="E23" s="109">
         <f>(99995.75*1000)/($O$1*$O$2)</f>
         <v>1666.5958333333333</v>
       </c>
-      <c r="F23" s="88"/>
-      <c r="G23" s="89"/>
-      <c r="H23" s="87">
+      <c r="F23" s="110"/>
+      <c r="G23" s="111"/>
+      <c r="H23" s="109">
         <f>1*(199991.48*1000)/($O$1*$O$2)</f>
         <v>3333.1913333333332</v>
       </c>
-      <c r="I23" s="88"/>
-      <c r="J23" s="89"/>
-      <c r="K23" s="90"/>
-      <c r="L23" s="91"/>
-      <c r="M23" s="92"/>
+      <c r="I23" s="110"/>
+      <c r="J23" s="111"/>
+      <c r="K23" s="115"/>
+      <c r="L23" s="116"/>
+      <c r="M23" s="117"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="22"/>
@@ -5371,6 +5395,69 @@
     </row>
   </sheetData>
   <mergeCells count="79">
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="A16:A21"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="H6:J6"/>
     <mergeCell ref="P7:Q7"/>
     <mergeCell ref="S7:T7"/>
     <mergeCell ref="P9:Q9"/>
@@ -5387,69 +5474,6 @@
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="E7:G7"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="A16:A21"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="H22:J22"/>
-    <mergeCell ref="K22:M22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5518,7 +5542,7 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
@@ -5588,7 +5612,7 @@
       <selection activeCell="G1" sqref="G1:G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1">

</xml_diff>

<commit_message>
Curva de calibracion bomba 1
</commit_message>
<xml_diff>
--- a/Calibracion.xlsx
+++ b/Calibracion.xlsx
@@ -4,14 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="20115" windowHeight="7950" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="20115" windowHeight="7950" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Flow Rate" sheetId="5" r:id="rId1"/>
-    <sheet name="3mL Bomba 1" sheetId="7" r:id="rId2"/>
-    <sheet name="3mL Bomba 2" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
-    <sheet name="Hoja1" sheetId="6" r:id="rId5"/>
+    <sheet name="3mL Bomba 2" sheetId="4" r:id="rId2"/>
+    <sheet name="3mL Bomba 1" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -104,6 +102,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>NANOMEDICINA</author>
+    <author>Lisbeth</author>
   </authors>
   <commentList>
     <comment ref="B4" authorId="0">
@@ -130,7 +129,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H4" authorId="0">
+    <comment ref="E4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -155,7 +154,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N4" authorId="0">
+    <comment ref="H4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -203,6 +202,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="P11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>NANOMEDICINA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+45251,7 dio calculo manual y se cargo en el software</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B16" authorId="0">
       <text>
         <r>
@@ -224,6 +247,30 @@
           </rPr>
           <t xml:space="preserve">
 20 gotas</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E16" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>NANOMEDICINA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+80 gotas</t>
         </r>
       </text>
     </comment>
@@ -251,7 +298,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N16" authorId="0">
+    <comment ref="B34" authorId="1">
       <text>
         <r>
           <rPr>
@@ -261,6 +308,102 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
+          <t>Lisbeth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Flujo (mg/min)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E34" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lisbeth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Frecuencia (Hz)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N34" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lisbeth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Flujo (mg/min)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q34" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lisbeth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Frecuencia (Hz)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H36" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
           <t>NANOMEDICINA:</t>
         </r>
         <r>
@@ -271,7 +414,80 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-80 gotas</t>
+teórico</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I36" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lisbeth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+mg/min</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J36" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>NANOMEDICINA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+teórico
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H37" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>NANOMEDICINA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+experimental</t>
         </r>
       </text>
     </comment>
@@ -383,7 +599,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P11" authorId="0">
+    <comment ref="U10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -391,7 +607,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>NANOMEDICINA:</t>
         </r>
@@ -400,10 +616,10 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-45251,7 dio calculo manual y se cargo en el software</t>
+45251,7 dio calculo manual y se cargo en el software (de la calibración de la bomba 2)</t>
         </r>
       </text>
     </comment>
@@ -479,6 +695,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="J25" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>NANOMEDICINA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+basado en la ecuación teórica</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B34" authorId="1">
       <text>
         <r>
@@ -527,7 +767,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N34" authorId="1">
+    <comment ref="M34" authorId="1">
       <text>
         <r>
           <rPr>
@@ -551,7 +791,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q34" authorId="1">
+    <comment ref="P34" authorId="1">
       <text>
         <r>
           <rPr>
@@ -575,7 +815,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H36" authorId="0">
+    <comment ref="H38" authorId="0">
       <text>
         <r>
           <rPr>
@@ -599,7 +839,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I36" authorId="1">
+    <comment ref="I38" authorId="1">
       <text>
         <r>
           <rPr>
@@ -623,7 +863,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J36" authorId="0">
+    <comment ref="J38" authorId="0">
       <text>
         <r>
           <rPr>
@@ -648,7 +888,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H37" authorId="0">
+    <comment ref="H39" authorId="0">
       <text>
         <r>
           <rPr>
@@ -677,7 +917,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="120">
   <si>
     <t>uL/h</t>
   </si>
@@ -939,9 +1179,6 @@
   </si>
   <si>
     <t>promedio</t>
-  </si>
-  <si>
-    <t>error</t>
   </si>
   <si>
     <t>Frecuencia experimental (Hz)</t>
@@ -1083,6 +1320,67 @@
   <si>
     <t>um</t>
   </si>
+  <si>
+    <t>31/31</t>
+  </si>
+  <si>
+    <t>170/179</t>
+  </si>
+  <si>
+    <t>853/896</t>
+  </si>
+  <si>
+    <t>1707/1792</t>
+  </si>
+  <si>
+    <t>8539/8960</t>
+  </si>
+  <si>
+    <t>17079/17919</t>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">e </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(mm)</t>
+    </r>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>% error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modo 4: </t>
+  </si>
+  <si>
+    <t>1500 uL</t>
+  </si>
+  <si>
+    <t>30 s</t>
+  </si>
+  <si>
+    <t>Repeticiones (mg)</t>
+  </si>
 </sst>
 </file>
 
@@ -1095,7 +1393,7 @@
     <numFmt numFmtId="167" formatCode="0.0%"/>
     <numFmt numFmtId="168" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1144,6 +1442,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1741,7 +2052,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1942,10 +2253,22 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1962,11 +2285,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1986,66 +2351,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2054,6 +2365,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2155,185 +2473,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="es-AR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Hoja1!$A$1:$A$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Hoja1!$B$1:$B$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>5.1347500000000004</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.3305199999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.2631600000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.5555599999999998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.1330200000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.8965500000000004</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>33.620690000000003</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>32.99145</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>32.93103</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>33.043480000000002</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>33.421050000000001</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>33.75</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="151045824"/>
-        <c:axId val="151047552"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="151045824"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151047552"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="151047552"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151045824"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2423,36 +2562,88 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="3 Gráfico"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>57150</xdr:colOff>
+          <xdr:row>36</xdr:row>
+          <xdr:rowOff>114300</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>238125</xdr:colOff>
+          <xdr:row>54</xdr:row>
+          <xdr:rowOff>76200</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9231" name="Object 15" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9231"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>12</xdr:col>
+          <xdr:colOff>50802</xdr:colOff>
+          <xdr:row>35</xdr:row>
+          <xdr:rowOff>114299</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>20</xdr:col>
+          <xdr:colOff>9527</xdr:colOff>
+          <xdr:row>53</xdr:row>
+          <xdr:rowOff>161924</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9235" name="Object 19" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9235"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
@@ -3120,47 +3311,47 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="82" t="s">
+      <c r="A8" s="84" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="83"/>
+      <c r="B8" s="85"/>
       <c r="C8" s="53">
         <v>16</v>
       </c>
-      <c r="D8" s="90" t="s">
+      <c r="D8" s="86" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="83"/>
+      <c r="E8" s="85"/>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" t="s">
         <v>44</v>
       </c>
-      <c r="H8" s="91" t="s">
+      <c r="H8" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="I8" s="91"/>
+      <c r="I8" s="87"/>
       <c r="J8">
         <v>25</v>
       </c>
-      <c r="K8" s="91" t="s">
+      <c r="K8" s="87" t="s">
         <v>46</v>
       </c>
-      <c r="L8" s="91"/>
+      <c r="L8" s="87"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="82" t="s">
+      <c r="A9" s="84" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="83"/>
+      <c r="B9" s="85"/>
       <c r="C9" s="54">
         <v>200</v>
       </c>
-      <c r="D9" s="84" t="s">
+      <c r="D9" s="88" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="85"/>
+      <c r="E9" s="89"/>
       <c r="F9">
         <f>F8*B8</f>
         <v>0</v>
@@ -3168,31 +3359,31 @@
       <c r="G9" t="s">
         <v>48</v>
       </c>
-      <c r="H9" s="91" t="s">
+      <c r="H9" s="87" t="s">
         <v>49</v>
       </c>
-      <c r="I9" s="91"/>
+      <c r="I9" s="87"/>
       <c r="J9" s="55">
         <f>C10*J8</f>
         <v>1272.3724999999999</v>
       </c>
-      <c r="K9" s="91" t="s">
+      <c r="K9" s="87" t="s">
         <v>50</v>
       </c>
-      <c r="L9" s="91"/>
+      <c r="L9" s="87"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="82" t="s">
+      <c r="A10" s="84" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="83"/>
+      <c r="B10" s="85"/>
       <c r="C10" s="54">
         <v>50.8949</v>
       </c>
-      <c r="D10" s="84" t="s">
+      <c r="D10" s="88" t="s">
         <v>52</v>
       </c>
-      <c r="E10" s="85"/>
+      <c r="E10" s="89"/>
       <c r="J10" s="55">
         <f>J9*C9*C8/60</f>
         <v>67859.866666666669</v>
@@ -3203,31 +3394,31 @@
       <c r="L10" s="56"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="82" t="s">
+      <c r="A11" s="84" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="83"/>
+      <c r="B11" s="85"/>
       <c r="C11" s="54">
         <v>8</v>
       </c>
-      <c r="D11" s="86" t="s">
+      <c r="D11" s="90" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="87"/>
+      <c r="E11" s="91"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="88" t="s">
+      <c r="A12" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="89"/>
+      <c r="B12" s="93"/>
       <c r="C12" s="57">
         <f>C8*C9*C10/C11</f>
         <v>20357.96</v>
       </c>
-      <c r="D12" s="84" t="s">
+      <c r="D12" s="88" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="85"/>
+      <c r="E12" s="89"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -3258,6 +3449,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="H8:I8"/>
@@ -3266,12 +3463,6 @@
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="K9:L9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="D12:E12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="67" orientation="landscape" r:id="rId1"/>
@@ -3284,862 +3475,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V23"/>
+  <dimension ref="A1:V52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:D10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8" customWidth="1"/>
-    <col min="20" max="20" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="2" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="6" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="104" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="92" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="93"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="92" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="93"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="92" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="93"/>
-      <c r="J1" s="94"/>
-      <c r="K1" s="92" t="s">
-        <v>3</v>
-      </c>
-      <c r="L1" s="93"/>
-      <c r="M1" s="94"/>
-      <c r="N1" s="92" t="s">
-        <v>3</v>
-      </c>
-      <c r="O1" s="93"/>
-      <c r="P1" s="94"/>
-      <c r="Q1" s="92" t="s">
-        <v>3</v>
-      </c>
-      <c r="R1" s="93"/>
-      <c r="S1" s="94"/>
-      <c r="T1" t="s">
-        <v>8</v>
-      </c>
-      <c r="U1">
-        <v>60</v>
-      </c>
-      <c r="V1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="105"/>
-      <c r="B2" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="M2" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="N2" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="P2" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q2" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="R2" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="S2" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="T2" t="s">
-        <v>10</v>
-      </c>
-      <c r="U2">
-        <v>1000</v>
-      </c>
-      <c r="V2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1">
-        <v>346</v>
-      </c>
-      <c r="C3" s="2">
-        <f>B3/($U$1*$U$2)</f>
-        <v>5.7666666666666665E-3</v>
-      </c>
-      <c r="D3" s="3">
-        <f>C3*1000</f>
-        <v>5.7666666666666666</v>
-      </c>
-      <c r="E3" s="1">
-        <v>1000</v>
-      </c>
-      <c r="F3" s="2">
-        <f>E3/($U$1*$U$2)</f>
-        <v>1.6666666666666666E-2</v>
-      </c>
-      <c r="G3" s="3">
-        <f>F3*1000</f>
-        <v>16.666666666666668</v>
-      </c>
-      <c r="H3" s="1">
-        <v>2000</v>
-      </c>
-      <c r="I3" s="2">
-        <f>H3/($U$1*$U$2)</f>
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="J3" s="3">
-        <f>I3*1000</f>
-        <v>33.333333333333336</v>
-      </c>
-      <c r="K3" s="1">
-        <v>5000</v>
-      </c>
-      <c r="L3" s="2">
-        <f>K3/($U$1*$U$2)</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="M3" s="3">
-        <f>L3*1000</f>
-        <v>83.333333333333329</v>
-      </c>
-      <c r="N3" s="1">
-        <v>10000</v>
-      </c>
-      <c r="O3" s="2">
-        <f>N3/($U$1*$U$2)</f>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="P3" s="3">
-        <f>O3*1000</f>
-        <v>166.66666666666666</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>15000</v>
-      </c>
-      <c r="R3" s="2">
-        <f>Q3/($U$1*$U$2)</f>
-        <v>0.25</v>
-      </c>
-      <c r="S3" s="3">
-        <f>R3*1000</f>
-        <v>250</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="95" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="98"/>
-      <c r="C4" s="99"/>
-      <c r="D4" s="100"/>
-      <c r="E4" s="101"/>
-      <c r="F4" s="102"/>
-      <c r="G4" s="103"/>
-      <c r="H4" s="98"/>
-      <c r="I4" s="99"/>
-      <c r="J4" s="100"/>
-      <c r="K4" s="98"/>
-      <c r="L4" s="99"/>
-      <c r="M4" s="100"/>
-      <c r="N4" s="98"/>
-      <c r="O4" s="99"/>
-      <c r="P4" s="100"/>
-      <c r="Q4" s="101"/>
-      <c r="R4" s="102"/>
-      <c r="S4" s="103"/>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="96"/>
-      <c r="B5" s="98"/>
-      <c r="C5" s="99"/>
-      <c r="D5" s="100"/>
-      <c r="E5" s="101"/>
-      <c r="F5" s="102"/>
-      <c r="G5" s="103"/>
-      <c r="H5" s="98"/>
-      <c r="I5" s="99"/>
-      <c r="J5" s="100"/>
-      <c r="K5" s="101"/>
-      <c r="L5" s="102"/>
-      <c r="M5" s="103"/>
-      <c r="N5" s="98"/>
-      <c r="O5" s="99"/>
-      <c r="P5" s="100"/>
-      <c r="Q5" s="98"/>
-      <c r="R5" s="99"/>
-      <c r="S5" s="100"/>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="96"/>
-      <c r="B6" s="98"/>
-      <c r="C6" s="99"/>
-      <c r="D6" s="100"/>
-      <c r="E6" s="101"/>
-      <c r="F6" s="102"/>
-      <c r="G6" s="103"/>
-      <c r="H6" s="98"/>
-      <c r="I6" s="99"/>
-      <c r="J6" s="100"/>
-      <c r="K6" s="101"/>
-      <c r="L6" s="102"/>
-      <c r="M6" s="103"/>
-      <c r="N6" s="98"/>
-      <c r="O6" s="99"/>
-      <c r="P6" s="100"/>
-      <c r="Q6" s="101"/>
-      <c r="R6" s="102"/>
-      <c r="S6" s="103"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="96"/>
-      <c r="B7" s="98"/>
-      <c r="C7" s="99"/>
-      <c r="D7" s="100"/>
-      <c r="E7" s="101"/>
-      <c r="F7" s="102"/>
-      <c r="G7" s="103"/>
-      <c r="H7" s="98"/>
-      <c r="I7" s="99"/>
-      <c r="J7" s="100"/>
-      <c r="K7" s="101"/>
-      <c r="L7" s="102"/>
-      <c r="M7" s="103"/>
-      <c r="N7" s="98"/>
-      <c r="O7" s="99"/>
-      <c r="P7" s="100"/>
-      <c r="Q7" s="98"/>
-      <c r="R7" s="99"/>
-      <c r="S7" s="100"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="96"/>
-      <c r="B8" s="98"/>
-      <c r="C8" s="99"/>
-      <c r="D8" s="100"/>
-      <c r="E8" s="101"/>
-      <c r="F8" s="102"/>
-      <c r="G8" s="103"/>
-      <c r="H8" s="98"/>
-      <c r="I8" s="99"/>
-      <c r="J8" s="100"/>
-      <c r="K8" s="101"/>
-      <c r="L8" s="102"/>
-      <c r="M8" s="103"/>
-      <c r="N8" s="98"/>
-      <c r="O8" s="99"/>
-      <c r="P8" s="100"/>
-      <c r="Q8" s="101"/>
-      <c r="R8" s="102"/>
-      <c r="S8" s="103"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="97"/>
-      <c r="B9" s="98"/>
-      <c r="C9" s="99"/>
-      <c r="D9" s="100"/>
-      <c r="E9" s="106"/>
-      <c r="F9" s="107"/>
-      <c r="G9" s="108"/>
-      <c r="H9" s="98"/>
-      <c r="I9" s="99"/>
-      <c r="J9" s="100"/>
-      <c r="K9" s="106"/>
-      <c r="L9" s="107"/>
-      <c r="M9" s="108"/>
-      <c r="N9" s="98"/>
-      <c r="O9" s="99"/>
-      <c r="P9" s="100"/>
-      <c r="Q9" s="101"/>
-      <c r="R9" s="102"/>
-      <c r="S9" s="103"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="112"/>
-      <c r="C10" s="113"/>
-      <c r="D10" s="114"/>
-      <c r="E10" s="112"/>
-      <c r="F10" s="113"/>
-      <c r="G10" s="114"/>
-      <c r="H10" s="112"/>
-      <c r="I10" s="113"/>
-      <c r="J10" s="114"/>
-      <c r="K10" s="112"/>
-      <c r="L10" s="113"/>
-      <c r="M10" s="114"/>
-      <c r="N10" s="112"/>
-      <c r="O10" s="113"/>
-      <c r="P10" s="114"/>
-      <c r="Q10" s="112"/>
-      <c r="R10" s="113"/>
-      <c r="S10" s="114"/>
-    </row>
-    <row r="11" spans="1:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="109"/>
-      <c r="C11" s="110"/>
-      <c r="D11" s="111"/>
-      <c r="E11" s="109"/>
-      <c r="F11" s="110"/>
-      <c r="G11" s="111"/>
-      <c r="H11" s="109"/>
-      <c r="I11" s="110"/>
-      <c r="J11" s="111"/>
-      <c r="K11" s="109"/>
-      <c r="L11" s="110"/>
-      <c r="M11" s="111"/>
-      <c r="N11" s="109"/>
-      <c r="O11" s="110"/>
-      <c r="P11" s="111"/>
-      <c r="Q11" s="109"/>
-      <c r="R11" s="110"/>
-      <c r="S11" s="111"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="104" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="92" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="93"/>
-      <c r="D13" s="94"/>
-      <c r="E13" s="92" t="s">
-        <v>3</v>
-      </c>
-      <c r="F13" s="93"/>
-      <c r="G13" s="94"/>
-      <c r="H13" s="92" t="s">
-        <v>3</v>
-      </c>
-      <c r="I13" s="93"/>
-      <c r="J13" s="94"/>
-      <c r="K13" s="92" t="s">
-        <v>3</v>
-      </c>
-      <c r="L13" s="93"/>
-      <c r="M13" s="94"/>
-      <c r="N13" s="92" t="s">
-        <v>3</v>
-      </c>
-      <c r="O13" s="93"/>
-      <c r="P13" s="94"/>
-      <c r="Q13" s="92" t="s">
-        <v>6</v>
-      </c>
-      <c r="R13" s="93"/>
-      <c r="S13" s="94"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="105"/>
-      <c r="B14" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="I14" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="J14" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="K14" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="L14" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="M14" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="N14" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="O14" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="P14" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q14" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="R14" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="S14" s="13" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="1">
-        <v>20000</v>
-      </c>
-      <c r="C15" s="2">
-        <f>B15/($U$1*$U$2)</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="D15" s="3">
-        <f>C15*1000</f>
-        <v>333.33333333333331</v>
-      </c>
-      <c r="E15" s="1">
-        <v>50000</v>
-      </c>
-      <c r="F15" s="2">
-        <f>E15/($U$1*$U$2)</f>
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="G15" s="3">
-        <f>F15*1000</f>
-        <v>833.33333333333337</v>
-      </c>
-      <c r="H15" s="1">
-        <v>100000</v>
-      </c>
-      <c r="I15" s="2">
-        <f>H15/($U$1*$U$2)</f>
-        <v>1.6666666666666667</v>
-      </c>
-      <c r="J15" s="3">
-        <f>I15*1000</f>
-        <v>1666.6666666666667</v>
-      </c>
-      <c r="K15" s="1">
-        <v>150000</v>
-      </c>
-      <c r="L15" s="2">
-        <f>K15/($U$1*$U$2)</f>
-        <v>2.5</v>
-      </c>
-      <c r="M15" s="3">
-        <f>L15*1000</f>
-        <v>2500</v>
-      </c>
-      <c r="N15" s="1">
-        <v>200000</v>
-      </c>
-      <c r="O15" s="2">
-        <f>N15/($U$1*$U$2)</f>
-        <v>3.3333333333333335</v>
-      </c>
-      <c r="P15" s="3">
-        <f>O15*1000</f>
-        <v>3333.3333333333335</v>
-      </c>
-      <c r="Q15" s="1">
-        <v>278744</v>
-      </c>
-      <c r="R15" s="2">
-        <f>Q15/($U$1*$U$2)</f>
-        <v>4.6457333333333333</v>
-      </c>
-      <c r="S15" s="3">
-        <f>R15*1000</f>
-        <v>4645.7333333333336</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="95" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="98"/>
-      <c r="C16" s="99"/>
-      <c r="D16" s="100"/>
-      <c r="E16" s="101"/>
-      <c r="F16" s="102"/>
-      <c r="G16" s="103"/>
-      <c r="H16" s="98"/>
-      <c r="I16" s="99"/>
-      <c r="J16" s="100"/>
-      <c r="K16" s="101"/>
-      <c r="L16" s="102"/>
-      <c r="M16" s="103"/>
-      <c r="N16" s="98"/>
-      <c r="O16" s="99"/>
-      <c r="P16" s="100"/>
-      <c r="Q16" s="101"/>
-      <c r="R16" s="102"/>
-      <c r="S16" s="103"/>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="96"/>
-      <c r="B17" s="98"/>
-      <c r="C17" s="99"/>
-      <c r="D17" s="100"/>
-      <c r="E17" s="101"/>
-      <c r="F17" s="102"/>
-      <c r="G17" s="103"/>
-      <c r="H17" s="98"/>
-      <c r="I17" s="99"/>
-      <c r="J17" s="100"/>
-      <c r="K17" s="101"/>
-      <c r="L17" s="102"/>
-      <c r="M17" s="103"/>
-      <c r="N17" s="98"/>
-      <c r="O17" s="99"/>
-      <c r="P17" s="100"/>
-      <c r="Q17" s="98"/>
-      <c r="R17" s="99"/>
-      <c r="S17" s="100"/>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="96"/>
-      <c r="B18" s="98"/>
-      <c r="C18" s="99"/>
-      <c r="D18" s="100"/>
-      <c r="E18" s="101"/>
-      <c r="F18" s="102"/>
-      <c r="G18" s="103"/>
-      <c r="H18" s="98"/>
-      <c r="I18" s="99"/>
-      <c r="J18" s="100"/>
-      <c r="K18" s="101"/>
-      <c r="L18" s="102"/>
-      <c r="M18" s="103"/>
-      <c r="N18" s="98"/>
-      <c r="O18" s="99"/>
-      <c r="P18" s="100"/>
-      <c r="Q18" s="101"/>
-      <c r="R18" s="102"/>
-      <c r="S18" s="103"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="96"/>
-      <c r="B19" s="98"/>
-      <c r="C19" s="99"/>
-      <c r="D19" s="100"/>
-      <c r="E19" s="101"/>
-      <c r="F19" s="102"/>
-      <c r="G19" s="103"/>
-      <c r="H19" s="98"/>
-      <c r="I19" s="99"/>
-      <c r="J19" s="100"/>
-      <c r="K19" s="101"/>
-      <c r="L19" s="102"/>
-      <c r="M19" s="103"/>
-      <c r="N19" s="98"/>
-      <c r="O19" s="99"/>
-      <c r="P19" s="100"/>
-      <c r="Q19" s="98"/>
-      <c r="R19" s="99"/>
-      <c r="S19" s="100"/>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="96"/>
-      <c r="B20" s="98"/>
-      <c r="C20" s="99"/>
-      <c r="D20" s="100"/>
-      <c r="E20" s="101"/>
-      <c r="F20" s="102"/>
-      <c r="G20" s="103"/>
-      <c r="H20" s="98"/>
-      <c r="I20" s="99"/>
-      <c r="J20" s="100"/>
-      <c r="K20" s="101"/>
-      <c r="L20" s="102"/>
-      <c r="M20" s="103"/>
-      <c r="N20" s="98"/>
-      <c r="O20" s="99"/>
-      <c r="P20" s="100"/>
-      <c r="Q20" s="101"/>
-      <c r="R20" s="102"/>
-      <c r="S20" s="103"/>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="97"/>
-      <c r="B21" s="98"/>
-      <c r="C21" s="99"/>
-      <c r="D21" s="100"/>
-      <c r="E21" s="106"/>
-      <c r="F21" s="107"/>
-      <c r="G21" s="108"/>
-      <c r="H21" s="98"/>
-      <c r="I21" s="99"/>
-      <c r="J21" s="100"/>
-      <c r="K21" s="106"/>
-      <c r="L21" s="107"/>
-      <c r="M21" s="108"/>
-      <c r="N21" s="98"/>
-      <c r="O21" s="99"/>
-      <c r="P21" s="100"/>
-      <c r="Q21" s="101"/>
-      <c r="R21" s="102"/>
-      <c r="S21" s="103"/>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="112"/>
-      <c r="C22" s="113"/>
-      <c r="D22" s="114"/>
-      <c r="E22" s="112"/>
-      <c r="F22" s="113"/>
-      <c r="G22" s="114"/>
-      <c r="H22" s="112"/>
-      <c r="I22" s="113"/>
-      <c r="J22" s="114"/>
-      <c r="K22" s="112"/>
-      <c r="L22" s="113"/>
-      <c r="M22" s="114"/>
-      <c r="N22" s="112"/>
-      <c r="O22" s="113"/>
-      <c r="P22" s="114"/>
-      <c r="Q22" s="112"/>
-      <c r="R22" s="113"/>
-      <c r="S22" s="114"/>
-    </row>
-    <row r="23" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" s="109"/>
-      <c r="C23" s="110"/>
-      <c r="D23" s="111"/>
-      <c r="E23" s="109"/>
-      <c r="F23" s="110"/>
-      <c r="G23" s="111"/>
-      <c r="H23" s="109"/>
-      <c r="I23" s="110"/>
-      <c r="J23" s="111"/>
-      <c r="K23" s="115"/>
-      <c r="L23" s="116"/>
-      <c r="M23" s="117"/>
-      <c r="N23" s="109"/>
-      <c r="O23" s="110"/>
-      <c r="P23" s="111"/>
-      <c r="Q23" s="115"/>
-      <c r="R23" s="116"/>
-      <c r="S23" s="117"/>
-    </row>
-  </sheetData>
-  <mergeCells count="112">
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="N23:P23"/>
-    <mergeCell ref="Q23:S23"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="H22:J22"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="N22:P22"/>
-    <mergeCell ref="Q22:S22"/>
-    <mergeCell ref="N17:P17"/>
-    <mergeCell ref="Q17:S17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="N18:P18"/>
-    <mergeCell ref="Q18:S18"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="N21:P21"/>
-    <mergeCell ref="Q21:S21"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="N20:P20"/>
-    <mergeCell ref="Q20:S20"/>
-    <mergeCell ref="Q13:S13"/>
-    <mergeCell ref="A16:A21"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="N16:P16"/>
-    <mergeCell ref="Q16:S16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="N13:P13"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="N19:P19"/>
-    <mergeCell ref="Q19:S19"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="N11:P11"/>
-    <mergeCell ref="Q11:S11"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="N10:P10"/>
-    <mergeCell ref="Q10:S10"/>
-    <mergeCell ref="N5:P5"/>
-    <mergeCell ref="Q5:S5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="Q6:S6"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="N9:P9"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="N8:P8"/>
-    <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="Q4:S4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:M5"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V44"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4153,7 +3492,7 @@
     <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
@@ -4168,26 +3507,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="116" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="118" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C1" s="119"/>
       <c r="D1" s="120"/>
       <c r="E1" s="118" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F1" s="119"/>
       <c r="G1" s="120"/>
       <c r="H1" s="118" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I1" s="119"/>
       <c r="J1" s="120"/>
       <c r="K1" s="118" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L1" s="119"/>
       <c r="M1" s="120"/>
@@ -4207,7 +3546,7 @@
         <v>60</v>
       </c>
       <c r="S1" s="65" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="T1" s="65" t="s">
         <v>63</v>
@@ -4216,11 +3555,11 @@
         <v>62</v>
       </c>
       <c r="V1" s="65" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="105"/>
+      <c r="A2" s="117"/>
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
@@ -4267,7 +3606,7 @@
         <v>11</v>
       </c>
       <c r="S2" s="65" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="T2" s="65" t="s">
         <v>60</v>
@@ -4329,7 +3668,7 @@
         <v>250</v>
       </c>
       <c r="S3" s="65" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="T3" s="65" t="s">
         <v>60</v>
@@ -4339,210 +3678,210 @@
         <v>3.0683333333333335E-3</v>
       </c>
       <c r="V3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="95" t="s">
+      <c r="A4" s="113" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="98">
+      <c r="B4" s="103">
         <f>36.2/7.05</f>
         <v>5.1347517730496461</v>
       </c>
-      <c r="C4" s="99"/>
-      <c r="D4" s="100"/>
-      <c r="E4" s="98">
+      <c r="C4" s="104"/>
+      <c r="D4" s="105"/>
+      <c r="E4" s="103">
         <f>39/1.16</f>
         <v>33.620689655172413</v>
       </c>
-      <c r="F4" s="99"/>
-      <c r="G4" s="100"/>
-      <c r="H4" s="98">
+      <c r="F4" s="104"/>
+      <c r="G4" s="105"/>
+      <c r="H4" s="103">
         <f>195/1.09</f>
         <v>178.89908256880733</v>
       </c>
-      <c r="I4" s="99"/>
-      <c r="J4" s="100"/>
-      <c r="K4" s="101"/>
-      <c r="L4" s="102"/>
-      <c r="M4" s="103"/>
+      <c r="I4" s="104"/>
+      <c r="J4" s="105"/>
+      <c r="K4" s="106"/>
+      <c r="L4" s="107"/>
+      <c r="M4" s="108"/>
       <c r="N4" s="63" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O4" s="63" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="P4" s="73" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q4" s="73" t="s">
         <v>86</v>
       </c>
-      <c r="Q4" s="73" t="s">
-        <v>87</v>
-      </c>
       <c r="R4" s="72"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="96"/>
-      <c r="B5" s="98">
+      <c r="A5" s="114"/>
+      <c r="B5" s="103">
         <f>37.9/7.11</f>
         <v>5.3305203938115326</v>
       </c>
-      <c r="C5" s="99"/>
-      <c r="D5" s="100"/>
-      <c r="E5" s="98">
+      <c r="C5" s="104"/>
+      <c r="D5" s="105"/>
+      <c r="E5" s="103">
         <f>38.6/1.17</f>
         <v>32.991452991452995</v>
       </c>
-      <c r="F5" s="99"/>
-      <c r="G5" s="100"/>
-      <c r="H5" s="98">
+      <c r="F5" s="104"/>
+      <c r="G5" s="105"/>
+      <c r="H5" s="103">
         <f>194/1.11</f>
         <v>174.77477477477476</v>
       </c>
-      <c r="I5" s="99"/>
-      <c r="J5" s="100"/>
-      <c r="K5" s="98"/>
-      <c r="L5" s="99"/>
-      <c r="M5" s="100"/>
+      <c r="I5" s="104"/>
+      <c r="J5" s="105"/>
+      <c r="K5" s="103"/>
+      <c r="L5" s="104"/>
+      <c r="M5" s="105"/>
       <c r="N5">
         <f>'Flow Rate'!C16</f>
         <v>21610</v>
       </c>
       <c r="P5" s="65" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q5" s="65" t="s">
         <v>89</v>
       </c>
-      <c r="Q5" s="65" t="s">
-        <v>90</v>
-      </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="96"/>
-      <c r="B6" s="98">
+      <c r="A6" s="114"/>
+      <c r="B6" s="103">
         <f>37/7.03</f>
         <v>5.2631578947368416</v>
       </c>
-      <c r="C6" s="99"/>
-      <c r="D6" s="100"/>
-      <c r="E6" s="98">
+      <c r="C6" s="104"/>
+      <c r="D6" s="105"/>
+      <c r="E6" s="103">
         <f>38.2/1.16</f>
         <v>32.931034482758626</v>
       </c>
-      <c r="F6" s="99"/>
-      <c r="G6" s="100"/>
-      <c r="H6" s="98">
+      <c r="F6" s="104"/>
+      <c r="G6" s="105"/>
+      <c r="H6" s="103">
         <f>194.3/1.1</f>
         <v>176.63636363636363</v>
       </c>
-      <c r="I6" s="99"/>
-      <c r="J6" s="100"/>
-      <c r="K6" s="101"/>
-      <c r="L6" s="102"/>
-      <c r="M6" s="103"/>
+      <c r="I6" s="104"/>
+      <c r="J6" s="105"/>
+      <c r="K6" s="106"/>
+      <c r="L6" s="107"/>
+      <c r="M6" s="108"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="96"/>
-      <c r="B7" s="98">
+      <c r="A7" s="114"/>
+      <c r="B7" s="103">
         <f>36/6.48</f>
         <v>5.5555555555555554</v>
       </c>
-      <c r="C7" s="99"/>
-      <c r="D7" s="100"/>
-      <c r="E7" s="98">
+      <c r="C7" s="104"/>
+      <c r="D7" s="105"/>
+      <c r="E7" s="103">
         <f>38/1.15</f>
         <v>33.04347826086957</v>
       </c>
-      <c r="F7" s="99"/>
-      <c r="G7" s="100"/>
-      <c r="H7" s="98">
+      <c r="F7" s="104"/>
+      <c r="G7" s="105"/>
+      <c r="H7" s="103">
         <f>192.4/1.08</f>
         <v>178.14814814814815</v>
       </c>
-      <c r="I7" s="99"/>
-      <c r="J7" s="100"/>
-      <c r="K7" s="98"/>
-      <c r="L7" s="99"/>
-      <c r="M7" s="100"/>
+      <c r="I7" s="104"/>
+      <c r="J7" s="105"/>
+      <c r="K7" s="103"/>
+      <c r="L7" s="104"/>
+      <c r="M7" s="105"/>
       <c r="O7" s="63" t="s">
-        <v>95</v>
-      </c>
-      <c r="P7" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q7" s="107"/>
+        <v>94</v>
+      </c>
+      <c r="P7" s="109" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q7" s="109"/>
       <c r="R7" s="65" t="s">
         <v>60</v>
       </c>
-      <c r="S7" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="T7" s="107"/>
+      <c r="S7" s="109" t="s">
+        <v>97</v>
+      </c>
+      <c r="T7" s="109"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="96"/>
-      <c r="B8" s="98">
+      <c r="A8" s="114"/>
+      <c r="B8" s="103">
         <f>32.8/6.39</f>
         <v>5.1330203442879494</v>
       </c>
-      <c r="C8" s="99"/>
-      <c r="D8" s="100"/>
-      <c r="E8" s="98">
+      <c r="C8" s="104"/>
+      <c r="D8" s="105"/>
+      <c r="E8" s="103">
         <f>38.1/1.14</f>
         <v>33.421052631578952</v>
       </c>
-      <c r="F8" s="99"/>
-      <c r="G8" s="100"/>
-      <c r="H8" s="98">
+      <c r="F8" s="104"/>
+      <c r="G8" s="105"/>
+      <c r="H8" s="103">
         <f>191.8/1.09</f>
         <v>175.96330275229357</v>
       </c>
-      <c r="I8" s="99"/>
-      <c r="J8" s="100"/>
-      <c r="K8" s="101"/>
-      <c r="L8" s="102"/>
-      <c r="M8" s="103"/>
+      <c r="I8" s="104"/>
+      <c r="J8" s="105"/>
+      <c r="K8" s="106"/>
+      <c r="L8" s="107"/>
+      <c r="M8" s="108"/>
       <c r="P8" s="65" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q8" s="65" t="s">
         <v>96</v>
       </c>
-      <c r="Q8" s="65" t="s">
-        <v>97</v>
-      </c>
       <c r="S8" s="77" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="T8" s="77" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="97"/>
-      <c r="B9" s="98">
+      <c r="A9" s="115"/>
+      <c r="B9" s="103">
         <f>35.5/7.25</f>
         <v>4.8965517241379306</v>
       </c>
-      <c r="C9" s="99"/>
-      <c r="D9" s="100"/>
-      <c r="E9" s="98">
+      <c r="C9" s="104"/>
+      <c r="D9" s="105"/>
+      <c r="E9" s="103">
         <f>37.8/1.12</f>
         <v>33.749999999999993</v>
       </c>
-      <c r="F9" s="99"/>
-      <c r="G9" s="100"/>
-      <c r="H9" s="98">
+      <c r="F9" s="104"/>
+      <c r="G9" s="105"/>
+      <c r="H9" s="103">
         <f>191.7/1.1</f>
         <v>174.27272727272725</v>
       </c>
-      <c r="I9" s="99"/>
-      <c r="J9" s="100"/>
-      <c r="K9" s="101"/>
-      <c r="L9" s="102"/>
-      <c r="M9" s="103"/>
+      <c r="I9" s="104"/>
+      <c r="J9" s="105"/>
+      <c r="K9" s="106"/>
+      <c r="L9" s="107"/>
+      <c r="M9" s="108"/>
       <c r="O9" s="63" t="s">
+        <v>100</v>
+      </c>
+      <c r="P9" s="109" t="s">
         <v>101</v>
       </c>
-      <c r="P9" s="107" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q9" s="107"/>
+      <c r="Q9" s="109"/>
       <c r="R9" t="s">
         <v>60</v>
       </c>
@@ -4551,89 +3890,89 @@
         <v>3000</v>
       </c>
       <c r="U9" s="80" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="V9" s="81"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="112" t="s">
+      <c r="B10" s="100" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="113"/>
-      <c r="D10" s="114"/>
-      <c r="E10" s="112" t="s">
+      <c r="C10" s="101"/>
+      <c r="D10" s="102"/>
+      <c r="E10" s="100" t="s">
         <v>67</v>
       </c>
-      <c r="F10" s="113"/>
-      <c r="G10" s="114"/>
-      <c r="H10" s="112" t="s">
+      <c r="F10" s="101"/>
+      <c r="G10" s="102"/>
+      <c r="H10" s="100" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="113"/>
-      <c r="J10" s="114"/>
-      <c r="K10" s="112" t="s">
+      <c r="I10" s="101"/>
+      <c r="J10" s="102"/>
+      <c r="K10" s="100" t="s">
         <v>76</v>
       </c>
-      <c r="L10" s="113"/>
-      <c r="M10" s="114"/>
+      <c r="L10" s="101"/>
+      <c r="M10" s="102"/>
       <c r="P10" s="65" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q10" s="65" t="s">
         <v>103</v>
-      </c>
-      <c r="Q10" s="65" t="s">
-        <v>104</v>
       </c>
       <c r="S10" s="78">
         <f>U3</f>
         <v>3.0683333333333335E-3</v>
       </c>
       <c r="T10" s="61" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="U10">
         <f>N5</f>
         <v>21610</v>
       </c>
       <c r="V10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" ht="30" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="30.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="109">
+      <c r="B11" s="94">
         <f>(336.12*1000)/($O$1*$O$2)</f>
         <v>5.6020000000000003</v>
       </c>
-      <c r="C11" s="110"/>
-      <c r="D11" s="111"/>
-      <c r="E11" s="109">
+      <c r="C11" s="95"/>
+      <c r="D11" s="96"/>
+      <c r="E11" s="94">
         <f>(1995.71*1000)/($O$1*$O$2)</f>
         <v>33.261833333333335</v>
       </c>
-      <c r="F11" s="110"/>
-      <c r="G11" s="111"/>
-      <c r="H11" s="109">
+      <c r="F11" s="95"/>
+      <c r="G11" s="96"/>
+      <c r="H11" s="94">
         <f>(9999.6*1000)/($O$1*$O$2)</f>
         <v>166.66</v>
       </c>
-      <c r="I11" s="110"/>
-      <c r="J11" s="111"/>
-      <c r="K11" s="109"/>
-      <c r="L11" s="110"/>
-      <c r="M11" s="111"/>
-      <c r="O11" s="63" t="s">
-        <v>101</v>
-      </c>
-      <c r="P11" s="55">
+      <c r="I11" s="95"/>
+      <c r="J11" s="96"/>
+      <c r="K11" s="94"/>
+      <c r="L11" s="95"/>
+      <c r="M11" s="96"/>
+      <c r="O11" s="121" t="s">
+        <v>100</v>
+      </c>
+      <c r="P11" s="122">
         <f>T9/(S10*U10)*1000</f>
         <v>45244.307951863069</v>
       </c>
-      <c r="Q11" t="s">
-        <v>107</v>
+      <c r="Q11" s="60" t="s">
+        <v>106</v>
       </c>
       <c r="S11" s="61"/>
       <c r="T11" s="61"/>
@@ -4643,34 +3982,34 @@
       <c r="T12" s="61"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="104" t="s">
+      <c r="A13" s="116" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="118" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C13" s="119"/>
       <c r="D13" s="120"/>
       <c r="E13" s="118" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F13" s="119"/>
       <c r="G13" s="120"/>
       <c r="H13" s="118" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I13" s="119"/>
       <c r="J13" s="120"/>
-      <c r="K13" s="92" t="s">
-        <v>94</v>
-      </c>
-      <c r="L13" s="93"/>
-      <c r="M13" s="94"/>
+      <c r="K13" s="110" t="s">
+        <v>93</v>
+      </c>
+      <c r="L13" s="111"/>
+      <c r="M13" s="112"/>
       <c r="S13" s="61"/>
       <c r="T13" s="61"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="105"/>
+      <c r="A14" s="117"/>
       <c r="B14" s="7" t="s">
         <v>0</v>
       </c>
@@ -4758,201 +4097,201 @@
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="95" t="s">
+      <c r="A16" s="113" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="98">
+      <c r="B16" s="103">
         <f>407.7/1.1</f>
         <v>370.63636363636357</v>
       </c>
-      <c r="C16" s="99"/>
-      <c r="D16" s="100"/>
-      <c r="E16" s="98">
+      <c r="C16" s="104"/>
+      <c r="D16" s="105"/>
+      <c r="E16" s="103">
         <f>1804.7/1.03</f>
         <v>1752.1359223300972</v>
       </c>
-      <c r="F16" s="99"/>
-      <c r="G16" s="100"/>
-      <c r="H16" s="98">
+      <c r="F16" s="104"/>
+      <c r="G16" s="105"/>
+      <c r="H16" s="103">
         <f>1796.1/(31/60)</f>
         <v>3476.3225806451605</v>
       </c>
-      <c r="I16" s="99"/>
-      <c r="J16" s="100"/>
-      <c r="K16" s="101"/>
-      <c r="L16" s="102"/>
-      <c r="M16" s="103"/>
+      <c r="I16" s="104"/>
+      <c r="J16" s="105"/>
+      <c r="K16" s="106"/>
+      <c r="L16" s="107"/>
+      <c r="M16" s="108"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="96"/>
-      <c r="B17" s="98">
+      <c r="A17" s="114"/>
+      <c r="B17" s="103">
         <f>401.3/1.09</f>
         <v>368.16513761467888</v>
       </c>
-      <c r="C17" s="99"/>
-      <c r="D17" s="100"/>
-      <c r="E17" s="98">
+      <c r="C17" s="104"/>
+      <c r="D17" s="105"/>
+      <c r="E17" s="103">
         <f>1744/1.01</f>
         <v>1726.7326732673266</v>
       </c>
-      <c r="F17" s="99"/>
-      <c r="G17" s="100"/>
-      <c r="H17" s="98">
+      <c r="F17" s="104"/>
+      <c r="G17" s="105"/>
+      <c r="H17" s="103">
         <f>1690.7/(29/60)</f>
         <v>3498</v>
       </c>
-      <c r="I17" s="99"/>
-      <c r="J17" s="100"/>
-      <c r="K17" s="98"/>
-      <c r="L17" s="99"/>
-      <c r="M17" s="100"/>
+      <c r="I17" s="104"/>
+      <c r="J17" s="105"/>
+      <c r="K17" s="103"/>
+      <c r="L17" s="104"/>
+      <c r="M17" s="105"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="96"/>
-      <c r="B18" s="98">
+      <c r="A18" s="114"/>
+      <c r="B18" s="103">
         <f>413.2/1.12</f>
         <v>368.92857142857139</v>
       </c>
-      <c r="C18" s="99"/>
-      <c r="D18" s="100"/>
-      <c r="E18" s="98">
+      <c r="C18" s="104"/>
+      <c r="D18" s="105"/>
+      <c r="E18" s="103">
         <f>1786/1.02</f>
         <v>1750.9803921568628</v>
       </c>
-      <c r="F18" s="99"/>
-      <c r="G18" s="100"/>
-      <c r="H18" s="98">
+      <c r="F18" s="104"/>
+      <c r="G18" s="105"/>
+      <c r="H18" s="103">
         <f>1838/(31/60)</f>
         <v>3557.4193548387093</v>
       </c>
-      <c r="I18" s="99"/>
-      <c r="J18" s="100"/>
-      <c r="K18" s="101"/>
-      <c r="L18" s="102"/>
-      <c r="M18" s="103"/>
+      <c r="I18" s="104"/>
+      <c r="J18" s="105"/>
+      <c r="K18" s="106"/>
+      <c r="L18" s="107"/>
+      <c r="M18" s="108"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="96"/>
-      <c r="B19" s="98">
+      <c r="A19" s="114"/>
+      <c r="B19" s="103">
         <f>406.3/1.11</f>
         <v>366.03603603603602</v>
       </c>
-      <c r="C19" s="99"/>
-      <c r="D19" s="100"/>
-      <c r="E19" s="98">
+      <c r="C19" s="104"/>
+      <c r="D19" s="105"/>
+      <c r="E19" s="103">
         <f>1801.7/1.02</f>
         <v>1766.372549019608</v>
       </c>
-      <c r="F19" s="99"/>
-      <c r="G19" s="100"/>
-      <c r="H19" s="98">
+      <c r="F19" s="104"/>
+      <c r="G19" s="105"/>
+      <c r="H19" s="103">
         <f>1751/(30/60)</f>
         <v>3502</v>
       </c>
-      <c r="I19" s="99"/>
-      <c r="J19" s="100"/>
-      <c r="K19" s="98"/>
-      <c r="L19" s="99"/>
-      <c r="M19" s="100"/>
+      <c r="I19" s="104"/>
+      <c r="J19" s="105"/>
+      <c r="K19" s="103"/>
+      <c r="L19" s="104"/>
+      <c r="M19" s="105"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="96"/>
-      <c r="B20" s="98">
+      <c r="A20" s="114"/>
+      <c r="B20" s="103">
         <f>419.5/1.14</f>
         <v>367.98245614035091</v>
       </c>
-      <c r="C20" s="99"/>
-      <c r="D20" s="100"/>
-      <c r="E20" s="98">
+      <c r="C20" s="104"/>
+      <c r="D20" s="105"/>
+      <c r="E20" s="103">
         <f>1738.2/1</f>
         <v>1738.2</v>
       </c>
-      <c r="F20" s="99"/>
-      <c r="G20" s="100"/>
-      <c r="H20" s="98">
+      <c r="F20" s="104"/>
+      <c r="G20" s="105"/>
+      <c r="H20" s="103">
         <f>1933.9/(33/60)</f>
         <v>3516.181818181818</v>
       </c>
-      <c r="I20" s="99"/>
-      <c r="J20" s="100"/>
-      <c r="K20" s="101"/>
-      <c r="L20" s="102"/>
-      <c r="M20" s="103"/>
+      <c r="I20" s="104"/>
+      <c r="J20" s="105"/>
+      <c r="K20" s="106"/>
+      <c r="L20" s="107"/>
+      <c r="M20" s="108"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="97"/>
-      <c r="B21" s="98">
+      <c r="A21" s="115"/>
+      <c r="B21" s="103">
         <f>405.1/1.13</f>
         <v>358.49557522123899</v>
       </c>
-      <c r="C21" s="99"/>
-      <c r="D21" s="100"/>
-      <c r="E21" s="98">
+      <c r="C21" s="104"/>
+      <c r="D21" s="105"/>
+      <c r="E21" s="103">
         <f>1734.7/1</f>
         <v>1734.7</v>
       </c>
-      <c r="F21" s="99"/>
-      <c r="G21" s="100"/>
-      <c r="H21" s="98">
+      <c r="F21" s="104"/>
+      <c r="G21" s="105"/>
+      <c r="H21" s="103">
         <f>1697.8/(29/60)</f>
         <v>3512.6896551724135</v>
       </c>
-      <c r="I21" s="99"/>
-      <c r="J21" s="100"/>
-      <c r="K21" s="101"/>
-      <c r="L21" s="102"/>
-      <c r="M21" s="103"/>
+      <c r="I21" s="104"/>
+      <c r="J21" s="105"/>
+      <c r="K21" s="106"/>
+      <c r="L21" s="107"/>
+      <c r="M21" s="108"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="112" t="s">
+      <c r="B22" s="100" t="s">
         <v>73</v>
       </c>
-      <c r="C22" s="113"/>
-      <c r="D22" s="114"/>
-      <c r="E22" s="112" t="s">
+      <c r="C22" s="101"/>
+      <c r="D22" s="102"/>
+      <c r="E22" s="100" t="s">
         <v>74</v>
       </c>
-      <c r="F22" s="113"/>
-      <c r="G22" s="114"/>
-      <c r="H22" s="112" t="s">
+      <c r="F22" s="101"/>
+      <c r="G22" s="102"/>
+      <c r="H22" s="100" t="s">
         <v>75</v>
       </c>
-      <c r="I22" s="113"/>
-      <c r="J22" s="114"/>
-      <c r="K22" s="112" t="s">
+      <c r="I22" s="101"/>
+      <c r="J22" s="102"/>
+      <c r="K22" s="100" t="s">
         <v>66</v>
       </c>
-      <c r="L22" s="113"/>
-      <c r="M22" s="114"/>
+      <c r="L22" s="101"/>
+      <c r="M22" s="102"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="109">
+      <c r="B23" s="94">
         <f>(19999.15*1000)/($O$1*$O$2)</f>
         <v>333.31916666666666</v>
       </c>
-      <c r="C23" s="110"/>
-      <c r="D23" s="111"/>
-      <c r="E23" s="109">
+      <c r="C23" s="95"/>
+      <c r="D23" s="96"/>
+      <c r="E23" s="94">
         <f>(99995.75*1000)/($O$1*$O$2)</f>
         <v>1666.5958333333333</v>
       </c>
-      <c r="F23" s="110"/>
-      <c r="G23" s="111"/>
-      <c r="H23" s="109">
+      <c r="F23" s="95"/>
+      <c r="G23" s="96"/>
+      <c r="H23" s="94">
         <f>1*(199991.48*1000)/($O$1*$O$2)</f>
         <v>3333.1913333333332</v>
       </c>
-      <c r="I23" s="110"/>
-      <c r="J23" s="111"/>
-      <c r="K23" s="115"/>
-      <c r="L23" s="116"/>
-      <c r="M23" s="117"/>
+      <c r="I23" s="95"/>
+      <c r="J23" s="96"/>
+      <c r="K23" s="97"/>
+      <c r="L23" s="98"/>
+      <c r="M23" s="99"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="22"/>
@@ -4983,10 +4322,10 @@
         <v>78</v>
       </c>
       <c r="N25" s="68" t="s">
+        <v>83</v>
+      </c>
+      <c r="O25" s="68" t="s">
         <v>84</v>
-      </c>
-      <c r="O25" s="68" t="s">
-        <v>85</v>
       </c>
       <c r="P25" s="66" t="s">
         <v>65</v>
@@ -5011,7 +4350,7 @@
         <v>32</v>
       </c>
       <c r="J26" s="61">
-        <f t="shared" ref="J26:J31" si="1">I26*$D$34+$G$34</f>
+        <f>I26*$D$34+$G$34</f>
         <v>6.2972099999999998</v>
       </c>
       <c r="N26">
@@ -5037,14 +4376,14 @@
         <v>33.658498786127176</v>
       </c>
       <c r="E27" s="70">
-        <f t="shared" ref="E27:E33" si="2">(B27-D27)/B27</f>
+        <f t="shared" ref="E27:E33" si="1">(B27-D27)/B27</f>
         <v>-9.754963583815196E-3</v>
       </c>
       <c r="I27">
         <v>190</v>
       </c>
       <c r="J27" s="61">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="J26:J31" si="2">I27*$D$34+$G$34</f>
         <v>35.667830000000002</v>
       </c>
       <c r="N27">
@@ -5070,14 +4409,14 @@
         <v>166.89757393063584</v>
       </c>
       <c r="E28" s="70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-1.3854435838151177E-3</v>
       </c>
       <c r="I28">
         <v>952</v>
       </c>
       <c r="J28" s="61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>177.31600999999998</v>
       </c>
       <c r="N28">
@@ -5103,14 +4442,14 @@
         <v>250.17199589595378</v>
       </c>
       <c r="E29" s="70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-6.8798358381513933E-4</v>
       </c>
       <c r="I29">
         <v>1904</v>
       </c>
       <c r="J29" s="61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>354.28328999999997</v>
       </c>
       <c r="N29">
@@ -5136,14 +4475,14 @@
         <v>333.4464178612717</v>
       </c>
       <c r="E30" s="70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-3.3925358381515028E-4</v>
       </c>
       <c r="I30">
         <v>9520</v>
       </c>
       <c r="J30" s="61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1770.02153</v>
       </c>
       <c r="N30">
@@ -5169,14 +4508,14 @@
         <v>1665.8371693063586</v>
       </c>
       <c r="E31" s="70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4.9769841618485771E-4</v>
       </c>
       <c r="I31">
         <v>19040</v>
       </c>
       <c r="J31" s="61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3539.6943300000003</v>
       </c>
       <c r="N31">
@@ -5202,7 +4541,7 @@
         <v>3331.3256086127176</v>
       </c>
       <c r="E32" s="70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>6.0231741618476916E-4</v>
       </c>
     </row>
@@ -5218,26 +4557,26 @@
         <v>4647.5987299999997</v>
       </c>
       <c r="E33" s="70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-4.0152900152099321E-4</v>
       </c>
+      <c r="H33" s="65" t="s">
+        <v>59</v>
+      </c>
       <c r="I33" s="65" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J33" s="65" t="s">
-        <v>60</v>
+        <v>98</v>
       </c>
       <c r="K33" s="65" t="s">
+        <v>63</v>
+      </c>
+      <c r="L33" s="65" t="s">
+        <v>62</v>
+      </c>
+      <c r="M33" s="65" t="s">
         <v>99</v>
-      </c>
-      <c r="L33" s="65" t="s">
-        <v>63</v>
-      </c>
-      <c r="M33" s="65" t="s">
-        <v>62</v>
-      </c>
-      <c r="N33" s="65" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5376,7 +4715,7 @@
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="J43" s="61">
+      <c r="J43" s="55">
         <f>SUM(J37:J42)/6</f>
         <v>2983.8839178247072</v>
       </c>
@@ -5385,38 +4724,111 @@
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="J44" s="61">
+      <c r="J44" s="55">
         <f>(J36-J43)/J36*100</f>
         <v>0.53720273917642769</v>
       </c>
       <c r="K44" t="s">
-        <v>83</v>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="H46" t="s">
+        <v>116</v>
+      </c>
+      <c r="I46" s="123" t="s">
+        <v>119</v>
+      </c>
+      <c r="J46" s="123"/>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="H47" t="s">
+        <v>117</v>
+      </c>
+      <c r="J47" s="61">
+        <v>1459.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="H48" t="s">
+        <v>118</v>
+      </c>
+      <c r="J48" s="61">
+        <v>1465</v>
+      </c>
+    </row>
+    <row r="49" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J49" s="61">
+        <v>1465.8</v>
+      </c>
+    </row>
+    <row r="50" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J50" s="61">
+        <v>1465.3</v>
+      </c>
+    </row>
+    <row r="51" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J51" s="61">
+        <f>SUM(J47:J50)/4</f>
+        <v>1463.9</v>
+      </c>
+      <c r="K51" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="52" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J52">
+        <f>(1500-J47)/1500*100</f>
+        <v>2.7</v>
+      </c>
+      <c r="K52" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="79">
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="H22:J22"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="K20:M20"/>
+  <mergeCells count="80">
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="K7:M7"/>
     <mergeCell ref="K13:M13"/>
     <mergeCell ref="A16:A21"/>
     <mergeCell ref="B16:D16"/>
@@ -5433,47 +4845,28 @@
     <mergeCell ref="H19:J19"/>
     <mergeCell ref="K19:M19"/>
     <mergeCell ref="E17:G17"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="S7:T7"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="K22:M22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5534,274 +4927,1361 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8" customWidth="1"/>
+    <col min="14" max="14" width="13" customWidth="1"/>
+    <col min="15" max="15" width="14" customWidth="1"/>
+    <col min="16" max="16" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="6" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="116" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="110" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="111"/>
+      <c r="D1" s="112"/>
+      <c r="E1" s="110" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="111"/>
+      <c r="G1" s="112"/>
+      <c r="H1" s="110" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="111"/>
+      <c r="J1" s="112"/>
+      <c r="K1" s="110" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="111"/>
+      <c r="M1" s="112"/>
+      <c r="N1" s="76" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" s="67">
+        <v>60</v>
+      </c>
+      <c r="P1" s="67" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q1" s="63" t="s">
+        <v>59</v>
+      </c>
+      <c r="R1" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="S1" s="65" t="s">
+        <v>98</v>
+      </c>
+      <c r="T1" s="65" t="s">
+        <v>63</v>
+      </c>
+      <c r="U1" s="65" t="s">
+        <v>62</v>
+      </c>
+      <c r="V1" s="65" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" s="117"/>
+      <c r="B2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B1">
-        <v>5.2189300000000003</v>
-      </c>
-      <c r="C1">
-        <v>0.22186</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="D2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>33.292949999999998</v>
-      </c>
-      <c r="C2">
-        <v>0.35124</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="E2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="63" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2">
+        <v>1000</v>
+      </c>
+      <c r="P2" t="s">
+        <v>11</v>
+      </c>
+      <c r="S2" s="65" t="s">
+        <v>98</v>
+      </c>
+      <c r="T2" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="U2">
+        <f>O34</f>
+        <v>0.18609999999999999</v>
+      </c>
+      <c r="V2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1">
+        <v>364</v>
+      </c>
+      <c r="C3" s="2">
+        <f>B3/($O$1*$O$2)</f>
+        <v>6.0666666666666664E-3</v>
+      </c>
+      <c r="D3" s="3">
+        <f>C3*1000</f>
+        <v>6.0666666666666664</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2000</v>
+      </c>
+      <c r="F3" s="2">
+        <f>E3/($O$1*$O$2)</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="G3" s="3">
+        <f>F3*1000</f>
+        <v>33.333333333333336</v>
+      </c>
+      <c r="H3" s="1">
+        <v>10000</v>
+      </c>
+      <c r="I3" s="2">
+        <f>H3/($O$1*$O$2)</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="J3" s="3">
+        <f>I3*1000</f>
+        <v>166.66666666666666</v>
+      </c>
+      <c r="K3" s="1">
+        <v>15000</v>
+      </c>
+      <c r="L3" s="2">
+        <f>K3/($O$1*$O$2)</f>
+        <v>0.25</v>
+      </c>
+      <c r="M3" s="3">
+        <f>L3*1000</f>
+        <v>250</v>
+      </c>
+      <c r="S3" s="65" t="s">
+        <v>98</v>
+      </c>
+      <c r="T3" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="U3" s="78">
+        <f>U2/60</f>
+        <v>3.1016666666666666E-3</v>
+      </c>
+      <c r="V3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="113" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="103">
+        <f>46.6/9.39</f>
+        <v>4.9627263045793395</v>
+      </c>
+      <c r="C4" s="104"/>
+      <c r="D4" s="105"/>
+      <c r="E4" s="103">
+        <f>48.1/1.44</f>
+        <v>33.402777777777779</v>
+      </c>
+      <c r="F4" s="104"/>
+      <c r="G4" s="105"/>
+      <c r="H4" s="103">
+        <f>245.8/1.4</f>
+        <v>175.57142857142858</v>
+      </c>
+      <c r="I4" s="104"/>
+      <c r="J4" s="105"/>
+      <c r="K4" s="106"/>
+      <c r="L4" s="107"/>
+      <c r="M4" s="108"/>
+      <c r="N4" s="63" t="s">
+        <v>90</v>
+      </c>
+      <c r="O4" s="63" t="s">
+        <v>87</v>
+      </c>
+      <c r="P4" s="83" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q4" s="83" t="s">
+        <v>86</v>
+      </c>
+      <c r="R4" s="82"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="114"/>
+      <c r="B5" s="103">
+        <f>46.9/9.08</f>
+        <v>5.1651982378854626</v>
+      </c>
+      <c r="C5" s="104"/>
+      <c r="D5" s="105"/>
+      <c r="E5" s="103">
+        <f>48/1.43</f>
+        <v>33.566433566433567</v>
+      </c>
+      <c r="F5" s="104"/>
+      <c r="G5" s="105"/>
+      <c r="H5" s="103">
+        <f>245.5/1.33</f>
+        <v>184.58646616541353</v>
+      </c>
+      <c r="I5" s="104"/>
+      <c r="J5" s="105"/>
+      <c r="K5" s="103"/>
+      <c r="L5" s="104"/>
+      <c r="M5" s="105"/>
+      <c r="N5">
+        <v>20381</v>
+      </c>
+      <c r="P5" s="65" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q5" s="65" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="114"/>
+      <c r="B6" s="103">
+        <f>46.6/8.53</f>
+        <v>5.4630715123094964</v>
+      </c>
+      <c r="C6" s="104"/>
+      <c r="D6" s="105"/>
+      <c r="E6" s="103">
+        <f>47.8/1.39</f>
+        <v>34.388489208633096</v>
+      </c>
+      <c r="F6" s="104"/>
+      <c r="G6" s="105"/>
+      <c r="H6" s="103">
+        <f>244.7/1.37</f>
+        <v>178.61313868613138</v>
+      </c>
+      <c r="I6" s="104"/>
+      <c r="J6" s="105"/>
+      <c r="K6" s="106"/>
+      <c r="L6" s="107"/>
+      <c r="M6" s="108"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="114"/>
+      <c r="B7" s="103">
+        <f>46.4/8.39</f>
+        <v>5.5303933253873652</v>
+      </c>
+      <c r="C7" s="104"/>
+      <c r="D7" s="105"/>
+      <c r="E7" s="103">
+        <f>47.5/1.37</f>
+        <v>34.671532846715323</v>
+      </c>
+      <c r="F7" s="104"/>
+      <c r="G7" s="105"/>
+      <c r="H7" s="103">
+        <f>243.4/1.32</f>
+        <v>184.39393939393938</v>
+      </c>
+      <c r="I7" s="104"/>
+      <c r="J7" s="105"/>
+      <c r="K7" s="103"/>
+      <c r="L7" s="104"/>
+      <c r="M7" s="105"/>
+      <c r="O7" s="63" t="s">
+        <v>94</v>
+      </c>
+      <c r="P7" s="109" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q7" s="109"/>
+      <c r="R7" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="S7" s="109" t="s">
+        <v>97</v>
+      </c>
+      <c r="T7" s="109"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="114"/>
+      <c r="B8" s="103">
+        <f>47.8/8.44</f>
+        <v>5.6635071090047395</v>
+      </c>
+      <c r="C8" s="104"/>
+      <c r="D8" s="105"/>
+      <c r="E8" s="103">
+        <f>47.6/1.39</f>
+        <v>34.244604316546763</v>
+      </c>
+      <c r="F8" s="104"/>
+      <c r="G8" s="105"/>
+      <c r="H8" s="103">
+        <f>243.5/1.39</f>
+        <v>175.17985611510792</v>
+      </c>
+      <c r="I8" s="104"/>
+      <c r="J8" s="105"/>
+      <c r="K8" s="106"/>
+      <c r="L8" s="107"/>
+      <c r="M8" s="108"/>
+      <c r="P8" s="65" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q8" s="65" t="s">
+        <v>96</v>
+      </c>
+      <c r="S8" s="77" t="s">
+        <v>98</v>
+      </c>
+      <c r="T8" s="77" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="115"/>
+      <c r="B9" s="103">
+        <f>47.3/8.55</f>
+        <v>5.5321637426900576</v>
+      </c>
+      <c r="C9" s="104"/>
+      <c r="D9" s="105"/>
+      <c r="E9" s="103">
+        <f>47.3/1.38</f>
+        <v>34.275362318840578</v>
+      </c>
+      <c r="F9" s="104"/>
+      <c r="G9" s="105"/>
+      <c r="H9" s="103">
+        <f>243.9/1.33</f>
+        <v>183.38345864661653</v>
+      </c>
+      <c r="I9" s="104"/>
+      <c r="J9" s="105"/>
+      <c r="K9" s="106"/>
+      <c r="L9" s="107"/>
+      <c r="M9" s="108"/>
+      <c r="O9" s="63" t="s">
+        <v>94</v>
+      </c>
+      <c r="P9" s="109" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q9" s="109"/>
+      <c r="R9" t="s">
+        <v>60</v>
+      </c>
+      <c r="S9" s="81"/>
+      <c r="T9" s="79">
+        <v>3000</v>
+      </c>
+      <c r="U9" s="80" t="s">
+        <v>104</v>
+      </c>
+      <c r="V9" s="81"/>
+    </row>
+    <row r="10" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="100" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="101"/>
+      <c r="D10" s="102"/>
+      <c r="E10" s="100" t="s">
+        <v>108</v>
+      </c>
+      <c r="F10" s="101"/>
+      <c r="G10" s="102"/>
+      <c r="H10" s="100" t="s">
+        <v>109</v>
+      </c>
+      <c r="I10" s="101"/>
+      <c r="J10" s="102"/>
+      <c r="K10" s="100" t="s">
+        <v>76</v>
+      </c>
+      <c r="L10" s="101"/>
+      <c r="M10" s="102"/>
+      <c r="P10" s="77" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q10" s="77" t="s">
+        <v>113</v>
+      </c>
+      <c r="S10" s="78">
+        <f>U3</f>
+        <v>3.1016666666666666E-3</v>
+      </c>
+      <c r="T10" s="61" t="s">
+        <v>104</v>
+      </c>
+      <c r="U10">
+        <v>45252</v>
+      </c>
+      <c r="V10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="94">
+        <f>(363.12*1000)/($O$1*$O$2)</f>
+        <v>6.0519999999999996</v>
+      </c>
+      <c r="C11" s="95"/>
+      <c r="D11" s="96"/>
+      <c r="E11" s="94">
+        <f>(1990.7*1000)/($O$1*$O$2)</f>
+        <v>33.178333333333335</v>
+      </c>
+      <c r="F11" s="95"/>
+      <c r="G11" s="96"/>
+      <c r="H11" s="94">
+        <f>(9988.7*1000)/($O$1*$O$2)</f>
+        <v>166.47833333333332</v>
+      </c>
+      <c r="I11" s="95"/>
+      <c r="J11" s="96"/>
+      <c r="K11" s="94"/>
+      <c r="L11" s="95"/>
+      <c r="M11" s="96"/>
+      <c r="O11" s="121" t="s">
+        <v>94</v>
+      </c>
+      <c r="P11" s="122">
+        <f>T9/(S10*U10)*1000</f>
+        <v>21374.125424222955</v>
+      </c>
+      <c r="Q11" s="60" t="s">
+        <v>114</v>
+      </c>
+      <c r="S11" s="61"/>
+      <c r="T11" s="61"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" s="116" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="110" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="111"/>
+      <c r="D13" s="112"/>
+      <c r="E13" s="110" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>176.44907000000001</v>
-      </c>
-      <c r="C3">
-        <v>1.82758</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="F13" s="111"/>
+      <c r="G13" s="112"/>
+      <c r="H13" s="110" t="s">
+        <v>3</v>
+      </c>
+      <c r="I13" s="111"/>
+      <c r="J13" s="112"/>
+      <c r="K13" s="110" t="s">
+        <v>6</v>
+      </c>
+      <c r="L13" s="111"/>
+      <c r="M13" s="112"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" s="117"/>
+      <c r="B14" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="K14" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="L14" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="M14" s="13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
-        <v>366.70735999999999</v>
-      </c>
-      <c r="C4">
-        <v>4.2896599999999996</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>1744.8535899999999</v>
-      </c>
-      <c r="C5">
-        <v>14.3483</v>
+      <c r="B15" s="1">
+        <v>20000</v>
+      </c>
+      <c r="C15" s="2">
+        <f>B15/($O$1*$O$2)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D15" s="3">
+        <f>C15*1000</f>
+        <v>333.33333333333331</v>
+      </c>
+      <c r="E15" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F15" s="2">
+        <f>E15/($O$1*$O$2)</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="G15" s="3">
+        <f>F15*1000</f>
+        <v>1666.6666666666667</v>
+      </c>
+      <c r="H15" s="1">
+        <v>200000</v>
+      </c>
+      <c r="I15" s="2">
+        <f>H15/($O$1*$O$2)</f>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="J15" s="3">
+        <f>I15*1000</f>
+        <v>3333.3333333333335</v>
+      </c>
+      <c r="K15" s="1">
+        <v>278744</v>
+      </c>
+      <c r="L15" s="2">
+        <f>K15/($O$1*$O$2)</f>
+        <v>4.6457333333333333</v>
+      </c>
+      <c r="M15" s="3">
+        <f>L15*1000</f>
+        <v>4645.7333333333336</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" s="113" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="103">
+        <f>428.8/1.22</f>
+        <v>351.47540983606558</v>
+      </c>
+      <c r="C16" s="104"/>
+      <c r="D16" s="105"/>
+      <c r="E16" s="103">
+        <f>2145.4/1.22</f>
+        <v>1758.5245901639346</v>
+      </c>
+      <c r="F16" s="104"/>
+      <c r="G16" s="105"/>
+      <c r="H16" s="103">
+        <f>2024.6/(39/60)</f>
+        <v>3114.7692307692305</v>
+      </c>
+      <c r="I16" s="104"/>
+      <c r="J16" s="105"/>
+      <c r="K16" s="106"/>
+      <c r="L16" s="107"/>
+      <c r="M16" s="108"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="114"/>
+      <c r="B17" s="103">
+        <f>424.4/1.21</f>
+        <v>350.74380165289256</v>
+      </c>
+      <c r="C17" s="104"/>
+      <c r="D17" s="105"/>
+      <c r="E17" s="103">
+        <f>1986.8/1.16</f>
+        <v>1712.7586206896553</v>
+      </c>
+      <c r="F17" s="104"/>
+      <c r="G17" s="105"/>
+      <c r="H17" s="103">
+        <f>2065.8/(39/60)</f>
+        <v>3178.1538461538462</v>
+      </c>
+      <c r="I17" s="104"/>
+      <c r="J17" s="105"/>
+      <c r="K17" s="103"/>
+      <c r="L17" s="104"/>
+      <c r="M17" s="105"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="114"/>
+      <c r="B18" s="103">
+        <f>368.3/1.11</f>
+        <v>331.80180180180179</v>
+      </c>
+      <c r="C18" s="104"/>
+      <c r="D18" s="105"/>
+      <c r="E18" s="103">
+        <f>2012/1.16</f>
+        <v>1734.4827586206898</v>
+      </c>
+      <c r="F18" s="104"/>
+      <c r="G18" s="105"/>
+      <c r="H18" s="103">
+        <f>2031.6/(39/60)</f>
+        <v>3125.5384615384614</v>
+      </c>
+      <c r="I18" s="104"/>
+      <c r="J18" s="105"/>
+      <c r="K18" s="106"/>
+      <c r="L18" s="107"/>
+      <c r="M18" s="108"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="114"/>
+      <c r="B19" s="103">
+        <f>404/1.19</f>
+        <v>339.49579831932772</v>
+      </c>
+      <c r="C19" s="104"/>
+      <c r="D19" s="105"/>
+      <c r="E19" s="103">
+        <f>2027.7/1.17</f>
+        <v>1733.0769230769233</v>
+      </c>
+      <c r="F19" s="104"/>
+      <c r="G19" s="105"/>
+      <c r="H19" s="103">
+        <f>2047.4/(39/60)</f>
+        <v>3149.8461538461538</v>
+      </c>
+      <c r="I19" s="104"/>
+      <c r="J19" s="105"/>
+      <c r="K19" s="103"/>
+      <c r="L19" s="104"/>
+      <c r="M19" s="105"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="114"/>
+      <c r="B20" s="103">
+        <f>415.5/1.2</f>
+        <v>346.25</v>
+      </c>
+      <c r="C20" s="104"/>
+      <c r="D20" s="105"/>
+      <c r="E20" s="103">
+        <f>2031.7/1.18</f>
+        <v>1721.7796610169494</v>
+      </c>
+      <c r="F20" s="104"/>
+      <c r="G20" s="105"/>
+      <c r="H20" s="103">
+        <f>2058.3/(39/60)</f>
+        <v>3166.6153846153848</v>
+      </c>
+      <c r="I20" s="104"/>
+      <c r="J20" s="105"/>
+      <c r="K20" s="106"/>
+      <c r="L20" s="107"/>
+      <c r="M20" s="108"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="115"/>
+      <c r="B21" s="103">
+        <f>421.9/1.21</f>
+        <v>348.67768595041321</v>
+      </c>
+      <c r="C21" s="104"/>
+      <c r="D21" s="105"/>
+      <c r="E21" s="103">
+        <f>2032.4/1.17</f>
+        <v>1737.0940170940173</v>
+      </c>
+      <c r="F21" s="104"/>
+      <c r="G21" s="105"/>
+      <c r="H21" s="103">
+        <f>2313.1/(44/60)</f>
+        <v>3154.227272727273</v>
+      </c>
+      <c r="I21" s="104"/>
+      <c r="J21" s="105"/>
+      <c r="K21" s="106"/>
+      <c r="L21" s="107"/>
+      <c r="M21" s="108"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="100" t="s">
+        <v>110</v>
+      </c>
+      <c r="C22" s="101"/>
+      <c r="D22" s="102"/>
+      <c r="E22" s="100" t="s">
+        <v>111</v>
+      </c>
+      <c r="F22" s="101"/>
+      <c r="G22" s="102"/>
+      <c r="H22" s="100" t="s">
+        <v>112</v>
+      </c>
+      <c r="I22" s="101"/>
+      <c r="J22" s="102"/>
+      <c r="K22" s="100" t="s">
+        <v>66</v>
+      </c>
+      <c r="L22" s="101"/>
+      <c r="M22" s="102"/>
+    </row>
+    <row r="23" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="94">
+        <f>(19989.14*1000)/($O$1*$O$2)</f>
+        <v>333.15233333333333</v>
+      </c>
+      <c r="C23" s="95"/>
+      <c r="D23" s="96"/>
+      <c r="E23" s="94">
+        <f>(99999.52*1000)/($O$1*$O$2)</f>
+        <v>1666.6586666666667</v>
+      </c>
+      <c r="F23" s="95"/>
+      <c r="G23" s="96"/>
+      <c r="H23" s="94">
+        <f>1*(199996.73*1000)/($O$1*$O$2)</f>
+        <v>3333.2788333333333</v>
+      </c>
+      <c r="I23" s="95"/>
+      <c r="J23" s="96"/>
+      <c r="K23" s="97"/>
+      <c r="L23" s="98"/>
+      <c r="M23" s="99"/>
+    </row>
+    <row r="25" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="68" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" s="68" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" s="75" t="s">
+        <v>59</v>
+      </c>
+      <c r="E25" s="75" t="s">
+        <v>78</v>
+      </c>
+      <c r="I25" s="68" t="s">
+        <v>83</v>
+      </c>
+      <c r="J25" s="68" t="s">
+        <v>77</v>
+      </c>
+      <c r="N25" s="68" t="s">
+        <v>83</v>
+      </c>
+      <c r="O25" s="68" t="s">
+        <v>84</v>
+      </c>
+      <c r="P25" s="66" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>31</v>
+      </c>
+      <c r="B26" s="61">
+        <v>5.7666666666666666</v>
+      </c>
+      <c r="D26">
+        <f t="shared" ref="D26:D33" si="0">A26*$D$34+$G$34</f>
+        <v>6.1113200000000001</v>
+      </c>
+      <c r="E26" s="70">
+        <f>(B26-D26)/B26</f>
+        <v>-5.9766473988439331E-2</v>
+      </c>
+      <c r="I26">
+        <v>31</v>
+      </c>
+      <c r="J26" s="61">
+        <f>I26*$D$34+$G$34</f>
+        <v>6.1113200000000001</v>
+      </c>
+      <c r="N26">
+        <v>31</v>
+      </c>
+      <c r="O26" s="61">
+        <v>5.3861800000000004</v>
+      </c>
+      <c r="P26" s="61">
+        <v>0.26573999999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" s="55">
+        <f>(A26*B27)/B26</f>
+        <v>179.19075144508673</v>
+      </c>
+      <c r="B27" s="61">
+        <v>33.333333333333336</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>33.658498786127176</v>
+      </c>
+      <c r="E27" s="70">
+        <f t="shared" ref="E27:E33" si="1">(B27-D27)/B27</f>
+        <v>-9.754963583815196E-3</v>
+      </c>
+      <c r="I27">
+        <v>170</v>
+      </c>
+      <c r="J27" s="61">
+        <f t="shared" ref="J27:J31" si="2">I27*$D$34+$G$34</f>
+        <v>31.950029999999998</v>
+      </c>
+      <c r="N27">
+        <v>170</v>
+      </c>
+      <c r="O27" s="61">
+        <v>34.091529999999999</v>
+      </c>
+      <c r="P27" s="61">
+        <v>0.49636999999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="55">
+        <f t="shared" ref="A28:A32" si="3">(A27*B28)/B27</f>
+        <v>895.95375722543361</v>
+      </c>
+      <c r="B28" s="61">
+        <v>166.66666666666666</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>166.89757393063584</v>
+      </c>
+      <c r="E28" s="70">
+        <f t="shared" si="1"/>
+        <v>-1.3854435838151177E-3</v>
+      </c>
+      <c r="I28">
+        <v>853</v>
+      </c>
+      <c r="J28" s="61">
+        <f t="shared" si="2"/>
+        <v>158.91289999999998</v>
+      </c>
+      <c r="N28">
+        <v>853</v>
+      </c>
+      <c r="O28" s="61">
+        <v>180.28805</v>
+      </c>
+      <c r="P28" s="61">
+        <v>4.3831899999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="55">
+        <f t="shared" si="3"/>
+        <v>1343.9306358381505</v>
+      </c>
+      <c r="B29" s="61">
+        <v>250</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>250.17199589595378</v>
+      </c>
+      <c r="E29" s="70">
+        <f t="shared" si="1"/>
+        <v>-6.8798358381513933E-4</v>
+      </c>
+      <c r="I29">
+        <v>1707</v>
+      </c>
+      <c r="J29" s="61">
+        <f t="shared" si="2"/>
+        <v>317.66296</v>
+      </c>
+      <c r="N29">
+        <v>1707</v>
+      </c>
+      <c r="O29" s="61">
+        <v>344.74074999999999</v>
+      </c>
+      <c r="P29" s="61">
+        <v>7.6693600000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="55">
+        <f t="shared" si="3"/>
+        <v>1791.9075144508672</v>
+      </c>
+      <c r="B30" s="61">
+        <v>333.33333333333331</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>333.4464178612717</v>
+      </c>
+      <c r="E30" s="70">
+        <f t="shared" si="1"/>
+        <v>-3.3925358381515028E-4</v>
+      </c>
+      <c r="I30">
+        <v>8539</v>
+      </c>
+      <c r="J30" s="61">
+        <f t="shared" si="2"/>
+        <v>1587.66344</v>
+      </c>
+      <c r="N30">
+        <v>8539</v>
+      </c>
+      <c r="O30" s="61">
+        <v>1732.9527599999999</v>
+      </c>
+      <c r="P30" s="61">
+        <v>15.531040000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="55">
+        <f t="shared" si="3"/>
+        <v>8959.5375722543376</v>
+      </c>
+      <c r="B31" s="61">
+        <v>1666.6666666666667</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>1665.8371693063586</v>
+      </c>
+      <c r="E31" s="70">
+        <f t="shared" si="1"/>
+        <v>4.9769841618485771E-4</v>
+      </c>
+      <c r="I31">
+        <v>17079</v>
+      </c>
+      <c r="J31" s="61">
+        <f t="shared" si="2"/>
+        <v>3175.1640400000001</v>
+      </c>
+      <c r="N31">
+        <v>17079</v>
+      </c>
+      <c r="O31" s="61">
+        <v>3148.1917199999998</v>
+      </c>
+      <c r="P31" s="61">
+        <v>24.110410000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="55">
+        <f t="shared" si="3"/>
+        <v>17919.075144508675</v>
+      </c>
+      <c r="B32" s="61">
+        <v>3333.3333333333335</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>3331.3256086127176</v>
+      </c>
+      <c r="E32" s="70">
+        <f t="shared" si="1"/>
+        <v>6.0231741618476916E-4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>25000</v>
+      </c>
+      <c r="B33" s="61">
+        <v>4645.7333333333336</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>4647.5987299999997</v>
+      </c>
+      <c r="E33" s="70">
+        <f t="shared" si="1"/>
+        <v>-4.0152900152099321E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="58" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="62" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" s="64" t="s">
+        <v>60</v>
+      </c>
+      <c r="D34" s="59">
+        <v>0.18589</v>
+      </c>
+      <c r="E34" s="64" t="s">
+        <v>61</v>
+      </c>
+      <c r="F34" s="64" t="s">
+        <v>62</v>
+      </c>
+      <c r="G34" s="60">
+        <v>0.34872999999999998</v>
+      </c>
+      <c r="M34" s="121" t="s">
+        <v>59</v>
+      </c>
+      <c r="N34" s="64" t="s">
+        <v>60</v>
+      </c>
+      <c r="O34" s="59">
+        <v>0.18609999999999999</v>
+      </c>
+      <c r="P34" s="64" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q34" s="64" t="s">
+        <v>62</v>
+      </c>
+      <c r="R34" s="60">
+        <v>27.384129999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B35" s="63" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="M35" s="63" t="s">
+        <v>64</v>
+      </c>
+      <c r="N35" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="O35">
+        <v>0.99887000000000004</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H37" s="66" t="s">
+        <v>63</v>
+      </c>
+      <c r="I37" s="66" t="s">
+        <v>79</v>
+      </c>
+      <c r="J37" s="66" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H38" s="74">
+        <f>(J38-R34)/O34</f>
+        <v>15973.218001074692</v>
+      </c>
+      <c r="I38" s="65">
+        <f>J38*60</f>
+        <v>180000</v>
+      </c>
+      <c r="J38">
+        <v>3000</v>
+      </c>
+      <c r="K38" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H39" s="74">
+        <v>16120</v>
+      </c>
+      <c r="I39">
+        <v>180000</v>
+      </c>
+      <c r="J39" s="55">
+        <f>2.7623*1000/(56/60)</f>
+        <v>2959.6071428571431</v>
+      </c>
+      <c r="K39" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J40" s="55">
+        <f>2.7897*1000/(57/60)</f>
+        <v>2936.5263157894738</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J41" s="55">
+        <f>2.717*1000/(55/60)</f>
+        <v>2964</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J42" s="55">
+        <f>2.6923*1000/(55/60)</f>
+        <v>2937.0545454545454</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J43" s="55">
+        <f>2.685*1000/(55/60)</f>
+        <v>2929.090909090909</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J44" s="55">
+        <f>SUM(J39:J43)/5</f>
+        <v>2945.2557826384136</v>
+      </c>
+      <c r="K44" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J45" s="55">
+        <f>(J38-J44)/J38*100</f>
+        <v>1.8248072453862125</v>
+      </c>
+      <c r="K45" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="79">
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="A16:A21"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="S7:T7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>1</v>
-      </c>
-      <c r="B1">
-        <v>5.1347500000000004</v>
-      </c>
-      <c r="C1">
-        <v>33.620690000000003</v>
-      </c>
-      <c r="D1">
-        <v>178.89908</v>
-      </c>
-      <c r="E1">
-        <v>370.63636000000002</v>
-      </c>
-      <c r="F1">
-        <v>1752.1359199999999</v>
-      </c>
-      <c r="G1">
-        <v>3476.32258</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>5.3305199999999999</v>
-      </c>
-      <c r="C2">
-        <v>32.99145</v>
-      </c>
-      <c r="D2">
-        <v>174.77476999999999</v>
-      </c>
-      <c r="E2">
-        <v>368.16514000000001</v>
-      </c>
-      <c r="F2">
-        <v>1726.7326700000001</v>
-      </c>
-      <c r="G2">
-        <v>3498</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>5.2631600000000001</v>
-      </c>
-      <c r="C3">
-        <v>32.93103</v>
-      </c>
-      <c r="D3">
-        <v>176.63636</v>
-      </c>
-      <c r="E3">
-        <v>368.92856999999998</v>
-      </c>
-      <c r="F3">
-        <v>1750.9803899999999</v>
-      </c>
-      <c r="G3">
-        <v>3557.4193500000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>5.5555599999999998</v>
-      </c>
-      <c r="C4">
-        <v>33.043480000000002</v>
-      </c>
-      <c r="D4">
-        <v>178.14814999999999</v>
-      </c>
-      <c r="E4">
-        <v>366.03604000000001</v>
-      </c>
-      <c r="F4">
-        <v>1766.37255</v>
-      </c>
-      <c r="G4">
-        <v>3502</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>5.1330200000000001</v>
-      </c>
-      <c r="C5">
-        <v>33.421050000000001</v>
-      </c>
-      <c r="D5">
-        <v>175.9633</v>
-      </c>
-      <c r="E5">
-        <v>367.98246</v>
-      </c>
-      <c r="F5">
-        <v>1738.2</v>
-      </c>
-      <c r="G5">
-        <v>3516.1818199999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>4.8965500000000004</v>
-      </c>
-      <c r="C6">
-        <v>33.75</v>
-      </c>
-      <c r="D6">
-        <v>174.27273</v>
-      </c>
-      <c r="E6">
-        <v>358.49558000000002</v>
-      </c>
-      <c r="F6">
-        <v>1734.7</v>
-      </c>
-      <c r="G6">
-        <v>3512.68966</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7">
-        <v>33.620690000000003</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2</v>
-      </c>
-      <c r="B8">
-        <v>32.99145</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2</v>
-      </c>
-      <c r="B9">
-        <v>32.93103</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>2</v>
-      </c>
-      <c r="B10">
-        <v>33.043480000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>2</v>
-      </c>
-      <c r="B11">
-        <v>33.421050000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>2</v>
-      </c>
-      <c r="B12">
-        <v>33.75</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <oleObjects>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Origin50.Graph" shapeId="9231" r:id="rId4">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>57150</xdr:colOff>
+                <xdr:row>36</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>238125</xdr:colOff>
+                <xdr:row>54</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Origin50.Graph" shapeId="9231" r:id="rId4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Origin50.Graph" shapeId="9235" r:id="rId6">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>12</xdr:col>
+                <xdr:colOff>47625</xdr:colOff>
+                <xdr:row>35</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>20</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>53</xdr:row>
+                <xdr:rowOff>161925</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Origin50.Graph" shapeId="9235" r:id="rId6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </oleObjects>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Calculos de flujos de prueba de chip
</commit_message>
<xml_diff>
--- a/Calibracion.xlsx
+++ b/Calibracion.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="20115" windowHeight="7950" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="20115" windowHeight="7950" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Flow Rate" sheetId="5" r:id="rId1"/>
     <sheet name="3mL Bomba 2" sheetId="4" r:id="rId2"/>
     <sheet name="3mL Bomba 1" sheetId="7" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -917,7 +918,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="121">
   <si>
     <t>uL/h</t>
   </si>
@@ -1380,6 +1381,9 @@
   </si>
   <si>
     <t>Repeticiones (mg)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ml/min</t>
   </si>
 </sst>
 </file>
@@ -2259,16 +2263,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2285,6 +2287,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2295,6 +2351,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2302,76 +2376,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2608,15 +2612,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>12</xdr:col>
-          <xdr:colOff>50802</xdr:colOff>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>35</xdr:row>
-          <xdr:rowOff>114299</xdr:rowOff>
+          <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>20</xdr:col>
-          <xdr:colOff>9527</xdr:colOff>
+          <xdr:colOff>9525</xdr:colOff>
           <xdr:row>53</xdr:row>
-          <xdr:rowOff>161924</xdr:rowOff>
+          <xdr:rowOff>161925</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2975,7 +2979,7 @@
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3311,40 +3315,40 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="84" t="s">
+      <c r="A8" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="85"/>
+      <c r="B8" s="87"/>
       <c r="C8" s="53">
         <v>16</v>
       </c>
-      <c r="D8" s="86" t="s">
+      <c r="D8" s="94" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="85"/>
+      <c r="E8" s="87"/>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" t="s">
         <v>44</v>
       </c>
-      <c r="H8" s="87" t="s">
+      <c r="H8" s="95" t="s">
         <v>45</v>
       </c>
-      <c r="I8" s="87"/>
+      <c r="I8" s="95"/>
       <c r="J8">
         <v>25</v>
       </c>
-      <c r="K8" s="87" t="s">
+      <c r="K8" s="95" t="s">
         <v>46</v>
       </c>
-      <c r="L8" s="87"/>
+      <c r="L8" s="95"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="84" t="s">
+      <c r="A9" s="86" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="85"/>
+      <c r="B9" s="87"/>
       <c r="C9" s="54">
         <v>200</v>
       </c>
@@ -3359,24 +3363,24 @@
       <c r="G9" t="s">
         <v>48</v>
       </c>
-      <c r="H9" s="87" t="s">
+      <c r="H9" s="95" t="s">
         <v>49</v>
       </c>
-      <c r="I9" s="87"/>
+      <c r="I9" s="95"/>
       <c r="J9" s="55">
         <f>C10*J8</f>
         <v>1272.3724999999999</v>
       </c>
-      <c r="K9" s="87" t="s">
+      <c r="K9" s="95" t="s">
         <v>50</v>
       </c>
-      <c r="L9" s="87"/>
+      <c r="L9" s="95"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="84" t="s">
+      <c r="A10" s="86" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="85"/>
+      <c r="B10" s="87"/>
       <c r="C10" s="54">
         <v>50.8949</v>
       </c>
@@ -3394,10 +3398,10 @@
       <c r="L10" s="56"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="84" t="s">
+      <c r="A11" s="86" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="85"/>
+      <c r="B11" s="87"/>
       <c r="C11" s="54">
         <v>8</v>
       </c>
@@ -3449,12 +3453,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="H8:I8"/>
@@ -3463,6 +3461,12 @@
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="K9:L9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="D12:E12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="67" orientation="landscape" r:id="rId1"/>
@@ -3477,8 +3481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="I47" sqref="I47"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3507,29 +3511,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="110" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="118" t="s">
+      <c r="B1" s="98" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="119"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="118" t="s">
+      <c r="C1" s="99"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="98" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="119"/>
-      <c r="G1" s="120"/>
-      <c r="H1" s="118" t="s">
+      <c r="F1" s="99"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="98" t="s">
         <v>92</v>
       </c>
-      <c r="I1" s="119"/>
-      <c r="J1" s="120"/>
-      <c r="K1" s="118" t="s">
+      <c r="I1" s="99"/>
+      <c r="J1" s="100"/>
+      <c r="K1" s="98" t="s">
         <v>92</v>
       </c>
-      <c r="L1" s="119"/>
-      <c r="M1" s="120"/>
+      <c r="L1" s="99"/>
+      <c r="M1" s="100"/>
       <c r="N1" s="76" t="s">
         <v>8</v>
       </c>
@@ -3559,7 +3563,7 @@
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="117"/>
+      <c r="A2" s="111"/>
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
@@ -3682,30 +3686,30 @@
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="113" t="s">
+      <c r="A4" s="101" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="103">
+      <c r="B4" s="104">
         <f>36.2/7.05</f>
         <v>5.1347517730496461</v>
       </c>
-      <c r="C4" s="104"/>
-      <c r="D4" s="105"/>
-      <c r="E4" s="103">
+      <c r="C4" s="105"/>
+      <c r="D4" s="106"/>
+      <c r="E4" s="104">
         <f>39/1.16</f>
         <v>33.620689655172413</v>
       </c>
-      <c r="F4" s="104"/>
-      <c r="G4" s="105"/>
-      <c r="H4" s="103">
+      <c r="F4" s="105"/>
+      <c r="G4" s="106"/>
+      <c r="H4" s="104">
         <f>195/1.09</f>
         <v>178.89908256880733</v>
       </c>
-      <c r="I4" s="104"/>
-      <c r="J4" s="105"/>
-      <c r="K4" s="106"/>
-      <c r="L4" s="107"/>
-      <c r="M4" s="108"/>
+      <c r="I4" s="105"/>
+      <c r="J4" s="106"/>
+      <c r="K4" s="107"/>
+      <c r="L4" s="108"/>
+      <c r="M4" s="109"/>
       <c r="N4" s="63" t="s">
         <v>90</v>
       </c>
@@ -3721,28 +3725,28 @@
       <c r="R4" s="72"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="114"/>
-      <c r="B5" s="103">
+      <c r="A5" s="102"/>
+      <c r="B5" s="104">
         <f>37.9/7.11</f>
         <v>5.3305203938115326</v>
       </c>
-      <c r="C5" s="104"/>
-      <c r="D5" s="105"/>
-      <c r="E5" s="103">
+      <c r="C5" s="105"/>
+      <c r="D5" s="106"/>
+      <c r="E5" s="104">
         <f>38.6/1.17</f>
         <v>32.991452991452995</v>
       </c>
-      <c r="F5" s="104"/>
-      <c r="G5" s="105"/>
-      <c r="H5" s="103">
+      <c r="F5" s="105"/>
+      <c r="G5" s="106"/>
+      <c r="H5" s="104">
         <f>194/1.11</f>
         <v>174.77477477477476</v>
       </c>
-      <c r="I5" s="104"/>
-      <c r="J5" s="105"/>
-      <c r="K5" s="103"/>
-      <c r="L5" s="104"/>
-      <c r="M5" s="105"/>
+      <c r="I5" s="105"/>
+      <c r="J5" s="106"/>
+      <c r="K5" s="104"/>
+      <c r="L5" s="105"/>
+      <c r="M5" s="106"/>
       <c r="N5">
         <f>'Flow Rate'!C16</f>
         <v>21610</v>
@@ -3755,90 +3759,90 @@
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="114"/>
-      <c r="B6" s="103">
+      <c r="A6" s="102"/>
+      <c r="B6" s="104">
         <f>37/7.03</f>
         <v>5.2631578947368416</v>
       </c>
-      <c r="C6" s="104"/>
-      <c r="D6" s="105"/>
-      <c r="E6" s="103">
+      <c r="C6" s="105"/>
+      <c r="D6" s="106"/>
+      <c r="E6" s="104">
         <f>38.2/1.16</f>
         <v>32.931034482758626</v>
       </c>
-      <c r="F6" s="104"/>
-      <c r="G6" s="105"/>
-      <c r="H6" s="103">
+      <c r="F6" s="105"/>
+      <c r="G6" s="106"/>
+      <c r="H6" s="104">
         <f>194.3/1.1</f>
         <v>176.63636363636363</v>
       </c>
-      <c r="I6" s="104"/>
-      <c r="J6" s="105"/>
-      <c r="K6" s="106"/>
-      <c r="L6" s="107"/>
-      <c r="M6" s="108"/>
+      <c r="I6" s="105"/>
+      <c r="J6" s="106"/>
+      <c r="K6" s="107"/>
+      <c r="L6" s="108"/>
+      <c r="M6" s="109"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="114"/>
-      <c r="B7" s="103">
+      <c r="A7" s="102"/>
+      <c r="B7" s="104">
         <f>36/6.48</f>
         <v>5.5555555555555554</v>
       </c>
-      <c r="C7" s="104"/>
-      <c r="D7" s="105"/>
-      <c r="E7" s="103">
+      <c r="C7" s="105"/>
+      <c r="D7" s="106"/>
+      <c r="E7" s="104">
         <f>38/1.15</f>
         <v>33.04347826086957</v>
       </c>
-      <c r="F7" s="104"/>
-      <c r="G7" s="105"/>
-      <c r="H7" s="103">
+      <c r="F7" s="105"/>
+      <c r="G7" s="106"/>
+      <c r="H7" s="104">
         <f>192.4/1.08</f>
         <v>178.14814814814815</v>
       </c>
-      <c r="I7" s="104"/>
-      <c r="J7" s="105"/>
-      <c r="K7" s="103"/>
-      <c r="L7" s="104"/>
-      <c r="M7" s="105"/>
+      <c r="I7" s="105"/>
+      <c r="J7" s="106"/>
+      <c r="K7" s="104"/>
+      <c r="L7" s="105"/>
+      <c r="M7" s="106"/>
       <c r="O7" s="63" t="s">
         <v>94</v>
       </c>
-      <c r="P7" s="109" t="s">
+      <c r="P7" s="97" t="s">
         <v>97</v>
       </c>
-      <c r="Q7" s="109"/>
+      <c r="Q7" s="97"/>
       <c r="R7" s="65" t="s">
         <v>60</v>
       </c>
-      <c r="S7" s="109" t="s">
+      <c r="S7" s="97" t="s">
         <v>97</v>
       </c>
-      <c r="T7" s="109"/>
+      <c r="T7" s="97"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="114"/>
-      <c r="B8" s="103">
+      <c r="A8" s="102"/>
+      <c r="B8" s="104">
         <f>32.8/6.39</f>
         <v>5.1330203442879494</v>
       </c>
-      <c r="C8" s="104"/>
-      <c r="D8" s="105"/>
-      <c r="E8" s="103">
+      <c r="C8" s="105"/>
+      <c r="D8" s="106"/>
+      <c r="E8" s="104">
         <f>38.1/1.14</f>
         <v>33.421052631578952</v>
       </c>
-      <c r="F8" s="104"/>
-      <c r="G8" s="105"/>
-      <c r="H8" s="103">
+      <c r="F8" s="105"/>
+      <c r="G8" s="106"/>
+      <c r="H8" s="104">
         <f>191.8/1.09</f>
         <v>175.96330275229357</v>
       </c>
-      <c r="I8" s="104"/>
-      <c r="J8" s="105"/>
-      <c r="K8" s="106"/>
-      <c r="L8" s="107"/>
-      <c r="M8" s="108"/>
+      <c r="I8" s="105"/>
+      <c r="J8" s="106"/>
+      <c r="K8" s="107"/>
+      <c r="L8" s="108"/>
+      <c r="M8" s="109"/>
       <c r="P8" s="65" t="s">
         <v>95</v>
       </c>
@@ -3853,35 +3857,35 @@
       </c>
     </row>
     <row r="9" spans="1:22" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="115"/>
-      <c r="B9" s="103">
+      <c r="A9" s="103"/>
+      <c r="B9" s="104">
         <f>35.5/7.25</f>
         <v>4.8965517241379306</v>
       </c>
-      <c r="C9" s="104"/>
-      <c r="D9" s="105"/>
-      <c r="E9" s="103">
+      <c r="C9" s="105"/>
+      <c r="D9" s="106"/>
+      <c r="E9" s="104">
         <f>37.8/1.12</f>
         <v>33.749999999999993</v>
       </c>
-      <c r="F9" s="104"/>
-      <c r="G9" s="105"/>
-      <c r="H9" s="103">
+      <c r="F9" s="105"/>
+      <c r="G9" s="106"/>
+      <c r="H9" s="104">
         <f>191.7/1.1</f>
         <v>174.27272727272725</v>
       </c>
-      <c r="I9" s="104"/>
-      <c r="J9" s="105"/>
-      <c r="K9" s="106"/>
-      <c r="L9" s="107"/>
-      <c r="M9" s="108"/>
+      <c r="I9" s="105"/>
+      <c r="J9" s="106"/>
+      <c r="K9" s="107"/>
+      <c r="L9" s="108"/>
+      <c r="M9" s="109"/>
       <c r="O9" s="63" t="s">
         <v>100</v>
       </c>
-      <c r="P9" s="109" t="s">
+      <c r="P9" s="97" t="s">
         <v>101</v>
       </c>
-      <c r="Q9" s="109"/>
+      <c r="Q9" s="97"/>
       <c r="R9" t="s">
         <v>60</v>
       </c>
@@ -3898,26 +3902,26 @@
       <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="100" t="s">
+      <c r="B10" s="115" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="101"/>
-      <c r="D10" s="102"/>
-      <c r="E10" s="100" t="s">
+      <c r="C10" s="116"/>
+      <c r="D10" s="117"/>
+      <c r="E10" s="115" t="s">
         <v>67</v>
       </c>
-      <c r="F10" s="101"/>
-      <c r="G10" s="102"/>
-      <c r="H10" s="100" t="s">
+      <c r="F10" s="116"/>
+      <c r="G10" s="117"/>
+      <c r="H10" s="115" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="101"/>
-      <c r="J10" s="102"/>
-      <c r="K10" s="100" t="s">
+      <c r="I10" s="116"/>
+      <c r="J10" s="117"/>
+      <c r="K10" s="115" t="s">
         <v>76</v>
       </c>
-      <c r="L10" s="101"/>
-      <c r="M10" s="102"/>
+      <c r="L10" s="116"/>
+      <c r="M10" s="117"/>
       <c r="P10" s="65" t="s">
         <v>102</v>
       </c>
@@ -3943,31 +3947,31 @@
       <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="94">
+      <c r="B11" s="112">
         <f>(336.12*1000)/($O$1*$O$2)</f>
         <v>5.6020000000000003</v>
       </c>
-      <c r="C11" s="95"/>
-      <c r="D11" s="96"/>
-      <c r="E11" s="94">
+      <c r="C11" s="113"/>
+      <c r="D11" s="114"/>
+      <c r="E11" s="112">
         <f>(1995.71*1000)/($O$1*$O$2)</f>
         <v>33.261833333333335</v>
       </c>
-      <c r="F11" s="95"/>
-      <c r="G11" s="96"/>
-      <c r="H11" s="94">
+      <c r="F11" s="113"/>
+      <c r="G11" s="114"/>
+      <c r="H11" s="112">
         <f>(9999.6*1000)/($O$1*$O$2)</f>
         <v>166.66</v>
       </c>
-      <c r="I11" s="95"/>
-      <c r="J11" s="96"/>
-      <c r="K11" s="94"/>
-      <c r="L11" s="95"/>
-      <c r="M11" s="96"/>
-      <c r="O11" s="121" t="s">
+      <c r="I11" s="113"/>
+      <c r="J11" s="114"/>
+      <c r="K11" s="112"/>
+      <c r="L11" s="113"/>
+      <c r="M11" s="114"/>
+      <c r="O11" s="84" t="s">
         <v>100</v>
       </c>
-      <c r="P11" s="122">
+      <c r="P11" s="85">
         <f>T9/(S10*U10)*1000</f>
         <v>45244.307951863069</v>
       </c>
@@ -3982,34 +3986,34 @@
       <c r="T12" s="61"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="116" t="s">
+      <c r="A13" s="110" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="118" t="s">
+      <c r="B13" s="98" t="s">
         <v>92</v>
       </c>
-      <c r="C13" s="119"/>
-      <c r="D13" s="120"/>
-      <c r="E13" s="118" t="s">
+      <c r="C13" s="99"/>
+      <c r="D13" s="100"/>
+      <c r="E13" s="98" t="s">
         <v>92</v>
       </c>
-      <c r="F13" s="119"/>
-      <c r="G13" s="120"/>
-      <c r="H13" s="118" t="s">
+      <c r="F13" s="99"/>
+      <c r="G13" s="100"/>
+      <c r="H13" s="98" t="s">
         <v>92</v>
       </c>
-      <c r="I13" s="119"/>
-      <c r="J13" s="120"/>
-      <c r="K13" s="110" t="s">
+      <c r="I13" s="99"/>
+      <c r="J13" s="100"/>
+      <c r="K13" s="118" t="s">
         <v>93</v>
       </c>
-      <c r="L13" s="111"/>
-      <c r="M13" s="112"/>
+      <c r="L13" s="119"/>
+      <c r="M13" s="120"/>
       <c r="S13" s="61"/>
       <c r="T13" s="61"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="117"/>
+      <c r="A14" s="111"/>
       <c r="B14" s="7" t="s">
         <v>0</v>
       </c>
@@ -4097,201 +4101,201 @@
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="113" t="s">
+      <c r="A16" s="101" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="103">
+      <c r="B16" s="104">
         <f>407.7/1.1</f>
         <v>370.63636363636357</v>
       </c>
-      <c r="C16" s="104"/>
-      <c r="D16" s="105"/>
-      <c r="E16" s="103">
+      <c r="C16" s="105"/>
+      <c r="D16" s="106"/>
+      <c r="E16" s="104">
         <f>1804.7/1.03</f>
         <v>1752.1359223300972</v>
       </c>
-      <c r="F16" s="104"/>
-      <c r="G16" s="105"/>
-      <c r="H16" s="103">
+      <c r="F16" s="105"/>
+      <c r="G16" s="106"/>
+      <c r="H16" s="104">
         <f>1796.1/(31/60)</f>
         <v>3476.3225806451605</v>
       </c>
-      <c r="I16" s="104"/>
-      <c r="J16" s="105"/>
-      <c r="K16" s="106"/>
-      <c r="L16" s="107"/>
-      <c r="M16" s="108"/>
+      <c r="I16" s="105"/>
+      <c r="J16" s="106"/>
+      <c r="K16" s="107"/>
+      <c r="L16" s="108"/>
+      <c r="M16" s="109"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="114"/>
-      <c r="B17" s="103">
+      <c r="A17" s="102"/>
+      <c r="B17" s="104">
         <f>401.3/1.09</f>
         <v>368.16513761467888</v>
       </c>
-      <c r="C17" s="104"/>
-      <c r="D17" s="105"/>
-      <c r="E17" s="103">
+      <c r="C17" s="105"/>
+      <c r="D17" s="106"/>
+      <c r="E17" s="104">
         <f>1744/1.01</f>
         <v>1726.7326732673266</v>
       </c>
-      <c r="F17" s="104"/>
-      <c r="G17" s="105"/>
-      <c r="H17" s="103">
+      <c r="F17" s="105"/>
+      <c r="G17" s="106"/>
+      <c r="H17" s="104">
         <f>1690.7/(29/60)</f>
         <v>3498</v>
       </c>
-      <c r="I17" s="104"/>
-      <c r="J17" s="105"/>
-      <c r="K17" s="103"/>
-      <c r="L17" s="104"/>
-      <c r="M17" s="105"/>
+      <c r="I17" s="105"/>
+      <c r="J17" s="106"/>
+      <c r="K17" s="104"/>
+      <c r="L17" s="105"/>
+      <c r="M17" s="106"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="114"/>
-      <c r="B18" s="103">
+      <c r="A18" s="102"/>
+      <c r="B18" s="104">
         <f>413.2/1.12</f>
         <v>368.92857142857139</v>
       </c>
-      <c r="C18" s="104"/>
-      <c r="D18" s="105"/>
-      <c r="E18" s="103">
+      <c r="C18" s="105"/>
+      <c r="D18" s="106"/>
+      <c r="E18" s="104">
         <f>1786/1.02</f>
         <v>1750.9803921568628</v>
       </c>
-      <c r="F18" s="104"/>
-      <c r="G18" s="105"/>
-      <c r="H18" s="103">
+      <c r="F18" s="105"/>
+      <c r="G18" s="106"/>
+      <c r="H18" s="104">
         <f>1838/(31/60)</f>
         <v>3557.4193548387093</v>
       </c>
-      <c r="I18" s="104"/>
-      <c r="J18" s="105"/>
-      <c r="K18" s="106"/>
-      <c r="L18" s="107"/>
-      <c r="M18" s="108"/>
+      <c r="I18" s="105"/>
+      <c r="J18" s="106"/>
+      <c r="K18" s="107"/>
+      <c r="L18" s="108"/>
+      <c r="M18" s="109"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="114"/>
-      <c r="B19" s="103">
+      <c r="A19" s="102"/>
+      <c r="B19" s="104">
         <f>406.3/1.11</f>
         <v>366.03603603603602</v>
       </c>
-      <c r="C19" s="104"/>
-      <c r="D19" s="105"/>
-      <c r="E19" s="103">
+      <c r="C19" s="105"/>
+      <c r="D19" s="106"/>
+      <c r="E19" s="104">
         <f>1801.7/1.02</f>
         <v>1766.372549019608</v>
       </c>
-      <c r="F19" s="104"/>
-      <c r="G19" s="105"/>
-      <c r="H19" s="103">
+      <c r="F19" s="105"/>
+      <c r="G19" s="106"/>
+      <c r="H19" s="104">
         <f>1751/(30/60)</f>
         <v>3502</v>
       </c>
-      <c r="I19" s="104"/>
-      <c r="J19" s="105"/>
-      <c r="K19" s="103"/>
-      <c r="L19" s="104"/>
-      <c r="M19" s="105"/>
+      <c r="I19" s="105"/>
+      <c r="J19" s="106"/>
+      <c r="K19" s="104"/>
+      <c r="L19" s="105"/>
+      <c r="M19" s="106"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="114"/>
-      <c r="B20" s="103">
+      <c r="A20" s="102"/>
+      <c r="B20" s="104">
         <f>419.5/1.14</f>
         <v>367.98245614035091</v>
       </c>
-      <c r="C20" s="104"/>
-      <c r="D20" s="105"/>
-      <c r="E20" s="103">
+      <c r="C20" s="105"/>
+      <c r="D20" s="106"/>
+      <c r="E20" s="104">
         <f>1738.2/1</f>
         <v>1738.2</v>
       </c>
-      <c r="F20" s="104"/>
-      <c r="G20" s="105"/>
-      <c r="H20" s="103">
+      <c r="F20" s="105"/>
+      <c r="G20" s="106"/>
+      <c r="H20" s="104">
         <f>1933.9/(33/60)</f>
         <v>3516.181818181818</v>
       </c>
-      <c r="I20" s="104"/>
-      <c r="J20" s="105"/>
-      <c r="K20" s="106"/>
-      <c r="L20" s="107"/>
-      <c r="M20" s="108"/>
+      <c r="I20" s="105"/>
+      <c r="J20" s="106"/>
+      <c r="K20" s="107"/>
+      <c r="L20" s="108"/>
+      <c r="M20" s="109"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="115"/>
-      <c r="B21" s="103">
+      <c r="A21" s="103"/>
+      <c r="B21" s="104">
         <f>405.1/1.13</f>
         <v>358.49557522123899</v>
       </c>
-      <c r="C21" s="104"/>
-      <c r="D21" s="105"/>
-      <c r="E21" s="103">
+      <c r="C21" s="105"/>
+      <c r="D21" s="106"/>
+      <c r="E21" s="104">
         <f>1734.7/1</f>
         <v>1734.7</v>
       </c>
-      <c r="F21" s="104"/>
-      <c r="G21" s="105"/>
-      <c r="H21" s="103">
+      <c r="F21" s="105"/>
+      <c r="G21" s="106"/>
+      <c r="H21" s="104">
         <f>1697.8/(29/60)</f>
         <v>3512.6896551724135</v>
       </c>
-      <c r="I21" s="104"/>
-      <c r="J21" s="105"/>
-      <c r="K21" s="106"/>
-      <c r="L21" s="107"/>
-      <c r="M21" s="108"/>
+      <c r="I21" s="105"/>
+      <c r="J21" s="106"/>
+      <c r="K21" s="107"/>
+      <c r="L21" s="108"/>
+      <c r="M21" s="109"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="100" t="s">
+      <c r="B22" s="115" t="s">
         <v>73</v>
       </c>
-      <c r="C22" s="101"/>
-      <c r="D22" s="102"/>
-      <c r="E22" s="100" t="s">
+      <c r="C22" s="116"/>
+      <c r="D22" s="117"/>
+      <c r="E22" s="115" t="s">
         <v>74</v>
       </c>
-      <c r="F22" s="101"/>
-      <c r="G22" s="102"/>
-      <c r="H22" s="100" t="s">
+      <c r="F22" s="116"/>
+      <c r="G22" s="117"/>
+      <c r="H22" s="115" t="s">
         <v>75</v>
       </c>
-      <c r="I22" s="101"/>
-      <c r="J22" s="102"/>
-      <c r="K22" s="100" t="s">
+      <c r="I22" s="116"/>
+      <c r="J22" s="117"/>
+      <c r="K22" s="115" t="s">
         <v>66</v>
       </c>
-      <c r="L22" s="101"/>
-      <c r="M22" s="102"/>
+      <c r="L22" s="116"/>
+      <c r="M22" s="117"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="94">
+      <c r="B23" s="112">
         <f>(19999.15*1000)/($O$1*$O$2)</f>
         <v>333.31916666666666</v>
       </c>
-      <c r="C23" s="95"/>
-      <c r="D23" s="96"/>
-      <c r="E23" s="94">
+      <c r="C23" s="113"/>
+      <c r="D23" s="114"/>
+      <c r="E23" s="112">
         <f>(99995.75*1000)/($O$1*$O$2)</f>
         <v>1666.5958333333333</v>
       </c>
-      <c r="F23" s="95"/>
-      <c r="G23" s="96"/>
-      <c r="H23" s="94">
+      <c r="F23" s="113"/>
+      <c r="G23" s="114"/>
+      <c r="H23" s="112">
         <f>1*(199991.48*1000)/($O$1*$O$2)</f>
         <v>3333.1913333333332</v>
       </c>
-      <c r="I23" s="95"/>
-      <c r="J23" s="96"/>
-      <c r="K23" s="97"/>
-      <c r="L23" s="98"/>
-      <c r="M23" s="99"/>
+      <c r="I23" s="113"/>
+      <c r="J23" s="114"/>
+      <c r="K23" s="121"/>
+      <c r="L23" s="122"/>
+      <c r="M23" s="123"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="22"/>
@@ -4383,7 +4387,7 @@
         <v>190</v>
       </c>
       <c r="J27" s="61">
-        <f t="shared" ref="J26:J31" si="2">I27*$D$34+$G$34</f>
+        <f t="shared" ref="J27:J31" si="2">I27*$D$34+$G$34</f>
         <v>35.667830000000002</v>
       </c>
       <c r="N27">
@@ -4736,10 +4740,10 @@
       <c r="H46" t="s">
         <v>116</v>
       </c>
-      <c r="I46" s="123" t="s">
+      <c r="I46" s="96" t="s">
         <v>119</v>
       </c>
-      <c r="J46" s="123"/>
+      <c r="J46" s="96"/>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H47" t="s">
@@ -4787,17 +4791,50 @@
     </row>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="I46:J46"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="S7:T7"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="A16:A21"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="K10:M10"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
@@ -4805,6 +4842,17 @@
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="E7:G7"/>
     <mergeCell ref="E5:G5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="B5:D5"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="E9:G9"/>
     <mergeCell ref="H9:J9"/>
@@ -4813,60 +4861,16 @@
     <mergeCell ref="E8:G8"/>
     <mergeCell ref="H8:J8"/>
     <mergeCell ref="K8:M8"/>
-    <mergeCell ref="H5:J5"/>
     <mergeCell ref="K5:M5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="H6:J6"/>
     <mergeCell ref="K6:M6"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="K1:M1"/>
     <mergeCell ref="K7:M7"/>
     <mergeCell ref="K13:M13"/>
-    <mergeCell ref="A16:A21"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="H18:J18"/>
     <mergeCell ref="K18:M18"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="H22:J22"/>
-    <mergeCell ref="K22:M22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4931,8 +4935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V45"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4963,29 +4967,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="110" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="110" t="s">
+      <c r="B1" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="111"/>
-      <c r="D1" s="112"/>
-      <c r="E1" s="110" t="s">
+      <c r="C1" s="119"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="118" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="111"/>
-      <c r="G1" s="112"/>
-      <c r="H1" s="110" t="s">
+      <c r="F1" s="119"/>
+      <c r="G1" s="120"/>
+      <c r="H1" s="118" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="111"/>
-      <c r="J1" s="112"/>
-      <c r="K1" s="110" t="s">
+      <c r="I1" s="119"/>
+      <c r="J1" s="120"/>
+      <c r="K1" s="118" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="111"/>
-      <c r="M1" s="112"/>
+      <c r="L1" s="119"/>
+      <c r="M1" s="120"/>
       <c r="N1" s="76" t="s">
         <v>8</v>
       </c>
@@ -5015,7 +5019,7 @@
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="117"/>
+      <c r="A2" s="111"/>
       <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
@@ -5138,30 +5142,30 @@
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="113" t="s">
+      <c r="A4" s="101" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="103">
+      <c r="B4" s="104">
         <f>46.6/9.39</f>
         <v>4.9627263045793395</v>
       </c>
-      <c r="C4" s="104"/>
-      <c r="D4" s="105"/>
-      <c r="E4" s="103">
+      <c r="C4" s="105"/>
+      <c r="D4" s="106"/>
+      <c r="E4" s="104">
         <f>48.1/1.44</f>
         <v>33.402777777777779</v>
       </c>
-      <c r="F4" s="104"/>
-      <c r="G4" s="105"/>
-      <c r="H4" s="103">
+      <c r="F4" s="105"/>
+      <c r="G4" s="106"/>
+      <c r="H4" s="104">
         <f>245.8/1.4</f>
         <v>175.57142857142858</v>
       </c>
-      <c r="I4" s="104"/>
-      <c r="J4" s="105"/>
-      <c r="K4" s="106"/>
-      <c r="L4" s="107"/>
-      <c r="M4" s="108"/>
+      <c r="I4" s="105"/>
+      <c r="J4" s="106"/>
+      <c r="K4" s="107"/>
+      <c r="L4" s="108"/>
+      <c r="M4" s="109"/>
       <c r="N4" s="63" t="s">
         <v>90</v>
       </c>
@@ -5177,28 +5181,28 @@
       <c r="R4" s="82"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="114"/>
-      <c r="B5" s="103">
+      <c r="A5" s="102"/>
+      <c r="B5" s="104">
         <f>46.9/9.08</f>
         <v>5.1651982378854626</v>
       </c>
-      <c r="C5" s="104"/>
-      <c r="D5" s="105"/>
-      <c r="E5" s="103">
+      <c r="C5" s="105"/>
+      <c r="D5" s="106"/>
+      <c r="E5" s="104">
         <f>48/1.43</f>
         <v>33.566433566433567</v>
       </c>
-      <c r="F5" s="104"/>
-      <c r="G5" s="105"/>
-      <c r="H5" s="103">
+      <c r="F5" s="105"/>
+      <c r="G5" s="106"/>
+      <c r="H5" s="104">
         <f>245.5/1.33</f>
         <v>184.58646616541353</v>
       </c>
-      <c r="I5" s="104"/>
-      <c r="J5" s="105"/>
-      <c r="K5" s="103"/>
-      <c r="L5" s="104"/>
-      <c r="M5" s="105"/>
+      <c r="I5" s="105"/>
+      <c r="J5" s="106"/>
+      <c r="K5" s="104"/>
+      <c r="L5" s="105"/>
+      <c r="M5" s="106"/>
       <c r="N5">
         <v>20381</v>
       </c>
@@ -5210,90 +5214,90 @@
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="114"/>
-      <c r="B6" s="103">
+      <c r="A6" s="102"/>
+      <c r="B6" s="104">
         <f>46.6/8.53</f>
         <v>5.4630715123094964</v>
       </c>
-      <c r="C6" s="104"/>
-      <c r="D6" s="105"/>
-      <c r="E6" s="103">
+      <c r="C6" s="105"/>
+      <c r="D6" s="106"/>
+      <c r="E6" s="104">
         <f>47.8/1.39</f>
         <v>34.388489208633096</v>
       </c>
-      <c r="F6" s="104"/>
-      <c r="G6" s="105"/>
-      <c r="H6" s="103">
+      <c r="F6" s="105"/>
+      <c r="G6" s="106"/>
+      <c r="H6" s="104">
         <f>244.7/1.37</f>
         <v>178.61313868613138</v>
       </c>
-      <c r="I6" s="104"/>
-      <c r="J6" s="105"/>
-      <c r="K6" s="106"/>
-      <c r="L6" s="107"/>
-      <c r="M6" s="108"/>
+      <c r="I6" s="105"/>
+      <c r="J6" s="106"/>
+      <c r="K6" s="107"/>
+      <c r="L6" s="108"/>
+      <c r="M6" s="109"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="114"/>
-      <c r="B7" s="103">
+      <c r="A7" s="102"/>
+      <c r="B7" s="104">
         <f>46.4/8.39</f>
         <v>5.5303933253873652</v>
       </c>
-      <c r="C7" s="104"/>
-      <c r="D7" s="105"/>
-      <c r="E7" s="103">
+      <c r="C7" s="105"/>
+      <c r="D7" s="106"/>
+      <c r="E7" s="104">
         <f>47.5/1.37</f>
         <v>34.671532846715323</v>
       </c>
-      <c r="F7" s="104"/>
-      <c r="G7" s="105"/>
-      <c r="H7" s="103">
+      <c r="F7" s="105"/>
+      <c r="G7" s="106"/>
+      <c r="H7" s="104">
         <f>243.4/1.32</f>
         <v>184.39393939393938</v>
       </c>
-      <c r="I7" s="104"/>
-      <c r="J7" s="105"/>
-      <c r="K7" s="103"/>
-      <c r="L7" s="104"/>
-      <c r="M7" s="105"/>
+      <c r="I7" s="105"/>
+      <c r="J7" s="106"/>
+      <c r="K7" s="104"/>
+      <c r="L7" s="105"/>
+      <c r="M7" s="106"/>
       <c r="O7" s="63" t="s">
         <v>94</v>
       </c>
-      <c r="P7" s="109" t="s">
+      <c r="P7" s="97" t="s">
         <v>97</v>
       </c>
-      <c r="Q7" s="109"/>
+      <c r="Q7" s="97"/>
       <c r="R7" s="65" t="s">
         <v>60</v>
       </c>
-      <c r="S7" s="109" t="s">
+      <c r="S7" s="97" t="s">
         <v>97</v>
       </c>
-      <c r="T7" s="109"/>
+      <c r="T7" s="97"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="114"/>
-      <c r="B8" s="103">
+      <c r="A8" s="102"/>
+      <c r="B8" s="104">
         <f>47.8/8.44</f>
         <v>5.6635071090047395</v>
       </c>
-      <c r="C8" s="104"/>
-      <c r="D8" s="105"/>
-      <c r="E8" s="103">
+      <c r="C8" s="105"/>
+      <c r="D8" s="106"/>
+      <c r="E8" s="104">
         <f>47.6/1.39</f>
         <v>34.244604316546763</v>
       </c>
-      <c r="F8" s="104"/>
-      <c r="G8" s="105"/>
-      <c r="H8" s="103">
+      <c r="F8" s="105"/>
+      <c r="G8" s="106"/>
+      <c r="H8" s="104">
         <f>243.5/1.39</f>
         <v>175.17985611510792</v>
       </c>
-      <c r="I8" s="104"/>
-      <c r="J8" s="105"/>
-      <c r="K8" s="106"/>
-      <c r="L8" s="107"/>
-      <c r="M8" s="108"/>
+      <c r="I8" s="105"/>
+      <c r="J8" s="106"/>
+      <c r="K8" s="107"/>
+      <c r="L8" s="108"/>
+      <c r="M8" s="109"/>
       <c r="P8" s="65" t="s">
         <v>95</v>
       </c>
@@ -5308,35 +5312,35 @@
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="115"/>
-      <c r="B9" s="103">
+      <c r="A9" s="103"/>
+      <c r="B9" s="104">
         <f>47.3/8.55</f>
         <v>5.5321637426900576</v>
       </c>
-      <c r="C9" s="104"/>
-      <c r="D9" s="105"/>
-      <c r="E9" s="103">
+      <c r="C9" s="105"/>
+      <c r="D9" s="106"/>
+      <c r="E9" s="104">
         <f>47.3/1.38</f>
         <v>34.275362318840578</v>
       </c>
-      <c r="F9" s="104"/>
-      <c r="G9" s="105"/>
-      <c r="H9" s="103">
+      <c r="F9" s="105"/>
+      <c r="G9" s="106"/>
+      <c r="H9" s="104">
         <f>243.9/1.33</f>
         <v>183.38345864661653</v>
       </c>
-      <c r="I9" s="104"/>
-      <c r="J9" s="105"/>
-      <c r="K9" s="106"/>
-      <c r="L9" s="107"/>
-      <c r="M9" s="108"/>
+      <c r="I9" s="105"/>
+      <c r="J9" s="106"/>
+      <c r="K9" s="107"/>
+      <c r="L9" s="108"/>
+      <c r="M9" s="109"/>
       <c r="O9" s="63" t="s">
         <v>94</v>
       </c>
-      <c r="P9" s="109" t="s">
+      <c r="P9" s="97" t="s">
         <v>101</v>
       </c>
-      <c r="Q9" s="109"/>
+      <c r="Q9" s="97"/>
       <c r="R9" t="s">
         <v>60</v>
       </c>
@@ -5353,26 +5357,26 @@
       <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="100" t="s">
+      <c r="B10" s="115" t="s">
         <v>107</v>
       </c>
-      <c r="C10" s="101"/>
-      <c r="D10" s="102"/>
-      <c r="E10" s="100" t="s">
+      <c r="C10" s="116"/>
+      <c r="D10" s="117"/>
+      <c r="E10" s="115" t="s">
         <v>108</v>
       </c>
-      <c r="F10" s="101"/>
-      <c r="G10" s="102"/>
-      <c r="H10" s="100" t="s">
+      <c r="F10" s="116"/>
+      <c r="G10" s="117"/>
+      <c r="H10" s="115" t="s">
         <v>109</v>
       </c>
-      <c r="I10" s="101"/>
-      <c r="J10" s="102"/>
-      <c r="K10" s="100" t="s">
+      <c r="I10" s="116"/>
+      <c r="J10" s="117"/>
+      <c r="K10" s="115" t="s">
         <v>76</v>
       </c>
-      <c r="L10" s="101"/>
-      <c r="M10" s="102"/>
+      <c r="L10" s="116"/>
+      <c r="M10" s="117"/>
       <c r="P10" s="77" t="s">
         <v>102</v>
       </c>
@@ -5397,31 +5401,31 @@
       <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="94">
+      <c r="B11" s="112">
         <f>(363.12*1000)/($O$1*$O$2)</f>
         <v>6.0519999999999996</v>
       </c>
-      <c r="C11" s="95"/>
-      <c r="D11" s="96"/>
-      <c r="E11" s="94">
+      <c r="C11" s="113"/>
+      <c r="D11" s="114"/>
+      <c r="E11" s="112">
         <f>(1990.7*1000)/($O$1*$O$2)</f>
         <v>33.178333333333335</v>
       </c>
-      <c r="F11" s="95"/>
-      <c r="G11" s="96"/>
-      <c r="H11" s="94">
+      <c r="F11" s="113"/>
+      <c r="G11" s="114"/>
+      <c r="H11" s="112">
         <f>(9988.7*1000)/($O$1*$O$2)</f>
         <v>166.47833333333332</v>
       </c>
-      <c r="I11" s="95"/>
-      <c r="J11" s="96"/>
-      <c r="K11" s="94"/>
-      <c r="L11" s="95"/>
-      <c r="M11" s="96"/>
-      <c r="O11" s="121" t="s">
+      <c r="I11" s="113"/>
+      <c r="J11" s="114"/>
+      <c r="K11" s="112"/>
+      <c r="L11" s="113"/>
+      <c r="M11" s="114"/>
+      <c r="O11" s="84" t="s">
         <v>94</v>
       </c>
-      <c r="P11" s="122">
+      <c r="P11" s="85">
         <f>T9/(S10*U10)*1000</f>
         <v>21374.125424222955</v>
       </c>
@@ -5432,32 +5436,32 @@
       <c r="T11" s="61"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="116" t="s">
+      <c r="A13" s="110" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="110" t="s">
+      <c r="B13" s="118" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="111"/>
-      <c r="D13" s="112"/>
-      <c r="E13" s="110" t="s">
+      <c r="C13" s="119"/>
+      <c r="D13" s="120"/>
+      <c r="E13" s="118" t="s">
         <v>3</v>
       </c>
-      <c r="F13" s="111"/>
-      <c r="G13" s="112"/>
-      <c r="H13" s="110" t="s">
+      <c r="F13" s="119"/>
+      <c r="G13" s="120"/>
+      <c r="H13" s="118" t="s">
         <v>3</v>
       </c>
-      <c r="I13" s="111"/>
-      <c r="J13" s="112"/>
-      <c r="K13" s="110" t="s">
+      <c r="I13" s="119"/>
+      <c r="J13" s="120"/>
+      <c r="K13" s="118" t="s">
         <v>6</v>
       </c>
-      <c r="L13" s="111"/>
-      <c r="M13" s="112"/>
+      <c r="L13" s="119"/>
+      <c r="M13" s="120"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="117"/>
+      <c r="A14" s="111"/>
       <c r="B14" s="11" t="s">
         <v>0</v>
       </c>
@@ -5545,201 +5549,201 @@
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="113" t="s">
+      <c r="A16" s="101" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="103">
+      <c r="B16" s="104">
         <f>428.8/1.22</f>
         <v>351.47540983606558</v>
       </c>
-      <c r="C16" s="104"/>
-      <c r="D16" s="105"/>
-      <c r="E16" s="103">
+      <c r="C16" s="105"/>
+      <c r="D16" s="106"/>
+      <c r="E16" s="104">
         <f>2145.4/1.22</f>
         <v>1758.5245901639346</v>
       </c>
-      <c r="F16" s="104"/>
-      <c r="G16" s="105"/>
-      <c r="H16" s="103">
+      <c r="F16" s="105"/>
+      <c r="G16" s="106"/>
+      <c r="H16" s="104">
         <f>2024.6/(39/60)</f>
         <v>3114.7692307692305</v>
       </c>
-      <c r="I16" s="104"/>
-      <c r="J16" s="105"/>
-      <c r="K16" s="106"/>
-      <c r="L16" s="107"/>
-      <c r="M16" s="108"/>
+      <c r="I16" s="105"/>
+      <c r="J16" s="106"/>
+      <c r="K16" s="107"/>
+      <c r="L16" s="108"/>
+      <c r="M16" s="109"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="114"/>
-      <c r="B17" s="103">
+      <c r="A17" s="102"/>
+      <c r="B17" s="104">
         <f>424.4/1.21</f>
         <v>350.74380165289256</v>
       </c>
-      <c r="C17" s="104"/>
-      <c r="D17" s="105"/>
-      <c r="E17" s="103">
+      <c r="C17" s="105"/>
+      <c r="D17" s="106"/>
+      <c r="E17" s="104">
         <f>1986.8/1.16</f>
         <v>1712.7586206896553</v>
       </c>
-      <c r="F17" s="104"/>
-      <c r="G17" s="105"/>
-      <c r="H17" s="103">
+      <c r="F17" s="105"/>
+      <c r="G17" s="106"/>
+      <c r="H17" s="104">
         <f>2065.8/(39/60)</f>
         <v>3178.1538461538462</v>
       </c>
-      <c r="I17" s="104"/>
-      <c r="J17" s="105"/>
-      <c r="K17" s="103"/>
-      <c r="L17" s="104"/>
-      <c r="M17" s="105"/>
+      <c r="I17" s="105"/>
+      <c r="J17" s="106"/>
+      <c r="K17" s="104"/>
+      <c r="L17" s="105"/>
+      <c r="M17" s="106"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="114"/>
-      <c r="B18" s="103">
+      <c r="A18" s="102"/>
+      <c r="B18" s="104">
         <f>368.3/1.11</f>
         <v>331.80180180180179</v>
       </c>
-      <c r="C18" s="104"/>
-      <c r="D18" s="105"/>
-      <c r="E18" s="103">
+      <c r="C18" s="105"/>
+      <c r="D18" s="106"/>
+      <c r="E18" s="104">
         <f>2012/1.16</f>
         <v>1734.4827586206898</v>
       </c>
-      <c r="F18" s="104"/>
-      <c r="G18" s="105"/>
-      <c r="H18" s="103">
+      <c r="F18" s="105"/>
+      <c r="G18" s="106"/>
+      <c r="H18" s="104">
         <f>2031.6/(39/60)</f>
         <v>3125.5384615384614</v>
       </c>
-      <c r="I18" s="104"/>
-      <c r="J18" s="105"/>
-      <c r="K18" s="106"/>
-      <c r="L18" s="107"/>
-      <c r="M18" s="108"/>
+      <c r="I18" s="105"/>
+      <c r="J18" s="106"/>
+      <c r="K18" s="107"/>
+      <c r="L18" s="108"/>
+      <c r="M18" s="109"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="114"/>
-      <c r="B19" s="103">
+      <c r="A19" s="102"/>
+      <c r="B19" s="104">
         <f>404/1.19</f>
         <v>339.49579831932772</v>
       </c>
-      <c r="C19" s="104"/>
-      <c r="D19" s="105"/>
-      <c r="E19" s="103">
+      <c r="C19" s="105"/>
+      <c r="D19" s="106"/>
+      <c r="E19" s="104">
         <f>2027.7/1.17</f>
         <v>1733.0769230769233</v>
       </c>
-      <c r="F19" s="104"/>
-      <c r="G19" s="105"/>
-      <c r="H19" s="103">
+      <c r="F19" s="105"/>
+      <c r="G19" s="106"/>
+      <c r="H19" s="104">
         <f>2047.4/(39/60)</f>
         <v>3149.8461538461538</v>
       </c>
-      <c r="I19" s="104"/>
-      <c r="J19" s="105"/>
-      <c r="K19" s="103"/>
-      <c r="L19" s="104"/>
-      <c r="M19" s="105"/>
+      <c r="I19" s="105"/>
+      <c r="J19" s="106"/>
+      <c r="K19" s="104"/>
+      <c r="L19" s="105"/>
+      <c r="M19" s="106"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="114"/>
-      <c r="B20" s="103">
+      <c r="A20" s="102"/>
+      <c r="B20" s="104">
         <f>415.5/1.2</f>
         <v>346.25</v>
       </c>
-      <c r="C20" s="104"/>
-      <c r="D20" s="105"/>
-      <c r="E20" s="103">
+      <c r="C20" s="105"/>
+      <c r="D20" s="106"/>
+      <c r="E20" s="104">
         <f>2031.7/1.18</f>
         <v>1721.7796610169494</v>
       </c>
-      <c r="F20" s="104"/>
-      <c r="G20" s="105"/>
-      <c r="H20" s="103">
+      <c r="F20" s="105"/>
+      <c r="G20" s="106"/>
+      <c r="H20" s="104">
         <f>2058.3/(39/60)</f>
         <v>3166.6153846153848</v>
       </c>
-      <c r="I20" s="104"/>
-      <c r="J20" s="105"/>
-      <c r="K20" s="106"/>
-      <c r="L20" s="107"/>
-      <c r="M20" s="108"/>
+      <c r="I20" s="105"/>
+      <c r="J20" s="106"/>
+      <c r="K20" s="107"/>
+      <c r="L20" s="108"/>
+      <c r="M20" s="109"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="115"/>
-      <c r="B21" s="103">
+      <c r="A21" s="103"/>
+      <c r="B21" s="104">
         <f>421.9/1.21</f>
         <v>348.67768595041321</v>
       </c>
-      <c r="C21" s="104"/>
-      <c r="D21" s="105"/>
-      <c r="E21" s="103">
+      <c r="C21" s="105"/>
+      <c r="D21" s="106"/>
+      <c r="E21" s="104">
         <f>2032.4/1.17</f>
         <v>1737.0940170940173</v>
       </c>
-      <c r="F21" s="104"/>
-      <c r="G21" s="105"/>
-      <c r="H21" s="103">
+      <c r="F21" s="105"/>
+      <c r="G21" s="106"/>
+      <c r="H21" s="104">
         <f>2313.1/(44/60)</f>
         <v>3154.227272727273</v>
       </c>
-      <c r="I21" s="104"/>
-      <c r="J21" s="105"/>
-      <c r="K21" s="106"/>
-      <c r="L21" s="107"/>
-      <c r="M21" s="108"/>
+      <c r="I21" s="105"/>
+      <c r="J21" s="106"/>
+      <c r="K21" s="107"/>
+      <c r="L21" s="108"/>
+      <c r="M21" s="109"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="100" t="s">
+      <c r="B22" s="115" t="s">
         <v>110</v>
       </c>
-      <c r="C22" s="101"/>
-      <c r="D22" s="102"/>
-      <c r="E22" s="100" t="s">
+      <c r="C22" s="116"/>
+      <c r="D22" s="117"/>
+      <c r="E22" s="115" t="s">
         <v>111</v>
       </c>
-      <c r="F22" s="101"/>
-      <c r="G22" s="102"/>
-      <c r="H22" s="100" t="s">
+      <c r="F22" s="116"/>
+      <c r="G22" s="117"/>
+      <c r="H22" s="115" t="s">
         <v>112</v>
       </c>
-      <c r="I22" s="101"/>
-      <c r="J22" s="102"/>
-      <c r="K22" s="100" t="s">
+      <c r="I22" s="116"/>
+      <c r="J22" s="117"/>
+      <c r="K22" s="115" t="s">
         <v>66</v>
       </c>
-      <c r="L22" s="101"/>
-      <c r="M22" s="102"/>
+      <c r="L22" s="116"/>
+      <c r="M22" s="117"/>
     </row>
     <row r="23" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="94">
+      <c r="B23" s="112">
         <f>(19989.14*1000)/($O$1*$O$2)</f>
         <v>333.15233333333333</v>
       </c>
-      <c r="C23" s="95"/>
-      <c r="D23" s="96"/>
-      <c r="E23" s="94">
+      <c r="C23" s="113"/>
+      <c r="D23" s="114"/>
+      <c r="E23" s="112">
         <f>(99999.52*1000)/($O$1*$O$2)</f>
         <v>1666.6586666666667</v>
       </c>
-      <c r="F23" s="95"/>
-      <c r="G23" s="96"/>
-      <c r="H23" s="94">
+      <c r="F23" s="113"/>
+      <c r="G23" s="114"/>
+      <c r="H23" s="112">
         <f>1*(199996.73*1000)/($O$1*$O$2)</f>
         <v>3333.2788333333333</v>
       </c>
-      <c r="I23" s="95"/>
-      <c r="J23" s="96"/>
-      <c r="K23" s="97"/>
-      <c r="L23" s="98"/>
-      <c r="M23" s="99"/>
+      <c r="I23" s="113"/>
+      <c r="J23" s="114"/>
+      <c r="K23" s="121"/>
+      <c r="L23" s="122"/>
+      <c r="M23" s="123"/>
     </row>
     <row r="25" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="68" t="s">
@@ -6022,7 +6026,7 @@
       <c r="G34" s="60">
         <v>0.34872999999999998</v>
       </c>
-      <c r="M34" s="121" t="s">
+      <c r="M34" s="84" t="s">
         <v>59</v>
       </c>
       <c r="N34" s="64" t="s">
@@ -6147,6 +6151,69 @@
     </row>
   </sheetData>
   <mergeCells count="79">
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="A16:A21"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="K6:M6"/>
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="A4:A9"/>
     <mergeCell ref="B4:D4"/>
@@ -6163,69 +6230,6 @@
     <mergeCell ref="H7:J7"/>
     <mergeCell ref="K7:M7"/>
     <mergeCell ref="E5:G5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="A16:A21"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="H22:J22"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="S7:T7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6284,4 +6288,75 @@
     </mc:AlternateContent>
   </oleObjects>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="76" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="67">
+        <v>60</v>
+      </c>
+      <c r="E1" s="67" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0.5</v>
+      </c>
+      <c r="B2">
+        <f>A2*$D$1*$D$2</f>
+        <v>30000</v>
+      </c>
+      <c r="C2" s="63" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>1000</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1.5</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B4" si="0">A3*$D$1*$D$2</f>
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2.5</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>150000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>